<commit_message>
PROS6113 - Changed Category for LACTACYD to 'Baby Care' in Template.xlsx file as per the category in the system and changed the project code to bivn in the deployment script
</commit_message>
<xml_diff>
--- a/Projects/BIVN/Data/Template.xlsx
+++ b/Projects/BIVN/Data/Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,7 +17,7 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">MSL!$A$2:$G$16</definedName>
-    <definedName function="false" hidden="true" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$F$16</definedName>
+    <definedName function="false" hidden="true" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$16</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_FilterDatabase_0" vbProcedure="false">MSL!$A$2:$G$16</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">MSL!$A$2:$G$16</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">MSL!$A$2:$G$16</definedName>
@@ -33,6 +33,7 @@
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$G$16</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$G$16</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$G$16</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$G$16</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">'Primary Shelf_Location'!$A$2:$G$2</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">MSL!$A$2:$E$2</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">MSL!$A$2:$E$2</definedName>
@@ -51,20 +52,21 @@
     <definedName function="false" hidden="false" localSheetId="5" name="_FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$F$16</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$F$16</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$F$16</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$16</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$F$16</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$16</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$F$16</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$16</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$F$16</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$16</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$F$16</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$16</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$F$16</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$16</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$F$16</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$16</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$F$16</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$F$16</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$16</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$F$16</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$16</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$F$16</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$16</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$F$16</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$16</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$F$16</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$16</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$F$16</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$16</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$F$16</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$16</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$F$16</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -400,6 +402,9 @@
     <t xml:space="preserve">600457,600458</t>
   </si>
   <si>
+    <t xml:space="preserve">Baby Care</t>
+  </si>
+  <si>
     <t xml:space="preserve">Lactacyd BB 250ML
 </t>
   </si>
@@ -457,9 +462,6 @@
   <si>
     <t xml:space="preserve">Telfast  HD 180mg</t>
   </si>
-  <si>
-    <t xml:space="preserve">Baby Care</t>
-  </si>
 </sst>
 </file>
 
@@ -471,7 +473,7 @@
     <numFmt numFmtId="166" formatCode="0.00"/>
     <numFmt numFmtId="167" formatCode="0"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -590,28 +592,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-      <charset val="204"/>
-    </font>
-    <font>
       <b val="true"/>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -632,6 +612,21 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="13">
@@ -1243,111 +1238,131 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="14" fillId="6" borderId="18" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="15" fillId="8" borderId="26" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="15" fillId="8" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="15" fillId="8" borderId="17" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="15" fillId="8" borderId="15" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="15" fillId="8" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="9" borderId="29" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="10" borderId="30" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="32" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="9" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="10" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="10" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="9" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="33" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="17" fillId="0" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="20" fillId="6" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="17" fillId="6" borderId="18" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="20" fillId="6" borderId="11" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="17" fillId="6" borderId="13" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="20" fillId="6" borderId="12" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="17" fillId="6" borderId="15" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="20" fillId="6" borderId="13" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="5" fillId="8" borderId="26" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="8" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="8" borderId="17" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="8" borderId="15" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="8" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="8" borderId="18" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="8" borderId="19" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="9" borderId="29" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="10" borderId="30" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="9" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="10" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="10" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="9" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="6" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="6" borderId="11" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="6" borderId="12" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1371,31 +1386,23 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="8" borderId="18" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="8" borderId="19" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="11" borderId="34" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="9" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="9" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="9" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="9" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="10" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="10" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="9" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="9" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1403,11 +1410,11 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="9" borderId="5" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="9" borderId="5" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="10" borderId="5" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="10" borderId="5" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1419,17 +1426,13 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="9" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="19" fillId="9" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="22" fillId="9" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="19" fillId="9" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="8" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="5" fillId="8" borderId="15" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
@@ -1451,27 +1454,19 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="9" borderId="5" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="9" borderId="5" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="10" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="9" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="9" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="11" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="11" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1573,12 +1568,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="28.4939271255061"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="24.1012145748988"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="20.4615384615385"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="22.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="23.995951417004"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="16.8178137651822"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="28.7085020242915"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="24.3157894736842"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="20.5668016194332"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="24.2105263157895"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="16.9230769230769"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1844,11 +1839,11 @@
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="23" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="23" width="36.3117408906883"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="23" width="26.1376518218623"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="23" width="23.3522267206478"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="23" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="23" width="15.6396761133603"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="23" width="36.6356275303644"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="23" width="26.3522267206478"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="23" width="23.4574898785425"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="23" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="23" width="15.7449392712551"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="23" width="13.9271255060729"/>
     <col collapsed="false" hidden="false" max="1023" min="8" style="23" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="9.10526315789474"/>
@@ -16604,7 +16599,7 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="50" width="13.6032388663968"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="50" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="50" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="50" width="23.4574898785425"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="50" width="23.5668016194332"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="50" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="7" min="6" style="50" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="50" width="9.10526315789474"/>
@@ -16674,327 +16669,327 @@
   </sheetPr>
   <dimension ref="1:11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I11" activeCellId="0" sqref="I11"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="50" width="13.8178137651822"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="50" width="10.8178137651822"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="50" width="13.7125506072874"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="45.8461538461538"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="50" width="21.2105263157895"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="50" width="10.9271255060729"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="50" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="61" width="13.8178137651822"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="61" width="10.8178137651822"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="61" width="13.7125506072874"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="46.2753036437247"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="61" width="21.3157894736842"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="61" width="10.9271255060729"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="61" width="10.497975708502"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="1" width="8.57085020242915"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="61"/>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54" t="s">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="62"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
+      <c r="I1" s="64"/>
     </row>
-    <row r="2" customFormat="false" ht="70.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="62" t="s">
+    <row r="2" customFormat="false" ht="36.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="63" t="s">
+      <c r="B2" s="66" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="64" t="s">
+      <c r="C2" s="67" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="65" t="s">
+      <c r="D2" s="68" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="66" t="s">
+      <c r="E2" s="69" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="59" t="s">
+      <c r="F2" s="70" t="s">
         <v>35</v>
       </c>
-      <c r="G2" s="60" t="s">
+      <c r="G2" s="71" t="s">
         <v>36</v>
       </c>
-      <c r="H2" s="59" t="s">
+      <c r="H2" s="70" t="s">
         <v>37</v>
       </c>
-      <c r="I2" s="60" t="s">
+      <c r="I2" s="71" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="27.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="67" t="s">
+    <row r="3" customFormat="false" ht="24.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="72" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="41" t="s">
+      <c r="B3" s="73" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="73" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="68" t="s">
+      <c r="D3" s="74" t="s">
         <v>73</v>
       </c>
-      <c r="E3" s="69" t="s">
+      <c r="E3" s="75" t="s">
         <v>74</v>
       </c>
-      <c r="F3" s="70" t="n">
+      <c r="F3" s="76" t="n">
         <v>1</v>
       </c>
-      <c r="G3" s="71" t="n">
+      <c r="G3" s="77" t="n">
         <v>0</v>
       </c>
-      <c r="H3" s="70" t="n">
+      <c r="H3" s="76" t="n">
         <v>1</v>
       </c>
-      <c r="I3" s="71" t="n">
+      <c r="I3" s="77" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="4" s="76" customFormat="true" ht="27.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="72" t="s">
+    <row r="4" s="82" customFormat="true" ht="24.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="73" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="41" t="s">
+      <c r="C4" s="73" t="s">
         <v>48</v>
       </c>
-      <c r="D4" s="68" t="s">
+      <c r="D4" s="74" t="s">
         <v>75</v>
       </c>
-      <c r="E4" s="73" t="s">
+      <c r="E4" s="79" t="s">
         <v>76</v>
       </c>
-      <c r="F4" s="74" t="n">
+      <c r="F4" s="80" t="n">
         <v>1</v>
       </c>
-      <c r="G4" s="75" t="n">
+      <c r="G4" s="81" t="n">
         <v>0</v>
       </c>
-      <c r="H4" s="74" t="n">
+      <c r="H4" s="80" t="n">
         <v>1</v>
       </c>
-      <c r="I4" s="75" t="n">
+      <c r="I4" s="81" t="n">
         <v>0</v>
       </c>
-      <c r="AMI4" s="0"/>
-      <c r="AMJ4" s="0"/>
+      <c r="AMI4" s="1"/>
+      <c r="AMJ4" s="1"/>
     </row>
-    <row r="5" customFormat="false" ht="16.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="72" t="s">
+    <row r="5" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="41" t="s">
+      <c r="B5" s="73" t="s">
         <v>44</v>
       </c>
-      <c r="C5" s="41" t="s">
+      <c r="C5" s="73" t="s">
         <v>45</v>
       </c>
-      <c r="D5" s="68" t="s">
+      <c r="D5" s="74" t="s">
         <v>43</v>
       </c>
-      <c r="E5" s="69" t="n">
+      <c r="E5" s="75" t="n">
         <v>652426</v>
       </c>
-      <c r="F5" s="74" t="n">
+      <c r="F5" s="80" t="n">
         <v>1</v>
       </c>
-      <c r="G5" s="75" t="n">
+      <c r="G5" s="81" t="n">
         <v>0</v>
       </c>
-      <c r="H5" s="74" t="n">
+      <c r="H5" s="80" t="n">
         <v>1</v>
       </c>
-      <c r="I5" s="75" t="n">
+      <c r="I5" s="81" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="6" s="76" customFormat="true" ht="28.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="72" t="s">
+    <row r="6" s="82" customFormat="true" ht="24.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="77" t="s">
+      <c r="B6" s="83" t="s">
         <v>53</v>
       </c>
-      <c r="C6" s="41" t="s">
+      <c r="C6" s="73" t="s">
         <v>41</v>
       </c>
-      <c r="D6" s="68" t="s">
+      <c r="D6" s="74" t="s">
         <v>77</v>
       </c>
-      <c r="E6" s="69" t="s">
+      <c r="E6" s="75" t="s">
         <v>78</v>
       </c>
-      <c r="F6" s="78" t="n">
+      <c r="F6" s="84" t="n">
         <v>0</v>
       </c>
-      <c r="G6" s="79" t="n">
+      <c r="G6" s="85" t="n">
         <v>1</v>
       </c>
-      <c r="H6" s="78" t="n">
+      <c r="H6" s="84" t="n">
         <v>0</v>
       </c>
-      <c r="I6" s="79" t="n">
+      <c r="I6" s="85" t="n">
         <v>1</v>
       </c>
-      <c r="AMI6" s="0"/>
-      <c r="AMJ6" s="0"/>
+      <c r="AMI6" s="1"/>
+      <c r="AMJ6" s="1"/>
     </row>
-    <row r="7" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="72" t="s">
+    <row r="7" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="77" t="s">
+      <c r="B7" s="83" t="s">
         <v>63</v>
       </c>
-      <c r="C7" s="41" t="s">
+      <c r="C7" s="73" t="s">
         <v>41</v>
       </c>
-      <c r="D7" s="68" t="s">
+      <c r="D7" s="74" t="s">
         <v>79</v>
       </c>
-      <c r="E7" s="69" t="n">
+      <c r="E7" s="75" t="n">
         <v>329697</v>
       </c>
-      <c r="F7" s="78" t="n">
+      <c r="F7" s="84" t="n">
         <v>0</v>
       </c>
-      <c r="G7" s="79" t="n">
+      <c r="G7" s="85" t="n">
         <v>1</v>
       </c>
-      <c r="H7" s="78" t="n">
+      <c r="H7" s="84" t="n">
         <v>0</v>
       </c>
-      <c r="I7" s="79" t="n">
+      <c r="I7" s="85" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="72" t="s">
+    <row r="8" customFormat="false" ht="24.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="41" t="s">
+      <c r="B8" s="73" t="s">
         <v>80</v>
       </c>
-      <c r="C8" s="41" t="s">
+      <c r="C8" s="73" t="s">
         <v>48</v>
       </c>
-      <c r="D8" s="41" t="s">
+      <c r="D8" s="73" t="s">
         <v>81</v>
       </c>
-      <c r="E8" s="69" t="s">
+      <c r="E8" s="75" t="s">
         <v>82</v>
       </c>
-      <c r="F8" s="78" t="n">
+      <c r="F8" s="84" t="n">
         <v>0</v>
       </c>
-      <c r="G8" s="79" t="n">
+      <c r="G8" s="85" t="n">
         <v>1</v>
       </c>
-      <c r="H8" s="78" t="n">
+      <c r="H8" s="84" t="n">
         <v>0</v>
       </c>
-      <c r="I8" s="79" t="n">
+      <c r="I8" s="85" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="72" t="s">
+    <row r="9" customFormat="false" ht="24.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="41" t="s">
+      <c r="B9" s="73" t="s">
         <v>51</v>
       </c>
-      <c r="C9" s="41" t="s">
+      <c r="C9" s="73" t="s">
         <v>45</v>
       </c>
-      <c r="D9" s="41" t="s">
+      <c r="D9" s="73" t="s">
         <v>50</v>
       </c>
-      <c r="E9" s="69" t="n">
+      <c r="E9" s="75" t="n">
         <v>282998</v>
       </c>
-      <c r="F9" s="78" t="n">
+      <c r="F9" s="84" t="n">
         <v>0</v>
       </c>
-      <c r="G9" s="79" t="n">
+      <c r="G9" s="85" t="n">
         <v>1</v>
       </c>
-      <c r="H9" s="78" t="n">
+      <c r="H9" s="84" t="n">
         <v>0</v>
       </c>
-      <c r="I9" s="79" t="n">
+      <c r="I9" s="85" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="72" t="s">
+    <row r="10" customFormat="false" ht="24.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="77" t="s">
+      <c r="B10" s="83" t="s">
         <v>56</v>
       </c>
-      <c r="C10" s="80" t="s">
+      <c r="C10" s="86" t="s">
         <v>83</v>
       </c>
-      <c r="D10" s="80" t="s">
+      <c r="D10" s="86" t="s">
         <v>84</v>
       </c>
-      <c r="E10" s="69" t="s">
+      <c r="E10" s="75" t="s">
         <v>85</v>
       </c>
-      <c r="F10" s="78" t="n">
+      <c r="F10" s="84" t="n">
         <v>0</v>
       </c>
-      <c r="G10" s="79" t="n">
+      <c r="G10" s="85" t="n">
         <v>1</v>
       </c>
-      <c r="H10" s="78" t="n">
+      <c r="H10" s="84" t="n">
         <v>0</v>
       </c>
-      <c r="I10" s="79" t="n">
+      <c r="I10" s="85" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="28.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="81" t="s">
+    <row r="11" customFormat="false" ht="24.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="87" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="77" t="s">
+      <c r="B11" s="83" t="s">
         <v>65</v>
       </c>
-      <c r="C11" s="77" t="s">
-        <v>66</v>
-      </c>
-      <c r="D11" s="68" t="s">
+      <c r="C11" s="88" t="s">
         <v>86</v>
       </c>
-      <c r="E11" s="82" t="n">
+      <c r="D11" s="74" t="s">
+        <v>87</v>
+      </c>
+      <c r="E11" s="89" t="n">
         <v>528655</v>
       </c>
-      <c r="F11" s="78" t="n">
+      <c r="F11" s="84" t="n">
         <v>0</v>
       </c>
-      <c r="G11" s="79" t="n">
+      <c r="G11" s="85" t="n">
         <v>1</v>
       </c>
-      <c r="H11" s="78" t="n">
+      <c r="H11" s="84" t="n">
         <v>0</v>
       </c>
-      <c r="I11" s="79" t="n">
+      <c r="I11" s="85" t="n">
         <v>1</v>
       </c>
     </row>
@@ -17027,231 +17022,231 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="83" width="21.8542510121457"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="83" width="12.1052631578947"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="83" width="15.8542510121457"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="61" width="22.0647773279352"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="61" width="12.2105263157895"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="61" width="15.9595141700405"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.9595141700405"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="83" width="23.0323886639676"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="83" width="27.5303643724696"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="27.8502024291498"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="30.7449392712551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="13.0688259109312"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="61" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="61" width="27.7449392712551"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="28.0647773279352"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="31.0647773279352"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="84"/>
-      <c r="B1" s="85"/>
-      <c r="C1" s="86"/>
-      <c r="D1" s="87"/>
-      <c r="E1" s="87"/>
-      <c r="F1" s="84" t="s">
+      <c r="A1" s="90"/>
+      <c r="B1" s="91"/>
+      <c r="C1" s="92"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="90" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="84"/>
-      <c r="H1" s="84"/>
-      <c r="I1" s="84"/>
+      <c r="G1" s="90"/>
+      <c r="H1" s="90"/>
+      <c r="I1" s="90"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="88" t="s">
+      <c r="A2" s="93" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="89" t="s">
+      <c r="B2" s="94" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="90" t="s">
+      <c r="C2" s="95" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="91" t="s">
+      <c r="D2" s="96" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="92" t="s">
+      <c r="E2" s="97" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="93" t="s">
+      <c r="F2" s="70" t="s">
         <v>35</v>
       </c>
-      <c r="G2" s="94" t="s">
+      <c r="G2" s="71" t="s">
         <v>36</v>
       </c>
-      <c r="H2" s="93" t="s">
+      <c r="H2" s="70" t="s">
         <v>37</v>
       </c>
-      <c r="I2" s="94" t="s">
+      <c r="I2" s="71" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="95" t="s">
+      <c r="A3" s="98" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="96" t="s">
-        <v>87</v>
-      </c>
-      <c r="C3" s="97" t="s">
+      <c r="B3" s="99" t="s">
         <v>88</v>
       </c>
-      <c r="D3" s="97" t="s">
+      <c r="C3" s="100" t="s">
         <v>89</v>
       </c>
-      <c r="E3" s="97" t="s">
+      <c r="D3" s="100" t="s">
         <v>90</v>
       </c>
-      <c r="F3" s="98" t="n">
+      <c r="E3" s="100" t="s">
+        <v>91</v>
+      </c>
+      <c r="F3" s="101" t="n">
         <v>0</v>
       </c>
-      <c r="G3" s="99" t="n">
+      <c r="G3" s="102" t="n">
         <v>1</v>
       </c>
-      <c r="H3" s="98" t="n">
+      <c r="H3" s="101" t="n">
         <v>0</v>
       </c>
-      <c r="I3" s="99" t="n">
+      <c r="I3" s="102" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="100" t="s">
+      <c r="A4" s="103" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="96" t="s">
+      <c r="B4" s="99" t="s">
+        <v>92</v>
+      </c>
+      <c r="C4" s="100" t="s">
+        <v>93</v>
+      </c>
+      <c r="D4" s="100" t="s">
+        <v>90</v>
+      </c>
+      <c r="E4" s="100" t="s">
         <v>91</v>
       </c>
-      <c r="C4" s="97" t="s">
-        <v>92</v>
-      </c>
-      <c r="D4" s="97" t="s">
-        <v>89</v>
-      </c>
-      <c r="E4" s="97" t="s">
-        <v>90</v>
-      </c>
-      <c r="F4" s="101" t="n">
+      <c r="F4" s="104" t="n">
         <v>1</v>
       </c>
-      <c r="G4" s="102" t="n">
+      <c r="G4" s="105" t="n">
         <v>0</v>
       </c>
-      <c r="H4" s="101" t="n">
+      <c r="H4" s="104" t="n">
         <v>1</v>
       </c>
-      <c r="I4" s="102" t="n">
+      <c r="I4" s="105" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="34.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="103" t="s">
+      <c r="A5" s="106" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="96" t="s">
-        <v>93</v>
-      </c>
-      <c r="C5" s="97" t="s">
+      <c r="B5" s="99" t="s">
         <v>94</v>
       </c>
-      <c r="D5" s="97" t="s">
+      <c r="C5" s="100" t="s">
+        <v>95</v>
+      </c>
+      <c r="D5" s="100" t="s">
         <v>53</v>
       </c>
-      <c r="E5" s="97" t="s">
+      <c r="E5" s="100" t="s">
         <v>41</v>
       </c>
-      <c r="F5" s="99" t="n">
+      <c r="F5" s="102" t="n">
         <v>0</v>
       </c>
-      <c r="G5" s="99" t="n">
+      <c r="G5" s="102" t="n">
         <v>1</v>
       </c>
-      <c r="H5" s="98" t="n">
+      <c r="H5" s="101" t="n">
         <v>0</v>
       </c>
-      <c r="I5" s="98" t="n">
+      <c r="I5" s="101" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="23.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="104" t="s">
+      <c r="A6" s="107" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="96" t="s">
-        <v>95</v>
-      </c>
-      <c r="C6" s="97" t="s">
+      <c r="B6" s="99" t="s">
         <v>96</v>
       </c>
-      <c r="D6" s="97" t="s">
+      <c r="C6" s="100" t="s">
+        <v>97</v>
+      </c>
+      <c r="D6" s="100" t="s">
         <v>51</v>
       </c>
-      <c r="E6" s="105" t="s">
+      <c r="E6" s="108" t="s">
         <v>45</v>
       </c>
-      <c r="F6" s="99" t="n">
+      <c r="F6" s="102" t="n">
         <v>0</v>
       </c>
-      <c r="G6" s="99" t="n">
+      <c r="G6" s="102" t="n">
         <v>1</v>
       </c>
-      <c r="H6" s="102" t="n">
+      <c r="H6" s="105" t="n">
         <v>0</v>
       </c>
-      <c r="I6" s="102" t="n">
+      <c r="I6" s="105" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="23.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="104" t="s">
+      <c r="A7" s="107" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="96" t="s">
-        <v>97</v>
-      </c>
-      <c r="C7" s="97" t="s">
+      <c r="B7" s="99" t="s">
         <v>98</v>
       </c>
-      <c r="D7" s="105" t="s">
+      <c r="C7" s="100" t="s">
+        <v>99</v>
+      </c>
+      <c r="D7" s="108" t="s">
         <v>40</v>
       </c>
-      <c r="E7" s="105" t="s">
+      <c r="E7" s="108" t="s">
         <v>41</v>
       </c>
-      <c r="F7" s="99" t="n">
+      <c r="F7" s="102" t="n">
         <v>1</v>
       </c>
-      <c r="G7" s="99" t="n">
+      <c r="G7" s="102" t="n">
         <v>0</v>
       </c>
-      <c r="H7" s="98" t="n">
+      <c r="H7" s="101" t="n">
         <v>0</v>
       </c>
-      <c r="I7" s="98" t="n">
+      <c r="I7" s="101" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="23.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="104" t="s">
+      <c r="A8" s="107" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="96" t="s">
-        <v>99</v>
-      </c>
-      <c r="C8" s="97" t="s">
+      <c r="B8" s="99" t="s">
         <v>100</v>
       </c>
-      <c r="D8" s="106" t="s">
+      <c r="C8" s="100" t="s">
+        <v>101</v>
+      </c>
+      <c r="D8" s="109" t="s">
         <v>44</v>
       </c>
-      <c r="E8" s="105" t="s">
+      <c r="E8" s="108" t="s">
         <v>45</v>
       </c>
-      <c r="F8" s="99" t="n">
+      <c r="F8" s="102" t="n">
         <v>1</v>
       </c>
-      <c r="G8" s="99" t="n">
+      <c r="G8" s="102" t="n">
         <v>0</v>
       </c>
-      <c r="H8" s="102" t="n">
+      <c r="H8" s="105" t="n">
         <v>0</v>
       </c>
-      <c r="I8" s="102" t="n">
+      <c r="I8" s="105" t="n">
         <v>0</v>
       </c>
     </row>
@@ -17277,61 +17272,61 @@
   </sheetPr>
   <dimension ref="1:17"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I16" activeCellId="0" sqref="I16"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="83" width="27.8502024291498"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="83" width="22.1740890688259"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="83" width="23.4574898785425"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="83" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="83" width="11.0323886639676"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="83" width="8.35627530364373"/>
-    <col collapsed="false" hidden="false" max="1023" min="8" style="83" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="61" width="28.0647773279352"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="61" width="22.3886639676113"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="61" width="23.5668016194332"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="61" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="61" width="11.0323886639676"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="61" width="8.35627530364373"/>
+    <col collapsed="false" hidden="false" max="1023" min="8" style="61" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1025" min="1024" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="84"/>
-      <c r="B1" s="85"/>
-      <c r="C1" s="86"/>
-      <c r="D1" s="87"/>
-      <c r="E1" s="87"/>
-      <c r="F1" s="84" t="s">
+      <c r="A1" s="90"/>
+      <c r="B1" s="91"/>
+      <c r="C1" s="92"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="90" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="84"/>
-      <c r="H1" s="84"/>
-      <c r="I1" s="84"/>
+      <c r="G1" s="90"/>
+      <c r="H1" s="90"/>
+      <c r="I1" s="90"/>
     </row>
     <row r="2" customFormat="false" ht="46.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="107" t="s">
+      <c r="A2" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="107" t="s">
+      <c r="B2" s="69" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="108" t="s">
+      <c r="C2" s="110" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="107" t="s">
+      <c r="D2" s="69" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="109" t="s">
+      <c r="E2" s="111" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="93" t="s">
+      <c r="F2" s="70" t="s">
         <v>35</v>
       </c>
-      <c r="G2" s="94" t="s">
+      <c r="G2" s="71" t="s">
         <v>36</v>
       </c>
-      <c r="H2" s="93" t="s">
+      <c r="H2" s="70" t="s">
         <v>37</v>
       </c>
-      <c r="I2" s="94" t="s">
+      <c r="I2" s="71" t="s">
         <v>38</v>
       </c>
       <c r="J2" s="0"/>
@@ -18351,31 +18346,31 @@
       <c r="AMJ2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="110" t="s">
+      <c r="A3" s="112" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="111" t="s">
+      <c r="B3" s="113" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="112" t="n">
+      <c r="C3" s="114" t="n">
         <v>653272</v>
       </c>
-      <c r="D3" s="113" t="s">
+      <c r="D3" s="115" t="s">
         <v>40</v>
       </c>
-      <c r="E3" s="113" t="s">
+      <c r="E3" s="115" t="s">
         <v>41</v>
       </c>
-      <c r="F3" s="114" t="n">
+      <c r="F3" s="116" t="n">
         <v>8</v>
       </c>
-      <c r="G3" s="115" t="n">
+      <c r="G3" s="84" t="n">
         <v>0</v>
       </c>
-      <c r="H3" s="114" t="n">
+      <c r="H3" s="116" t="n">
         <v>8</v>
       </c>
-      <c r="I3" s="115" t="n">
+      <c r="I3" s="84" t="n">
         <v>0</v>
       </c>
       <c r="J3" s="0"/>
@@ -19395,31 +19390,31 @@
       <c r="AMJ3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="23.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="110" t="s">
+      <c r="A4" s="112" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="111" t="s">
+      <c r="B4" s="113" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="112" t="n">
+      <c r="C4" s="114" t="n">
         <v>653082</v>
       </c>
-      <c r="D4" s="113" t="s">
+      <c r="D4" s="115" t="s">
         <v>40</v>
       </c>
-      <c r="E4" s="113" t="s">
+      <c r="E4" s="115" t="s">
         <v>41</v>
       </c>
-      <c r="F4" s="114" t="n">
+      <c r="F4" s="116" t="n">
         <v>8</v>
       </c>
-      <c r="G4" s="115" t="n">
+      <c r="G4" s="84" t="n">
         <v>0</v>
       </c>
-      <c r="H4" s="114" t="n">
+      <c r="H4" s="116" t="n">
         <v>8</v>
       </c>
-      <c r="I4" s="115" t="n">
+      <c r="I4" s="84" t="n">
         <v>0</v>
       </c>
       <c r="J4" s="0"/>
@@ -20438,117 +20433,117 @@
       <c r="AMI4" s="0"/>
       <c r="AMJ4" s="0"/>
     </row>
-    <row r="5" s="116" customFormat="true" ht="23.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="110" t="s">
+    <row r="5" s="82" customFormat="true" ht="23.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="112" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="111" t="s">
+      <c r="B5" s="113" t="s">
         <v>43</v>
       </c>
-      <c r="C5" s="112" t="n">
+      <c r="C5" s="114" t="n">
         <v>652426</v>
       </c>
-      <c r="D5" s="113" t="s">
+      <c r="D5" s="115" t="s">
         <v>44</v>
       </c>
-      <c r="E5" s="113" t="s">
+      <c r="E5" s="115" t="s">
         <v>45</v>
       </c>
-      <c r="F5" s="114" t="n">
+      <c r="F5" s="116" t="n">
         <v>8</v>
       </c>
-      <c r="G5" s="115" t="n">
+      <c r="G5" s="84" t="n">
         <v>0</v>
       </c>
-      <c r="H5" s="114" t="n">
+      <c r="H5" s="116" t="n">
         <v>8</v>
       </c>
-      <c r="I5" s="115" t="n">
+      <c r="I5" s="84" t="n">
         <v>0</v>
       </c>
       <c r="AMJ5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="110" t="s">
+      <c r="A6" s="112" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="111" t="s">
-        <v>101</v>
-      </c>
-      <c r="C6" s="112" t="n">
+      <c r="B6" s="113" t="s">
+        <v>102</v>
+      </c>
+      <c r="C6" s="114" t="n">
         <v>653546</v>
       </c>
-      <c r="D6" s="113" t="s">
+      <c r="D6" s="115" t="s">
         <v>47</v>
       </c>
-      <c r="E6" s="113" t="s">
+      <c r="E6" s="115" t="s">
         <v>48</v>
       </c>
-      <c r="F6" s="114" t="n">
+      <c r="F6" s="116" t="n">
         <v>4</v>
       </c>
-      <c r="G6" s="115" t="n">
+      <c r="G6" s="84" t="n">
         <v>0</v>
       </c>
-      <c r="H6" s="114" t="n">
+      <c r="H6" s="116" t="n">
         <v>4</v>
       </c>
-      <c r="I6" s="115" t="n">
+      <c r="I6" s="84" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="23.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="110" t="s">
+      <c r="A7" s="112" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="111" t="s">
-        <v>102</v>
-      </c>
-      <c r="C7" s="112" t="n">
+      <c r="B7" s="113" t="s">
+        <v>103</v>
+      </c>
+      <c r="C7" s="114" t="n">
         <v>653545</v>
       </c>
-      <c r="D7" s="113" t="s">
+      <c r="D7" s="115" t="s">
         <v>47</v>
       </c>
-      <c r="E7" s="113" t="s">
+      <c r="E7" s="115" t="s">
         <v>48</v>
       </c>
-      <c r="F7" s="114" t="n">
+      <c r="F7" s="116" t="n">
         <v>4</v>
       </c>
-      <c r="G7" s="115" t="n">
+      <c r="G7" s="84" t="n">
         <v>0</v>
       </c>
-      <c r="H7" s="114" t="n">
+      <c r="H7" s="116" t="n">
         <v>4</v>
       </c>
-      <c r="I7" s="115" t="n">
+      <c r="I7" s="84" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="110" t="s">
+      <c r="A8" s="112" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="111" t="s">
+      <c r="B8" s="113" t="s">
         <v>50</v>
       </c>
-      <c r="C8" s="112" t="n">
+      <c r="C8" s="114" t="n">
         <v>282998</v>
       </c>
-      <c r="D8" s="113" t="s">
+      <c r="D8" s="115" t="s">
         <v>51</v>
       </c>
-      <c r="E8" s="113" t="s">
+      <c r="E8" s="115" t="s">
         <v>45</v>
       </c>
-      <c r="F8" s="115" t="n">
+      <c r="F8" s="84" t="n">
         <v>0</v>
       </c>
       <c r="G8" s="117" t="n">
         <v>6</v>
       </c>
-      <c r="H8" s="115" t="n">
+      <c r="H8" s="84" t="n">
         <v>0</v>
       </c>
       <c r="I8" s="117" t="n">
@@ -20556,28 +20551,28 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="110" t="s">
+      <c r="A9" s="112" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="111" t="s">
+      <c r="B9" s="113" t="s">
         <v>52</v>
       </c>
-      <c r="C9" s="112" t="n">
+      <c r="C9" s="114" t="n">
         <v>610531</v>
       </c>
-      <c r="D9" s="113" t="s">
+      <c r="D9" s="115" t="s">
         <v>53</v>
       </c>
-      <c r="E9" s="113" t="s">
+      <c r="E9" s="115" t="s">
         <v>41</v>
       </c>
-      <c r="F9" s="115" t="n">
+      <c r="F9" s="84" t="n">
         <v>0</v>
       </c>
       <c r="G9" s="117" t="n">
         <v>4</v>
       </c>
-      <c r="H9" s="115" t="n">
+      <c r="H9" s="84" t="n">
         <v>0</v>
       </c>
       <c r="I9" s="117" t="n">
@@ -20585,28 +20580,28 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="110" t="s">
+      <c r="A10" s="112" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="111" t="s">
+      <c r="B10" s="113" t="s">
         <v>54</v>
       </c>
-      <c r="C10" s="112" t="n">
+      <c r="C10" s="114" t="n">
         <v>610528</v>
       </c>
-      <c r="D10" s="113" t="s">
+      <c r="D10" s="115" t="s">
         <v>53</v>
       </c>
-      <c r="E10" s="113" t="s">
+      <c r="E10" s="115" t="s">
         <v>41</v>
       </c>
-      <c r="F10" s="115" t="n">
+      <c r="F10" s="84" t="n">
         <v>0</v>
       </c>
       <c r="G10" s="117" t="n">
         <v>2</v>
       </c>
-      <c r="H10" s="115" t="n">
+      <c r="H10" s="84" t="n">
         <v>0</v>
       </c>
       <c r="I10" s="117" t="n">
@@ -20614,28 +20609,28 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="110" t="s">
+      <c r="A11" s="112" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="111" t="s">
-        <v>103</v>
-      </c>
-      <c r="C11" s="112" t="n">
+      <c r="B11" s="113" t="s">
+        <v>104</v>
+      </c>
+      <c r="C11" s="114" t="n">
         <v>329697</v>
       </c>
-      <c r="D11" s="113" t="s">
+      <c r="D11" s="115" t="s">
         <v>63</v>
       </c>
-      <c r="E11" s="113" t="s">
+      <c r="E11" s="115" t="s">
         <v>41</v>
       </c>
-      <c r="F11" s="115" t="n">
+      <c r="F11" s="84" t="n">
         <v>0</v>
       </c>
       <c r="G11" s="117" t="n">
         <v>2</v>
       </c>
-      <c r="H11" s="115" t="n">
+      <c r="H11" s="84" t="n">
         <v>0</v>
       </c>
       <c r="I11" s="117" t="n">
@@ -20643,28 +20638,28 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="110" t="s">
+      <c r="A12" s="112" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="111" t="s">
+      <c r="B12" s="113" t="s">
         <v>55</v>
       </c>
-      <c r="C12" s="112" t="n">
+      <c r="C12" s="114" t="n">
         <v>600457</v>
       </c>
-      <c r="D12" s="113" t="s">
+      <c r="D12" s="115" t="s">
         <v>56</v>
       </c>
-      <c r="E12" s="113" t="s">
+      <c r="E12" s="115" t="s">
         <v>83</v>
       </c>
-      <c r="F12" s="115" t="n">
+      <c r="F12" s="84" t="n">
         <v>0</v>
       </c>
       <c r="G12" s="117" t="n">
         <v>1</v>
       </c>
-      <c r="H12" s="115" t="n">
+      <c r="H12" s="84" t="n">
         <v>0</v>
       </c>
       <c r="I12" s="117" t="n">
@@ -20672,28 +20667,28 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="110" t="s">
+      <c r="A13" s="112" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="111" t="s">
-        <v>104</v>
-      </c>
-      <c r="C13" s="112" t="n">
+      <c r="B13" s="113" t="s">
+        <v>105</v>
+      </c>
+      <c r="C13" s="114" t="n">
         <v>600458</v>
       </c>
-      <c r="D13" s="113" t="s">
+      <c r="D13" s="115" t="s">
         <v>56</v>
       </c>
-      <c r="E13" s="113" t="s">
+      <c r="E13" s="115" t="s">
         <v>83</v>
       </c>
-      <c r="F13" s="115" t="n">
+      <c r="F13" s="84" t="n">
         <v>0</v>
       </c>
       <c r="G13" s="117" t="n">
         <v>1</v>
       </c>
-      <c r="H13" s="115" t="n">
+      <c r="H13" s="84" t="n">
         <v>0</v>
       </c>
       <c r="I13" s="117" t="n">
@@ -20701,28 +20696,28 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="110" t="s">
+      <c r="A14" s="112" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="111" t="s">
+      <c r="B14" s="113" t="s">
         <v>58</v>
       </c>
-      <c r="C14" s="112" t="n">
+      <c r="C14" s="114" t="n">
         <v>510190</v>
       </c>
-      <c r="D14" s="113" t="s">
+      <c r="D14" s="115" t="s">
         <v>80</v>
       </c>
-      <c r="E14" s="113" t="s">
+      <c r="E14" s="115" t="s">
         <v>48</v>
       </c>
-      <c r="F14" s="115" t="n">
+      <c r="F14" s="84" t="n">
         <v>0</v>
       </c>
       <c r="G14" s="117" t="n">
         <v>2</v>
       </c>
-      <c r="H14" s="115" t="n">
+      <c r="H14" s="84" t="n">
         <v>0</v>
       </c>
       <c r="I14" s="117" t="n">
@@ -20730,28 +20725,28 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="110" t="s">
+      <c r="A15" s="112" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="111" t="s">
+      <c r="B15" s="113" t="s">
         <v>60</v>
       </c>
-      <c r="C15" s="112" t="n">
+      <c r="C15" s="114" t="n">
         <v>613092</v>
       </c>
-      <c r="D15" s="113" t="s">
+      <c r="D15" s="115" t="s">
         <v>80</v>
       </c>
-      <c r="E15" s="113" t="s">
+      <c r="E15" s="115" t="s">
         <v>48</v>
       </c>
-      <c r="F15" s="115" t="n">
+      <c r="F15" s="84" t="n">
         <v>0</v>
       </c>
       <c r="G15" s="117" t="n">
         <v>1</v>
       </c>
-      <c r="H15" s="115" t="n">
+      <c r="H15" s="84" t="n">
         <v>0</v>
       </c>
       <c r="I15" s="117" t="n">
@@ -20759,28 +20754,28 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="110" t="s">
+      <c r="A16" s="112" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="111" t="s">
+      <c r="B16" s="113" t="s">
         <v>64</v>
       </c>
-      <c r="C16" s="112" t="n">
+      <c r="C16" s="114" t="n">
         <v>528655</v>
       </c>
-      <c r="D16" s="113" t="s">
+      <c r="D16" s="115" t="s">
         <v>65</v>
       </c>
-      <c r="E16" s="113" t="s">
-        <v>105</v>
-      </c>
-      <c r="F16" s="115" t="n">
+      <c r="E16" s="115" t="s">
+        <v>86</v>
+      </c>
+      <c r="F16" s="84" t="n">
         <v>0</v>
       </c>
       <c r="G16" s="117" t="n">
         <v>2</v>
       </c>
-      <c r="H16" s="115" t="n">
+      <c r="H16" s="84" t="n">
         <v>0</v>
       </c>
       <c r="I16" s="117" t="n">
@@ -20794,30 +20789,30 @@
       <c r="B17" s="119" t="s">
         <v>67</v>
       </c>
-      <c r="C17" s="112" t="n">
+      <c r="C17" s="114" t="n">
         <v>490435</v>
       </c>
-      <c r="D17" s="113" t="s">
+      <c r="D17" s="115" t="s">
         <v>65</v>
       </c>
-      <c r="E17" s="113" t="s">
+      <c r="E17" s="115" t="s">
         <v>66</v>
       </c>
-      <c r="F17" s="97" t="n">
+      <c r="F17" s="100" t="n">
         <v>0</v>
       </c>
-      <c r="G17" s="97" t="n">
+      <c r="G17" s="100" t="n">
         <v>0</v>
       </c>
-      <c r="H17" s="97" t="n">
+      <c r="H17" s="100" t="n">
         <v>0</v>
       </c>
-      <c r="I17" s="97" t="n">
+      <c r="I17" s="100" t="n">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:F16"/>
+  <autoFilter ref="A2:G16"/>
   <mergeCells count="1">
     <mergeCell ref="F1:I1"/>
   </mergeCells>

</xml_diff>

<commit_message>
PROS-7371 BIVN Brand Block remove
</commit_message>
<xml_diff>
--- a/Projects/BIVN/Data/Template.xlsx
+++ b/Projects/BIVN/Data/Template.xlsx
@@ -17,7 +17,7 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">MSL!$A$2:$G$16</definedName>
-    <definedName function="false" hidden="true" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$16</definedName>
+    <definedName function="false" hidden="true" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$F$16</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_FilterDatabase_0" vbProcedure="false">MSL!$A$2:$G$16</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">MSL!$A$2:$G$16</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">MSL!$A$2:$G$16</definedName>
@@ -34,6 +34,7 @@
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$G$16</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$G$16</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$G$16</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$G$16</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">'Primary Shelf_Location'!$A$2:$G$2</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">MSL!$A$2:$E$2</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">MSL!$A$2:$E$2</definedName>
@@ -52,21 +53,22 @@
     <definedName function="false" hidden="false" localSheetId="5" name="_FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$F$16</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$F$16</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$F$16</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$F$16</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$16</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$F$16</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$16</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$F$16</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$16</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$F$16</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$16</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$F$16</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$16</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$F$16</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$16</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$F$16</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$16</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$F$16</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$16</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$F$16</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$16</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$F$16</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$16</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$F$16</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$16</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$F$16</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$16</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$F$16</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$16</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$F$16</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$16</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$F$16</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$16</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$F$16</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -77,67 +79,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <authors>
-    <author/>
-  </authors>
-  <commentList>
-    <comment ref="B3" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">To be identical to SKUs Brand in Trax DB</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C3" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b val="true"/>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="204"/>
-          </rPr>
-          <t xml:space="preserve">To be </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="204"/>
-          </rPr>
-          <t xml:space="preserve">identical</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve"> to SKUs Category in Trax DB</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="94">
   <si>
     <t xml:space="preserve">KPI Name</t>
   </si>
@@ -358,57 +301,6 @@
     <t xml:space="preserve">Points</t>
   </si>
   <si>
-    <t xml:space="preserve">Pharmaton Bottle (30s),
-Pharmaton Kiddi Syrup 100ml (Bottle)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">653272,653082</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bisolvon Tab 8mg 30s,
-Bisolvon Kids Syrup 60ml (Bottle)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">653546,653545</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Calcium Corbiere 10ml x 30
-Calcium Corbiere 5ml x 30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">610531,610528</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MAGNE-B6 Tab B/50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Acemuc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Acemuc 200mg H/30 
-Acemuc 100mg H/30 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">510190,613092</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Allergy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Telfast BD 60mg
-Telfast HD 180mg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">600457,600458</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Baby Care</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lactacyd BB 250ML
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">Purple Frame</t>
   </si>
   <si>
@@ -460,7 +352,16 @@
     <t xml:space="preserve">Magne-B6 Corbiere Tab B50</t>
   </si>
   <si>
+    <t xml:space="preserve">Allergy</t>
+  </si>
+  <si>
     <t xml:space="preserve">Telfast  HD 180mg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acemuc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Baby Care</t>
   </si>
 </sst>
 </file>
@@ -473,7 +374,7 @@
     <numFmt numFmtId="166" formatCode="0.00"/>
     <numFmt numFmtId="167" formatCode="0"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -612,21 +513,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-      <charset val="204"/>
     </font>
   </fonts>
   <fills count="13">
@@ -1568,12 +1454,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="28.7085020242915"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="24.3157894736842"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="20.5668016194332"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="22.4939271255061"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="24.2105263157895"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="16.9230769230769"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="28.9230769230769"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="24.5303643724696"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="20.6720647773279"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="24.4251012145749"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="17.0323886639676"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1839,11 +1725,11 @@
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="23" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="23" width="36.6356275303644"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="23" width="26.3522267206478"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="23" width="23.4574898785425"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="23" width="22.8178137651822"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="23" width="15.7449392712551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="23" width="36.9554655870445"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="23" width="26.5668016194332"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="23" width="23.5668016194332"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="23" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="23" width="15.8542510121457"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="23" width="13.9271255060729"/>
     <col collapsed="false" hidden="false" max="1023" min="8" style="23" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="9.10526315789474"/>
@@ -16599,7 +16485,7 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="50" width="13.6032388663968"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="50" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="50" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="50" width="23.5668016194332"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="50" width="23.6720647773279"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="50" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="7" min="6" style="50" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="50" width="9.10526315789474"/>
@@ -16670,7 +16556,7 @@
   <dimension ref="1:11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
+      <selection pane="topLeft" activeCell="F26" activeCellId="0" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -16678,8 +16564,8 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="61" width="13.8178137651822"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="61" width="10.8178137651822"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="61" width="13.7125506072874"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="46.2753036437247"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="61" width="21.3157894736842"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="46.5951417004049"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="61" width="21.5303643724696"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="61" width="10.9271255060729"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="61" width="10.497975708502"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="1" width="13.3886639676113"/>
@@ -16698,6 +16584,1021 @@
       <c r="G1" s="64"/>
       <c r="H1" s="64"/>
       <c r="I1" s="64"/>
+      <c r="J1" s="0"/>
+      <c r="K1" s="0"/>
+      <c r="L1" s="0"/>
+      <c r="M1" s="0"/>
+      <c r="N1" s="0"/>
+      <c r="O1" s="0"/>
+      <c r="P1" s="0"/>
+      <c r="Q1" s="0"/>
+      <c r="R1" s="0"/>
+      <c r="S1" s="0"/>
+      <c r="T1" s="0"/>
+      <c r="U1" s="0"/>
+      <c r="V1" s="0"/>
+      <c r="W1" s="0"/>
+      <c r="X1" s="0"/>
+      <c r="Y1" s="0"/>
+      <c r="Z1" s="0"/>
+      <c r="AA1" s="0"/>
+      <c r="AB1" s="0"/>
+      <c r="AC1" s="0"/>
+      <c r="AD1" s="0"/>
+      <c r="AE1" s="0"/>
+      <c r="AF1" s="0"/>
+      <c r="AG1" s="0"/>
+      <c r="AH1" s="0"/>
+      <c r="AI1" s="0"/>
+      <c r="AJ1" s="0"/>
+      <c r="AK1" s="0"/>
+      <c r="AL1" s="0"/>
+      <c r="AM1" s="0"/>
+      <c r="AN1" s="0"/>
+      <c r="AO1" s="0"/>
+      <c r="AP1" s="0"/>
+      <c r="AQ1" s="0"/>
+      <c r="AR1" s="0"/>
+      <c r="AS1" s="0"/>
+      <c r="AT1" s="0"/>
+      <c r="AU1" s="0"/>
+      <c r="AV1" s="0"/>
+      <c r="AW1" s="0"/>
+      <c r="AX1" s="0"/>
+      <c r="AY1" s="0"/>
+      <c r="AZ1" s="0"/>
+      <c r="BA1" s="0"/>
+      <c r="BB1" s="0"/>
+      <c r="BC1" s="0"/>
+      <c r="BD1" s="0"/>
+      <c r="BE1" s="0"/>
+      <c r="BF1" s="0"/>
+      <c r="BG1" s="0"/>
+      <c r="BH1" s="0"/>
+      <c r="BI1" s="0"/>
+      <c r="BJ1" s="0"/>
+      <c r="BK1" s="0"/>
+      <c r="BL1" s="0"/>
+      <c r="BM1" s="0"/>
+      <c r="BN1" s="0"/>
+      <c r="BO1" s="0"/>
+      <c r="BP1" s="0"/>
+      <c r="BQ1" s="0"/>
+      <c r="BR1" s="0"/>
+      <c r="BS1" s="0"/>
+      <c r="BT1" s="0"/>
+      <c r="BU1" s="0"/>
+      <c r="BV1" s="0"/>
+      <c r="BW1" s="0"/>
+      <c r="BX1" s="0"/>
+      <c r="BY1" s="0"/>
+      <c r="BZ1" s="0"/>
+      <c r="CA1" s="0"/>
+      <c r="CB1" s="0"/>
+      <c r="CC1" s="0"/>
+      <c r="CD1" s="0"/>
+      <c r="CE1" s="0"/>
+      <c r="CF1" s="0"/>
+      <c r="CG1" s="0"/>
+      <c r="CH1" s="0"/>
+      <c r="CI1" s="0"/>
+      <c r="CJ1" s="0"/>
+      <c r="CK1" s="0"/>
+      <c r="CL1" s="0"/>
+      <c r="CM1" s="0"/>
+      <c r="CN1" s="0"/>
+      <c r="CO1" s="0"/>
+      <c r="CP1" s="0"/>
+      <c r="CQ1" s="0"/>
+      <c r="CR1" s="0"/>
+      <c r="CS1" s="0"/>
+      <c r="CT1" s="0"/>
+      <c r="CU1" s="0"/>
+      <c r="CV1" s="0"/>
+      <c r="CW1" s="0"/>
+      <c r="CX1" s="0"/>
+      <c r="CY1" s="0"/>
+      <c r="CZ1" s="0"/>
+      <c r="DA1" s="0"/>
+      <c r="DB1" s="0"/>
+      <c r="DC1" s="0"/>
+      <c r="DD1" s="0"/>
+      <c r="DE1" s="0"/>
+      <c r="DF1" s="0"/>
+      <c r="DG1" s="0"/>
+      <c r="DH1" s="0"/>
+      <c r="DI1" s="0"/>
+      <c r="DJ1" s="0"/>
+      <c r="DK1" s="0"/>
+      <c r="DL1" s="0"/>
+      <c r="DM1" s="0"/>
+      <c r="DN1" s="0"/>
+      <c r="DO1" s="0"/>
+      <c r="DP1" s="0"/>
+      <c r="DQ1" s="0"/>
+      <c r="DR1" s="0"/>
+      <c r="DS1" s="0"/>
+      <c r="DT1" s="0"/>
+      <c r="DU1" s="0"/>
+      <c r="DV1" s="0"/>
+      <c r="DW1" s="0"/>
+      <c r="DX1" s="0"/>
+      <c r="DY1" s="0"/>
+      <c r="DZ1" s="0"/>
+      <c r="EA1" s="0"/>
+      <c r="EB1" s="0"/>
+      <c r="EC1" s="0"/>
+      <c r="ED1" s="0"/>
+      <c r="EE1" s="0"/>
+      <c r="EF1" s="0"/>
+      <c r="EG1" s="0"/>
+      <c r="EH1" s="0"/>
+      <c r="EI1" s="0"/>
+      <c r="EJ1" s="0"/>
+      <c r="EK1" s="0"/>
+      <c r="EL1" s="0"/>
+      <c r="EM1" s="0"/>
+      <c r="EN1" s="0"/>
+      <c r="EO1" s="0"/>
+      <c r="EP1" s="0"/>
+      <c r="EQ1" s="0"/>
+      <c r="ER1" s="0"/>
+      <c r="ES1" s="0"/>
+      <c r="ET1" s="0"/>
+      <c r="EU1" s="0"/>
+      <c r="EV1" s="0"/>
+      <c r="EW1" s="0"/>
+      <c r="EX1" s="0"/>
+      <c r="EY1" s="0"/>
+      <c r="EZ1" s="0"/>
+      <c r="FA1" s="0"/>
+      <c r="FB1" s="0"/>
+      <c r="FC1" s="0"/>
+      <c r="FD1" s="0"/>
+      <c r="FE1" s="0"/>
+      <c r="FF1" s="0"/>
+      <c r="FG1" s="0"/>
+      <c r="FH1" s="0"/>
+      <c r="FI1" s="0"/>
+      <c r="FJ1" s="0"/>
+      <c r="FK1" s="0"/>
+      <c r="FL1" s="0"/>
+      <c r="FM1" s="0"/>
+      <c r="FN1" s="0"/>
+      <c r="FO1" s="0"/>
+      <c r="FP1" s="0"/>
+      <c r="FQ1" s="0"/>
+      <c r="FR1" s="0"/>
+      <c r="FS1" s="0"/>
+      <c r="FT1" s="0"/>
+      <c r="FU1" s="0"/>
+      <c r="FV1" s="0"/>
+      <c r="FW1" s="0"/>
+      <c r="FX1" s="0"/>
+      <c r="FY1" s="0"/>
+      <c r="FZ1" s="0"/>
+      <c r="GA1" s="0"/>
+      <c r="GB1" s="0"/>
+      <c r="GC1" s="0"/>
+      <c r="GD1" s="0"/>
+      <c r="GE1" s="0"/>
+      <c r="GF1" s="0"/>
+      <c r="GG1" s="0"/>
+      <c r="GH1" s="0"/>
+      <c r="GI1" s="0"/>
+      <c r="GJ1" s="0"/>
+      <c r="GK1" s="0"/>
+      <c r="GL1" s="0"/>
+      <c r="GM1" s="0"/>
+      <c r="GN1" s="0"/>
+      <c r="GO1" s="0"/>
+      <c r="GP1" s="0"/>
+      <c r="GQ1" s="0"/>
+      <c r="GR1" s="0"/>
+      <c r="GS1" s="0"/>
+      <c r="GT1" s="0"/>
+      <c r="GU1" s="0"/>
+      <c r="GV1" s="0"/>
+      <c r="GW1" s="0"/>
+      <c r="GX1" s="0"/>
+      <c r="GY1" s="0"/>
+      <c r="GZ1" s="0"/>
+      <c r="HA1" s="0"/>
+      <c r="HB1" s="0"/>
+      <c r="HC1" s="0"/>
+      <c r="HD1" s="0"/>
+      <c r="HE1" s="0"/>
+      <c r="HF1" s="0"/>
+      <c r="HG1" s="0"/>
+      <c r="HH1" s="0"/>
+      <c r="HI1" s="0"/>
+      <c r="HJ1" s="0"/>
+      <c r="HK1" s="0"/>
+      <c r="HL1" s="0"/>
+      <c r="HM1" s="0"/>
+      <c r="HN1" s="0"/>
+      <c r="HO1" s="0"/>
+      <c r="HP1" s="0"/>
+      <c r="HQ1" s="0"/>
+      <c r="HR1" s="0"/>
+      <c r="HS1" s="0"/>
+      <c r="HT1" s="0"/>
+      <c r="HU1" s="0"/>
+      <c r="HV1" s="0"/>
+      <c r="HW1" s="0"/>
+      <c r="HX1" s="0"/>
+      <c r="HY1" s="0"/>
+      <c r="HZ1" s="0"/>
+      <c r="IA1" s="0"/>
+      <c r="IB1" s="0"/>
+      <c r="IC1" s="0"/>
+      <c r="ID1" s="0"/>
+      <c r="IE1" s="0"/>
+      <c r="IF1" s="0"/>
+      <c r="IG1" s="0"/>
+      <c r="IH1" s="0"/>
+      <c r="II1" s="0"/>
+      <c r="IJ1" s="0"/>
+      <c r="IK1" s="0"/>
+      <c r="IL1" s="0"/>
+      <c r="IM1" s="0"/>
+      <c r="IN1" s="0"/>
+      <c r="IO1" s="0"/>
+      <c r="IP1" s="0"/>
+      <c r="IQ1" s="0"/>
+      <c r="IR1" s="0"/>
+      <c r="IS1" s="0"/>
+      <c r="IT1" s="0"/>
+      <c r="IU1" s="0"/>
+      <c r="IV1" s="0"/>
+      <c r="IW1" s="0"/>
+      <c r="IX1" s="0"/>
+      <c r="IY1" s="0"/>
+      <c r="IZ1" s="0"/>
+      <c r="JA1" s="0"/>
+      <c r="JB1" s="0"/>
+      <c r="JC1" s="0"/>
+      <c r="JD1" s="0"/>
+      <c r="JE1" s="0"/>
+      <c r="JF1" s="0"/>
+      <c r="JG1" s="0"/>
+      <c r="JH1" s="0"/>
+      <c r="JI1" s="0"/>
+      <c r="JJ1" s="0"/>
+      <c r="JK1" s="0"/>
+      <c r="JL1" s="0"/>
+      <c r="JM1" s="0"/>
+      <c r="JN1" s="0"/>
+      <c r="JO1" s="0"/>
+      <c r="JP1" s="0"/>
+      <c r="JQ1" s="0"/>
+      <c r="JR1" s="0"/>
+      <c r="JS1" s="0"/>
+      <c r="JT1" s="0"/>
+      <c r="JU1" s="0"/>
+      <c r="JV1" s="0"/>
+      <c r="JW1" s="0"/>
+      <c r="JX1" s="0"/>
+      <c r="JY1" s="0"/>
+      <c r="JZ1" s="0"/>
+      <c r="KA1" s="0"/>
+      <c r="KB1" s="0"/>
+      <c r="KC1" s="0"/>
+      <c r="KD1" s="0"/>
+      <c r="KE1" s="0"/>
+      <c r="KF1" s="0"/>
+      <c r="KG1" s="0"/>
+      <c r="KH1" s="0"/>
+      <c r="KI1" s="0"/>
+      <c r="KJ1" s="0"/>
+      <c r="KK1" s="0"/>
+      <c r="KL1" s="0"/>
+      <c r="KM1" s="0"/>
+      <c r="KN1" s="0"/>
+      <c r="KO1" s="0"/>
+      <c r="KP1" s="0"/>
+      <c r="KQ1" s="0"/>
+      <c r="KR1" s="0"/>
+      <c r="KS1" s="0"/>
+      <c r="KT1" s="0"/>
+      <c r="KU1" s="0"/>
+      <c r="KV1" s="0"/>
+      <c r="KW1" s="0"/>
+      <c r="KX1" s="0"/>
+      <c r="KY1" s="0"/>
+      <c r="KZ1" s="0"/>
+      <c r="LA1" s="0"/>
+      <c r="LB1" s="0"/>
+      <c r="LC1" s="0"/>
+      <c r="LD1" s="0"/>
+      <c r="LE1" s="0"/>
+      <c r="LF1" s="0"/>
+      <c r="LG1" s="0"/>
+      <c r="LH1" s="0"/>
+      <c r="LI1" s="0"/>
+      <c r="LJ1" s="0"/>
+      <c r="LK1" s="0"/>
+      <c r="LL1" s="0"/>
+      <c r="LM1" s="0"/>
+      <c r="LN1" s="0"/>
+      <c r="LO1" s="0"/>
+      <c r="LP1" s="0"/>
+      <c r="LQ1" s="0"/>
+      <c r="LR1" s="0"/>
+      <c r="LS1" s="0"/>
+      <c r="LT1" s="0"/>
+      <c r="LU1" s="0"/>
+      <c r="LV1" s="0"/>
+      <c r="LW1" s="0"/>
+      <c r="LX1" s="0"/>
+      <c r="LY1" s="0"/>
+      <c r="LZ1" s="0"/>
+      <c r="MA1" s="0"/>
+      <c r="MB1" s="0"/>
+      <c r="MC1" s="0"/>
+      <c r="MD1" s="0"/>
+      <c r="ME1" s="0"/>
+      <c r="MF1" s="0"/>
+      <c r="MG1" s="0"/>
+      <c r="MH1" s="0"/>
+      <c r="MI1" s="0"/>
+      <c r="MJ1" s="0"/>
+      <c r="MK1" s="0"/>
+      <c r="ML1" s="0"/>
+      <c r="MM1" s="0"/>
+      <c r="MN1" s="0"/>
+      <c r="MO1" s="0"/>
+      <c r="MP1" s="0"/>
+      <c r="MQ1" s="0"/>
+      <c r="MR1" s="0"/>
+      <c r="MS1" s="0"/>
+      <c r="MT1" s="0"/>
+      <c r="MU1" s="0"/>
+      <c r="MV1" s="0"/>
+      <c r="MW1" s="0"/>
+      <c r="MX1" s="0"/>
+      <c r="MY1" s="0"/>
+      <c r="MZ1" s="0"/>
+      <c r="NA1" s="0"/>
+      <c r="NB1" s="0"/>
+      <c r="NC1" s="0"/>
+      <c r="ND1" s="0"/>
+      <c r="NE1" s="0"/>
+      <c r="NF1" s="0"/>
+      <c r="NG1" s="0"/>
+      <c r="NH1" s="0"/>
+      <c r="NI1" s="0"/>
+      <c r="NJ1" s="0"/>
+      <c r="NK1" s="0"/>
+      <c r="NL1" s="0"/>
+      <c r="NM1" s="0"/>
+      <c r="NN1" s="0"/>
+      <c r="NO1" s="0"/>
+      <c r="NP1" s="0"/>
+      <c r="NQ1" s="0"/>
+      <c r="NR1" s="0"/>
+      <c r="NS1" s="0"/>
+      <c r="NT1" s="0"/>
+      <c r="NU1" s="0"/>
+      <c r="NV1" s="0"/>
+      <c r="NW1" s="0"/>
+      <c r="NX1" s="0"/>
+      <c r="NY1" s="0"/>
+      <c r="NZ1" s="0"/>
+      <c r="OA1" s="0"/>
+      <c r="OB1" s="0"/>
+      <c r="OC1" s="0"/>
+      <c r="OD1" s="0"/>
+      <c r="OE1" s="0"/>
+      <c r="OF1" s="0"/>
+      <c r="OG1" s="0"/>
+      <c r="OH1" s="0"/>
+      <c r="OI1" s="0"/>
+      <c r="OJ1" s="0"/>
+      <c r="OK1" s="0"/>
+      <c r="OL1" s="0"/>
+      <c r="OM1" s="0"/>
+      <c r="ON1" s="0"/>
+      <c r="OO1" s="0"/>
+      <c r="OP1" s="0"/>
+      <c r="OQ1" s="0"/>
+      <c r="OR1" s="0"/>
+      <c r="OS1" s="0"/>
+      <c r="OT1" s="0"/>
+      <c r="OU1" s="0"/>
+      <c r="OV1" s="0"/>
+      <c r="OW1" s="0"/>
+      <c r="OX1" s="0"/>
+      <c r="OY1" s="0"/>
+      <c r="OZ1" s="0"/>
+      <c r="PA1" s="0"/>
+      <c r="PB1" s="0"/>
+      <c r="PC1" s="0"/>
+      <c r="PD1" s="0"/>
+      <c r="PE1" s="0"/>
+      <c r="PF1" s="0"/>
+      <c r="PG1" s="0"/>
+      <c r="PH1" s="0"/>
+      <c r="PI1" s="0"/>
+      <c r="PJ1" s="0"/>
+      <c r="PK1" s="0"/>
+      <c r="PL1" s="0"/>
+      <c r="PM1" s="0"/>
+      <c r="PN1" s="0"/>
+      <c r="PO1" s="0"/>
+      <c r="PP1" s="0"/>
+      <c r="PQ1" s="0"/>
+      <c r="PR1" s="0"/>
+      <c r="PS1" s="0"/>
+      <c r="PT1" s="0"/>
+      <c r="PU1" s="0"/>
+      <c r="PV1" s="0"/>
+      <c r="PW1" s="0"/>
+      <c r="PX1" s="0"/>
+      <c r="PY1" s="0"/>
+      <c r="PZ1" s="0"/>
+      <c r="QA1" s="0"/>
+      <c r="QB1" s="0"/>
+      <c r="QC1" s="0"/>
+      <c r="QD1" s="0"/>
+      <c r="QE1" s="0"/>
+      <c r="QF1" s="0"/>
+      <c r="QG1" s="0"/>
+      <c r="QH1" s="0"/>
+      <c r="QI1" s="0"/>
+      <c r="QJ1" s="0"/>
+      <c r="QK1" s="0"/>
+      <c r="QL1" s="0"/>
+      <c r="QM1" s="0"/>
+      <c r="QN1" s="0"/>
+      <c r="QO1" s="0"/>
+      <c r="QP1" s="0"/>
+      <c r="QQ1" s="0"/>
+      <c r="QR1" s="0"/>
+      <c r="QS1" s="0"/>
+      <c r="QT1" s="0"/>
+      <c r="QU1" s="0"/>
+      <c r="QV1" s="0"/>
+      <c r="QW1" s="0"/>
+      <c r="QX1" s="0"/>
+      <c r="QY1" s="0"/>
+      <c r="QZ1" s="0"/>
+      <c r="RA1" s="0"/>
+      <c r="RB1" s="0"/>
+      <c r="RC1" s="0"/>
+      <c r="RD1" s="0"/>
+      <c r="RE1" s="0"/>
+      <c r="RF1" s="0"/>
+      <c r="RG1" s="0"/>
+      <c r="RH1" s="0"/>
+      <c r="RI1" s="0"/>
+      <c r="RJ1" s="0"/>
+      <c r="RK1" s="0"/>
+      <c r="RL1" s="0"/>
+      <c r="RM1" s="0"/>
+      <c r="RN1" s="0"/>
+      <c r="RO1" s="0"/>
+      <c r="RP1" s="0"/>
+      <c r="RQ1" s="0"/>
+      <c r="RR1" s="0"/>
+      <c r="RS1" s="0"/>
+      <c r="RT1" s="0"/>
+      <c r="RU1" s="0"/>
+      <c r="RV1" s="0"/>
+      <c r="RW1" s="0"/>
+      <c r="RX1" s="0"/>
+      <c r="RY1" s="0"/>
+      <c r="RZ1" s="0"/>
+      <c r="SA1" s="0"/>
+      <c r="SB1" s="0"/>
+      <c r="SC1" s="0"/>
+      <c r="SD1" s="0"/>
+      <c r="SE1" s="0"/>
+      <c r="SF1" s="0"/>
+      <c r="SG1" s="0"/>
+      <c r="SH1" s="0"/>
+      <c r="SI1" s="0"/>
+      <c r="SJ1" s="0"/>
+      <c r="SK1" s="0"/>
+      <c r="SL1" s="0"/>
+      <c r="SM1" s="0"/>
+      <c r="SN1" s="0"/>
+      <c r="SO1" s="0"/>
+      <c r="SP1" s="0"/>
+      <c r="SQ1" s="0"/>
+      <c r="SR1" s="0"/>
+      <c r="SS1" s="0"/>
+      <c r="ST1" s="0"/>
+      <c r="SU1" s="0"/>
+      <c r="SV1" s="0"/>
+      <c r="SW1" s="0"/>
+      <c r="SX1" s="0"/>
+      <c r="SY1" s="0"/>
+      <c r="SZ1" s="0"/>
+      <c r="TA1" s="0"/>
+      <c r="TB1" s="0"/>
+      <c r="TC1" s="0"/>
+      <c r="TD1" s="0"/>
+      <c r="TE1" s="0"/>
+      <c r="TF1" s="0"/>
+      <c r="TG1" s="0"/>
+      <c r="TH1" s="0"/>
+      <c r="TI1" s="0"/>
+      <c r="TJ1" s="0"/>
+      <c r="TK1" s="0"/>
+      <c r="TL1" s="0"/>
+      <c r="TM1" s="0"/>
+      <c r="TN1" s="0"/>
+      <c r="TO1" s="0"/>
+      <c r="TP1" s="0"/>
+      <c r="TQ1" s="0"/>
+      <c r="TR1" s="0"/>
+      <c r="TS1" s="0"/>
+      <c r="TT1" s="0"/>
+      <c r="TU1" s="0"/>
+      <c r="TV1" s="0"/>
+      <c r="TW1" s="0"/>
+      <c r="TX1" s="0"/>
+      <c r="TY1" s="0"/>
+      <c r="TZ1" s="0"/>
+      <c r="UA1" s="0"/>
+      <c r="UB1" s="0"/>
+      <c r="UC1" s="0"/>
+      <c r="UD1" s="0"/>
+      <c r="UE1" s="0"/>
+      <c r="UF1" s="0"/>
+      <c r="UG1" s="0"/>
+      <c r="UH1" s="0"/>
+      <c r="UI1" s="0"/>
+      <c r="UJ1" s="0"/>
+      <c r="UK1" s="0"/>
+      <c r="UL1" s="0"/>
+      <c r="UM1" s="0"/>
+      <c r="UN1" s="0"/>
+      <c r="UO1" s="0"/>
+      <c r="UP1" s="0"/>
+      <c r="UQ1" s="0"/>
+      <c r="UR1" s="0"/>
+      <c r="US1" s="0"/>
+      <c r="UT1" s="0"/>
+      <c r="UU1" s="0"/>
+      <c r="UV1" s="0"/>
+      <c r="UW1" s="0"/>
+      <c r="UX1" s="0"/>
+      <c r="UY1" s="0"/>
+      <c r="UZ1" s="0"/>
+      <c r="VA1" s="0"/>
+      <c r="VB1" s="0"/>
+      <c r="VC1" s="0"/>
+      <c r="VD1" s="0"/>
+      <c r="VE1" s="0"/>
+      <c r="VF1" s="0"/>
+      <c r="VG1" s="0"/>
+      <c r="VH1" s="0"/>
+      <c r="VI1" s="0"/>
+      <c r="VJ1" s="0"/>
+      <c r="VK1" s="0"/>
+      <c r="VL1" s="0"/>
+      <c r="VM1" s="0"/>
+      <c r="VN1" s="0"/>
+      <c r="VO1" s="0"/>
+      <c r="VP1" s="0"/>
+      <c r="VQ1" s="0"/>
+      <c r="VR1" s="0"/>
+      <c r="VS1" s="0"/>
+      <c r="VT1" s="0"/>
+      <c r="VU1" s="0"/>
+      <c r="VV1" s="0"/>
+      <c r="VW1" s="0"/>
+      <c r="VX1" s="0"/>
+      <c r="VY1" s="0"/>
+      <c r="VZ1" s="0"/>
+      <c r="WA1" s="0"/>
+      <c r="WB1" s="0"/>
+      <c r="WC1" s="0"/>
+      <c r="WD1" s="0"/>
+      <c r="WE1" s="0"/>
+      <c r="WF1" s="0"/>
+      <c r="WG1" s="0"/>
+      <c r="WH1" s="0"/>
+      <c r="WI1" s="0"/>
+      <c r="WJ1" s="0"/>
+      <c r="WK1" s="0"/>
+      <c r="WL1" s="0"/>
+      <c r="WM1" s="0"/>
+      <c r="WN1" s="0"/>
+      <c r="WO1" s="0"/>
+      <c r="WP1" s="0"/>
+      <c r="WQ1" s="0"/>
+      <c r="WR1" s="0"/>
+      <c r="WS1" s="0"/>
+      <c r="WT1" s="0"/>
+      <c r="WU1" s="0"/>
+      <c r="WV1" s="0"/>
+      <c r="WW1" s="0"/>
+      <c r="WX1" s="0"/>
+      <c r="WY1" s="0"/>
+      <c r="WZ1" s="0"/>
+      <c r="XA1" s="0"/>
+      <c r="XB1" s="0"/>
+      <c r="XC1" s="0"/>
+      <c r="XD1" s="0"/>
+      <c r="XE1" s="0"/>
+      <c r="XF1" s="0"/>
+      <c r="XG1" s="0"/>
+      <c r="XH1" s="0"/>
+      <c r="XI1" s="0"/>
+      <c r="XJ1" s="0"/>
+      <c r="XK1" s="0"/>
+      <c r="XL1" s="0"/>
+      <c r="XM1" s="0"/>
+      <c r="XN1" s="0"/>
+      <c r="XO1" s="0"/>
+      <c r="XP1" s="0"/>
+      <c r="XQ1" s="0"/>
+      <c r="XR1" s="0"/>
+      <c r="XS1" s="0"/>
+      <c r="XT1" s="0"/>
+      <c r="XU1" s="0"/>
+      <c r="XV1" s="0"/>
+      <c r="XW1" s="0"/>
+      <c r="XX1" s="0"/>
+      <c r="XY1" s="0"/>
+      <c r="XZ1" s="0"/>
+      <c r="YA1" s="0"/>
+      <c r="YB1" s="0"/>
+      <c r="YC1" s="0"/>
+      <c r="YD1" s="0"/>
+      <c r="YE1" s="0"/>
+      <c r="YF1" s="0"/>
+      <c r="YG1" s="0"/>
+      <c r="YH1" s="0"/>
+      <c r="YI1" s="0"/>
+      <c r="YJ1" s="0"/>
+      <c r="YK1" s="0"/>
+      <c r="YL1" s="0"/>
+      <c r="YM1" s="0"/>
+      <c r="YN1" s="0"/>
+      <c r="YO1" s="0"/>
+      <c r="YP1" s="0"/>
+      <c r="YQ1" s="0"/>
+      <c r="YR1" s="0"/>
+      <c r="YS1" s="0"/>
+      <c r="YT1" s="0"/>
+      <c r="YU1" s="0"/>
+      <c r="YV1" s="0"/>
+      <c r="YW1" s="0"/>
+      <c r="YX1" s="0"/>
+      <c r="YY1" s="0"/>
+      <c r="YZ1" s="0"/>
+      <c r="ZA1" s="0"/>
+      <c r="ZB1" s="0"/>
+      <c r="ZC1" s="0"/>
+      <c r="ZD1" s="0"/>
+      <c r="ZE1" s="0"/>
+      <c r="ZF1" s="0"/>
+      <c r="ZG1" s="0"/>
+      <c r="ZH1" s="0"/>
+      <c r="ZI1" s="0"/>
+      <c r="ZJ1" s="0"/>
+      <c r="ZK1" s="0"/>
+      <c r="ZL1" s="0"/>
+      <c r="ZM1" s="0"/>
+      <c r="ZN1" s="0"/>
+      <c r="ZO1" s="0"/>
+      <c r="ZP1" s="0"/>
+      <c r="ZQ1" s="0"/>
+      <c r="ZR1" s="0"/>
+      <c r="ZS1" s="0"/>
+      <c r="ZT1" s="0"/>
+      <c r="ZU1" s="0"/>
+      <c r="ZV1" s="0"/>
+      <c r="ZW1" s="0"/>
+      <c r="ZX1" s="0"/>
+      <c r="ZY1" s="0"/>
+      <c r="ZZ1" s="0"/>
+      <c r="AAA1" s="0"/>
+      <c r="AAB1" s="0"/>
+      <c r="AAC1" s="0"/>
+      <c r="AAD1" s="0"/>
+      <c r="AAE1" s="0"/>
+      <c r="AAF1" s="0"/>
+      <c r="AAG1" s="0"/>
+      <c r="AAH1" s="0"/>
+      <c r="AAI1" s="0"/>
+      <c r="AAJ1" s="0"/>
+      <c r="AAK1" s="0"/>
+      <c r="AAL1" s="0"/>
+      <c r="AAM1" s="0"/>
+      <c r="AAN1" s="0"/>
+      <c r="AAO1" s="0"/>
+      <c r="AAP1" s="0"/>
+      <c r="AAQ1" s="0"/>
+      <c r="AAR1" s="0"/>
+      <c r="AAS1" s="0"/>
+      <c r="AAT1" s="0"/>
+      <c r="AAU1" s="0"/>
+      <c r="AAV1" s="0"/>
+      <c r="AAW1" s="0"/>
+      <c r="AAX1" s="0"/>
+      <c r="AAY1" s="0"/>
+      <c r="AAZ1" s="0"/>
+      <c r="ABA1" s="0"/>
+      <c r="ABB1" s="0"/>
+      <c r="ABC1" s="0"/>
+      <c r="ABD1" s="0"/>
+      <c r="ABE1" s="0"/>
+      <c r="ABF1" s="0"/>
+      <c r="ABG1" s="0"/>
+      <c r="ABH1" s="0"/>
+      <c r="ABI1" s="0"/>
+      <c r="ABJ1" s="0"/>
+      <c r="ABK1" s="0"/>
+      <c r="ABL1" s="0"/>
+      <c r="ABM1" s="0"/>
+      <c r="ABN1" s="0"/>
+      <c r="ABO1" s="0"/>
+      <c r="ABP1" s="0"/>
+      <c r="ABQ1" s="0"/>
+      <c r="ABR1" s="0"/>
+      <c r="ABS1" s="0"/>
+      <c r="ABT1" s="0"/>
+      <c r="ABU1" s="0"/>
+      <c r="ABV1" s="0"/>
+      <c r="ABW1" s="0"/>
+      <c r="ABX1" s="0"/>
+      <c r="ABY1" s="0"/>
+      <c r="ABZ1" s="0"/>
+      <c r="ACA1" s="0"/>
+      <c r="ACB1" s="0"/>
+      <c r="ACC1" s="0"/>
+      <c r="ACD1" s="0"/>
+      <c r="ACE1" s="0"/>
+      <c r="ACF1" s="0"/>
+      <c r="ACG1" s="0"/>
+      <c r="ACH1" s="0"/>
+      <c r="ACI1" s="0"/>
+      <c r="ACJ1" s="0"/>
+      <c r="ACK1" s="0"/>
+      <c r="ACL1" s="0"/>
+      <c r="ACM1" s="0"/>
+      <c r="ACN1" s="0"/>
+      <c r="ACO1" s="0"/>
+      <c r="ACP1" s="0"/>
+      <c r="ACQ1" s="0"/>
+      <c r="ACR1" s="0"/>
+      <c r="ACS1" s="0"/>
+      <c r="ACT1" s="0"/>
+      <c r="ACU1" s="0"/>
+      <c r="ACV1" s="0"/>
+      <c r="ACW1" s="0"/>
+      <c r="ACX1" s="0"/>
+      <c r="ACY1" s="0"/>
+      <c r="ACZ1" s="0"/>
+      <c r="ADA1" s="0"/>
+      <c r="ADB1" s="0"/>
+      <c r="ADC1" s="0"/>
+      <c r="ADD1" s="0"/>
+      <c r="ADE1" s="0"/>
+      <c r="ADF1" s="0"/>
+      <c r="ADG1" s="0"/>
+      <c r="ADH1" s="0"/>
+      <c r="ADI1" s="0"/>
+      <c r="ADJ1" s="0"/>
+      <c r="ADK1" s="0"/>
+      <c r="ADL1" s="0"/>
+      <c r="ADM1" s="0"/>
+      <c r="ADN1" s="0"/>
+      <c r="ADO1" s="0"/>
+      <c r="ADP1" s="0"/>
+      <c r="ADQ1" s="0"/>
+      <c r="ADR1" s="0"/>
+      <c r="ADS1" s="0"/>
+      <c r="ADT1" s="0"/>
+      <c r="ADU1" s="0"/>
+      <c r="ADV1" s="0"/>
+      <c r="ADW1" s="0"/>
+      <c r="ADX1" s="0"/>
+      <c r="ADY1" s="0"/>
+      <c r="ADZ1" s="0"/>
+      <c r="AEA1" s="0"/>
+      <c r="AEB1" s="0"/>
+      <c r="AEC1" s="0"/>
+      <c r="AED1" s="0"/>
+      <c r="AEE1" s="0"/>
+      <c r="AEF1" s="0"/>
+      <c r="AEG1" s="0"/>
+      <c r="AEH1" s="0"/>
+      <c r="AEI1" s="0"/>
+      <c r="AEJ1" s="0"/>
+      <c r="AEK1" s="0"/>
+      <c r="AEL1" s="0"/>
+      <c r="AEM1" s="0"/>
+      <c r="AEN1" s="0"/>
+      <c r="AEO1" s="0"/>
+      <c r="AEP1" s="0"/>
+      <c r="AEQ1" s="0"/>
+      <c r="AER1" s="0"/>
+      <c r="AES1" s="0"/>
+      <c r="AET1" s="0"/>
+      <c r="AEU1" s="0"/>
+      <c r="AEV1" s="0"/>
+      <c r="AEW1" s="0"/>
+      <c r="AEX1" s="0"/>
+      <c r="AEY1" s="0"/>
+      <c r="AEZ1" s="0"/>
+      <c r="AFA1" s="0"/>
+      <c r="AFB1" s="0"/>
+      <c r="AFC1" s="0"/>
+      <c r="AFD1" s="0"/>
+      <c r="AFE1" s="0"/>
+      <c r="AFF1" s="0"/>
+      <c r="AFG1" s="0"/>
+      <c r="AFH1" s="0"/>
+      <c r="AFI1" s="0"/>
+      <c r="AFJ1" s="0"/>
+      <c r="AFK1" s="0"/>
+      <c r="AFL1" s="0"/>
+      <c r="AFM1" s="0"/>
+      <c r="AFN1" s="0"/>
+      <c r="AFO1" s="0"/>
+      <c r="AFP1" s="0"/>
+      <c r="AFQ1" s="0"/>
+      <c r="AFR1" s="0"/>
+      <c r="AFS1" s="0"/>
+      <c r="AFT1" s="0"/>
+      <c r="AFU1" s="0"/>
+      <c r="AFV1" s="0"/>
+      <c r="AFW1" s="0"/>
+      <c r="AFX1" s="0"/>
+      <c r="AFY1" s="0"/>
+      <c r="AFZ1" s="0"/>
+      <c r="AGA1" s="0"/>
+      <c r="AGB1" s="0"/>
+      <c r="AGC1" s="0"/>
+      <c r="AGD1" s="0"/>
+      <c r="AGE1" s="0"/>
+      <c r="AGF1" s="0"/>
+      <c r="AGG1" s="0"/>
+      <c r="AGH1" s="0"/>
+      <c r="AGI1" s="0"/>
+      <c r="AGJ1" s="0"/>
+      <c r="AGK1" s="0"/>
+      <c r="AGL1" s="0"/>
+      <c r="AGM1" s="0"/>
+      <c r="AGN1" s="0"/>
+      <c r="AGO1" s="0"/>
+      <c r="AGP1" s="0"/>
+      <c r="AGQ1" s="0"/>
+      <c r="AGR1" s="0"/>
+      <c r="AGS1" s="0"/>
+      <c r="AGT1" s="0"/>
+      <c r="AGU1" s="0"/>
+      <c r="AGV1" s="0"/>
+      <c r="AGW1" s="0"/>
+      <c r="AGX1" s="0"/>
+      <c r="AGY1" s="0"/>
+      <c r="AGZ1" s="0"/>
+      <c r="AHA1" s="0"/>
+      <c r="AHB1" s="0"/>
+      <c r="AHC1" s="0"/>
+      <c r="AHD1" s="0"/>
+      <c r="AHE1" s="0"/>
+      <c r="AHF1" s="0"/>
+      <c r="AHG1" s="0"/>
+      <c r="AHH1" s="0"/>
+      <c r="AHI1" s="0"/>
+      <c r="AHJ1" s="0"/>
+      <c r="AHK1" s="0"/>
+      <c r="AHL1" s="0"/>
+      <c r="AHM1" s="0"/>
+      <c r="AHN1" s="0"/>
+      <c r="AHO1" s="0"/>
+      <c r="AHP1" s="0"/>
+      <c r="AHQ1" s="0"/>
+      <c r="AHR1" s="0"/>
+      <c r="AHS1" s="0"/>
+      <c r="AHT1" s="0"/>
+      <c r="AHU1" s="0"/>
+      <c r="AHV1" s="0"/>
+      <c r="AHW1" s="0"/>
+      <c r="AHX1" s="0"/>
+      <c r="AHY1" s="0"/>
+      <c r="AHZ1" s="0"/>
+      <c r="AIA1" s="0"/>
+      <c r="AIB1" s="0"/>
+      <c r="AIC1" s="0"/>
+      <c r="AID1" s="0"/>
+      <c r="AIE1" s="0"/>
+      <c r="AIF1" s="0"/>
+      <c r="AIG1" s="0"/>
+      <c r="AIH1" s="0"/>
+      <c r="AII1" s="0"/>
+      <c r="AIJ1" s="0"/>
+      <c r="AIK1" s="0"/>
+      <c r="AIL1" s="0"/>
+      <c r="AIM1" s="0"/>
+      <c r="AIN1" s="0"/>
+      <c r="AIO1" s="0"/>
+      <c r="AIP1" s="0"/>
+      <c r="AIQ1" s="0"/>
+      <c r="AIR1" s="0"/>
+      <c r="AIS1" s="0"/>
+      <c r="AIT1" s="0"/>
+      <c r="AIU1" s="0"/>
+      <c r="AIV1" s="0"/>
+      <c r="AIW1" s="0"/>
+      <c r="AIX1" s="0"/>
+      <c r="AIY1" s="0"/>
+      <c r="AIZ1" s="0"/>
+      <c r="AJA1" s="0"/>
+      <c r="AJB1" s="0"/>
+      <c r="AJC1" s="0"/>
+      <c r="AJD1" s="0"/>
+      <c r="AJE1" s="0"/>
+      <c r="AJF1" s="0"/>
+      <c r="AJG1" s="0"/>
+      <c r="AJH1" s="0"/>
+      <c r="AJI1" s="0"/>
+      <c r="AJJ1" s="0"/>
+      <c r="AJK1" s="0"/>
+      <c r="AJL1" s="0"/>
+      <c r="AJM1" s="0"/>
+      <c r="AJN1" s="0"/>
+      <c r="AJO1" s="0"/>
+      <c r="AJP1" s="0"/>
+      <c r="AJQ1" s="0"/>
+      <c r="AJR1" s="0"/>
+      <c r="AJS1" s="0"/>
+      <c r="AJT1" s="0"/>
+      <c r="AJU1" s="0"/>
+      <c r="AJV1" s="0"/>
+      <c r="AJW1" s="0"/>
+      <c r="AJX1" s="0"/>
+      <c r="AJY1" s="0"/>
+      <c r="AJZ1" s="0"/>
+      <c r="AKA1" s="0"/>
+      <c r="AKB1" s="0"/>
+      <c r="AKC1" s="0"/>
+      <c r="AKD1" s="0"/>
+      <c r="AKE1" s="0"/>
+      <c r="AKF1" s="0"/>
+      <c r="AKG1" s="0"/>
+      <c r="AKH1" s="0"/>
+      <c r="AKI1" s="0"/>
+      <c r="AKJ1" s="0"/>
+      <c r="AKK1" s="0"/>
+      <c r="AKL1" s="0"/>
+      <c r="AKM1" s="0"/>
+      <c r="AKN1" s="0"/>
+      <c r="AKO1" s="0"/>
+      <c r="AKP1" s="0"/>
+      <c r="AKQ1" s="0"/>
+      <c r="AKR1" s="0"/>
+      <c r="AKS1" s="0"/>
+      <c r="AKT1" s="0"/>
+      <c r="AKU1" s="0"/>
+      <c r="AKV1" s="0"/>
+      <c r="AKW1" s="0"/>
+      <c r="AKX1" s="0"/>
+      <c r="AKY1" s="0"/>
+      <c r="AKZ1" s="0"/>
+      <c r="ALA1" s="0"/>
+      <c r="ALB1" s="0"/>
+      <c r="ALC1" s="0"/>
+      <c r="ALD1" s="0"/>
+      <c r="ALE1" s="0"/>
+      <c r="ALF1" s="0"/>
+      <c r="ALG1" s="0"/>
+      <c r="ALH1" s="0"/>
+      <c r="ALI1" s="0"/>
+      <c r="ALJ1" s="0"/>
+      <c r="ALK1" s="0"/>
+      <c r="ALL1" s="0"/>
+      <c r="ALM1" s="0"/>
+      <c r="ALN1" s="0"/>
+      <c r="ALO1" s="0"/>
+      <c r="ALP1" s="0"/>
+      <c r="ALQ1" s="0"/>
+      <c r="ALR1" s="0"/>
+      <c r="ALS1" s="0"/>
+      <c r="ALT1" s="0"/>
+      <c r="ALU1" s="0"/>
+      <c r="ALV1" s="0"/>
+      <c r="ALW1" s="0"/>
+      <c r="ALX1" s="0"/>
+      <c r="ALY1" s="0"/>
+      <c r="ALZ1" s="0"/>
+      <c r="AMA1" s="0"/>
+      <c r="AMB1" s="0"/>
+      <c r="AMC1" s="0"/>
+      <c r="AMD1" s="0"/>
+      <c r="AME1" s="0"/>
+      <c r="AMF1" s="0"/>
+      <c r="AMG1" s="0"/>
+      <c r="AMH1" s="0"/>
+      <c r="AMI1" s="0"/>
+      <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="36.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="65" t="s">
@@ -16727,271 +17628,3172 @@
       <c r="I2" s="71" t="s">
         <v>38</v>
       </c>
+      <c r="J2" s="0"/>
+      <c r="K2" s="0"/>
+      <c r="L2" s="0"/>
+      <c r="M2" s="0"/>
+      <c r="N2" s="0"/>
+      <c r="O2" s="0"/>
+      <c r="P2" s="0"/>
+      <c r="Q2" s="0"/>
+      <c r="R2" s="0"/>
+      <c r="S2" s="0"/>
+      <c r="T2" s="0"/>
+      <c r="U2" s="0"/>
+      <c r="V2" s="0"/>
+      <c r="W2" s="0"/>
+      <c r="X2" s="0"/>
+      <c r="Y2" s="0"/>
+      <c r="Z2" s="0"/>
+      <c r="AA2" s="0"/>
+      <c r="AB2" s="0"/>
+      <c r="AC2" s="0"/>
+      <c r="AD2" s="0"/>
+      <c r="AE2" s="0"/>
+      <c r="AF2" s="0"/>
+      <c r="AG2" s="0"/>
+      <c r="AH2" s="0"/>
+      <c r="AI2" s="0"/>
+      <c r="AJ2" s="0"/>
+      <c r="AK2" s="0"/>
+      <c r="AL2" s="0"/>
+      <c r="AM2" s="0"/>
+      <c r="AN2" s="0"/>
+      <c r="AO2" s="0"/>
+      <c r="AP2" s="0"/>
+      <c r="AQ2" s="0"/>
+      <c r="AR2" s="0"/>
+      <c r="AS2" s="0"/>
+      <c r="AT2" s="0"/>
+      <c r="AU2" s="0"/>
+      <c r="AV2" s="0"/>
+      <c r="AW2" s="0"/>
+      <c r="AX2" s="0"/>
+      <c r="AY2" s="0"/>
+      <c r="AZ2" s="0"/>
+      <c r="BA2" s="0"/>
+      <c r="BB2" s="0"/>
+      <c r="BC2" s="0"/>
+      <c r="BD2" s="0"/>
+      <c r="BE2" s="0"/>
+      <c r="BF2" s="0"/>
+      <c r="BG2" s="0"/>
+      <c r="BH2" s="0"/>
+      <c r="BI2" s="0"/>
+      <c r="BJ2" s="0"/>
+      <c r="BK2" s="0"/>
+      <c r="BL2" s="0"/>
+      <c r="BM2" s="0"/>
+      <c r="BN2" s="0"/>
+      <c r="BO2" s="0"/>
+      <c r="BP2" s="0"/>
+      <c r="BQ2" s="0"/>
+      <c r="BR2" s="0"/>
+      <c r="BS2" s="0"/>
+      <c r="BT2" s="0"/>
+      <c r="BU2" s="0"/>
+      <c r="BV2" s="0"/>
+      <c r="BW2" s="0"/>
+      <c r="BX2" s="0"/>
+      <c r="BY2" s="0"/>
+      <c r="BZ2" s="0"/>
+      <c r="CA2" s="0"/>
+      <c r="CB2" s="0"/>
+      <c r="CC2" s="0"/>
+      <c r="CD2" s="0"/>
+      <c r="CE2" s="0"/>
+      <c r="CF2" s="0"/>
+      <c r="CG2" s="0"/>
+      <c r="CH2" s="0"/>
+      <c r="CI2" s="0"/>
+      <c r="CJ2" s="0"/>
+      <c r="CK2" s="0"/>
+      <c r="CL2" s="0"/>
+      <c r="CM2" s="0"/>
+      <c r="CN2" s="0"/>
+      <c r="CO2" s="0"/>
+      <c r="CP2" s="0"/>
+      <c r="CQ2" s="0"/>
+      <c r="CR2" s="0"/>
+      <c r="CS2" s="0"/>
+      <c r="CT2" s="0"/>
+      <c r="CU2" s="0"/>
+      <c r="CV2" s="0"/>
+      <c r="CW2" s="0"/>
+      <c r="CX2" s="0"/>
+      <c r="CY2" s="0"/>
+      <c r="CZ2" s="0"/>
+      <c r="DA2" s="0"/>
+      <c r="DB2" s="0"/>
+      <c r="DC2" s="0"/>
+      <c r="DD2" s="0"/>
+      <c r="DE2" s="0"/>
+      <c r="DF2" s="0"/>
+      <c r="DG2" s="0"/>
+      <c r="DH2" s="0"/>
+      <c r="DI2" s="0"/>
+      <c r="DJ2" s="0"/>
+      <c r="DK2" s="0"/>
+      <c r="DL2" s="0"/>
+      <c r="DM2" s="0"/>
+      <c r="DN2" s="0"/>
+      <c r="DO2" s="0"/>
+      <c r="DP2" s="0"/>
+      <c r="DQ2" s="0"/>
+      <c r="DR2" s="0"/>
+      <c r="DS2" s="0"/>
+      <c r="DT2" s="0"/>
+      <c r="DU2" s="0"/>
+      <c r="DV2" s="0"/>
+      <c r="DW2" s="0"/>
+      <c r="DX2" s="0"/>
+      <c r="DY2" s="0"/>
+      <c r="DZ2" s="0"/>
+      <c r="EA2" s="0"/>
+      <c r="EB2" s="0"/>
+      <c r="EC2" s="0"/>
+      <c r="ED2" s="0"/>
+      <c r="EE2" s="0"/>
+      <c r="EF2" s="0"/>
+      <c r="EG2" s="0"/>
+      <c r="EH2" s="0"/>
+      <c r="EI2" s="0"/>
+      <c r="EJ2" s="0"/>
+      <c r="EK2" s="0"/>
+      <c r="EL2" s="0"/>
+      <c r="EM2" s="0"/>
+      <c r="EN2" s="0"/>
+      <c r="EO2" s="0"/>
+      <c r="EP2" s="0"/>
+      <c r="EQ2" s="0"/>
+      <c r="ER2" s="0"/>
+      <c r="ES2" s="0"/>
+      <c r="ET2" s="0"/>
+      <c r="EU2" s="0"/>
+      <c r="EV2" s="0"/>
+      <c r="EW2" s="0"/>
+      <c r="EX2" s="0"/>
+      <c r="EY2" s="0"/>
+      <c r="EZ2" s="0"/>
+      <c r="FA2" s="0"/>
+      <c r="FB2" s="0"/>
+      <c r="FC2" s="0"/>
+      <c r="FD2" s="0"/>
+      <c r="FE2" s="0"/>
+      <c r="FF2" s="0"/>
+      <c r="FG2" s="0"/>
+      <c r="FH2" s="0"/>
+      <c r="FI2" s="0"/>
+      <c r="FJ2" s="0"/>
+      <c r="FK2" s="0"/>
+      <c r="FL2" s="0"/>
+      <c r="FM2" s="0"/>
+      <c r="FN2" s="0"/>
+      <c r="FO2" s="0"/>
+      <c r="FP2" s="0"/>
+      <c r="FQ2" s="0"/>
+      <c r="FR2" s="0"/>
+      <c r="FS2" s="0"/>
+      <c r="FT2" s="0"/>
+      <c r="FU2" s="0"/>
+      <c r="FV2" s="0"/>
+      <c r="FW2" s="0"/>
+      <c r="FX2" s="0"/>
+      <c r="FY2" s="0"/>
+      <c r="FZ2" s="0"/>
+      <c r="GA2" s="0"/>
+      <c r="GB2" s="0"/>
+      <c r="GC2" s="0"/>
+      <c r="GD2" s="0"/>
+      <c r="GE2" s="0"/>
+      <c r="GF2" s="0"/>
+      <c r="GG2" s="0"/>
+      <c r="GH2" s="0"/>
+      <c r="GI2" s="0"/>
+      <c r="GJ2" s="0"/>
+      <c r="GK2" s="0"/>
+      <c r="GL2" s="0"/>
+      <c r="GM2" s="0"/>
+      <c r="GN2" s="0"/>
+      <c r="GO2" s="0"/>
+      <c r="GP2" s="0"/>
+      <c r="GQ2" s="0"/>
+      <c r="GR2" s="0"/>
+      <c r="GS2" s="0"/>
+      <c r="GT2" s="0"/>
+      <c r="GU2" s="0"/>
+      <c r="GV2" s="0"/>
+      <c r="GW2" s="0"/>
+      <c r="GX2" s="0"/>
+      <c r="GY2" s="0"/>
+      <c r="GZ2" s="0"/>
+      <c r="HA2" s="0"/>
+      <c r="HB2" s="0"/>
+      <c r="HC2" s="0"/>
+      <c r="HD2" s="0"/>
+      <c r="HE2" s="0"/>
+      <c r="HF2" s="0"/>
+      <c r="HG2" s="0"/>
+      <c r="HH2" s="0"/>
+      <c r="HI2" s="0"/>
+      <c r="HJ2" s="0"/>
+      <c r="HK2" s="0"/>
+      <c r="HL2" s="0"/>
+      <c r="HM2" s="0"/>
+      <c r="HN2" s="0"/>
+      <c r="HO2" s="0"/>
+      <c r="HP2" s="0"/>
+      <c r="HQ2" s="0"/>
+      <c r="HR2" s="0"/>
+      <c r="HS2" s="0"/>
+      <c r="HT2" s="0"/>
+      <c r="HU2" s="0"/>
+      <c r="HV2" s="0"/>
+      <c r="HW2" s="0"/>
+      <c r="HX2" s="0"/>
+      <c r="HY2" s="0"/>
+      <c r="HZ2" s="0"/>
+      <c r="IA2" s="0"/>
+      <c r="IB2" s="0"/>
+      <c r="IC2" s="0"/>
+      <c r="ID2" s="0"/>
+      <c r="IE2" s="0"/>
+      <c r="IF2" s="0"/>
+      <c r="IG2" s="0"/>
+      <c r="IH2" s="0"/>
+      <c r="II2" s="0"/>
+      <c r="IJ2" s="0"/>
+      <c r="IK2" s="0"/>
+      <c r="IL2" s="0"/>
+      <c r="IM2" s="0"/>
+      <c r="IN2" s="0"/>
+      <c r="IO2" s="0"/>
+      <c r="IP2" s="0"/>
+      <c r="IQ2" s="0"/>
+      <c r="IR2" s="0"/>
+      <c r="IS2" s="0"/>
+      <c r="IT2" s="0"/>
+      <c r="IU2" s="0"/>
+      <c r="IV2" s="0"/>
+      <c r="IW2" s="0"/>
+      <c r="IX2" s="0"/>
+      <c r="IY2" s="0"/>
+      <c r="IZ2" s="0"/>
+      <c r="JA2" s="0"/>
+      <c r="JB2" s="0"/>
+      <c r="JC2" s="0"/>
+      <c r="JD2" s="0"/>
+      <c r="JE2" s="0"/>
+      <c r="JF2" s="0"/>
+      <c r="JG2" s="0"/>
+      <c r="JH2" s="0"/>
+      <c r="JI2" s="0"/>
+      <c r="JJ2" s="0"/>
+      <c r="JK2" s="0"/>
+      <c r="JL2" s="0"/>
+      <c r="JM2" s="0"/>
+      <c r="JN2" s="0"/>
+      <c r="JO2" s="0"/>
+      <c r="JP2" s="0"/>
+      <c r="JQ2" s="0"/>
+      <c r="JR2" s="0"/>
+      <c r="JS2" s="0"/>
+      <c r="JT2" s="0"/>
+      <c r="JU2" s="0"/>
+      <c r="JV2" s="0"/>
+      <c r="JW2" s="0"/>
+      <c r="JX2" s="0"/>
+      <c r="JY2" s="0"/>
+      <c r="JZ2" s="0"/>
+      <c r="KA2" s="0"/>
+      <c r="KB2" s="0"/>
+      <c r="KC2" s="0"/>
+      <c r="KD2" s="0"/>
+      <c r="KE2" s="0"/>
+      <c r="KF2" s="0"/>
+      <c r="KG2" s="0"/>
+      <c r="KH2" s="0"/>
+      <c r="KI2" s="0"/>
+      <c r="KJ2" s="0"/>
+      <c r="KK2" s="0"/>
+      <c r="KL2" s="0"/>
+      <c r="KM2" s="0"/>
+      <c r="KN2" s="0"/>
+      <c r="KO2" s="0"/>
+      <c r="KP2" s="0"/>
+      <c r="KQ2" s="0"/>
+      <c r="KR2" s="0"/>
+      <c r="KS2" s="0"/>
+      <c r="KT2" s="0"/>
+      <c r="KU2" s="0"/>
+      <c r="KV2" s="0"/>
+      <c r="KW2" s="0"/>
+      <c r="KX2" s="0"/>
+      <c r="KY2" s="0"/>
+      <c r="KZ2" s="0"/>
+      <c r="LA2" s="0"/>
+      <c r="LB2" s="0"/>
+      <c r="LC2" s="0"/>
+      <c r="LD2" s="0"/>
+      <c r="LE2" s="0"/>
+      <c r="LF2" s="0"/>
+      <c r="LG2" s="0"/>
+      <c r="LH2" s="0"/>
+      <c r="LI2" s="0"/>
+      <c r="LJ2" s="0"/>
+      <c r="LK2" s="0"/>
+      <c r="LL2" s="0"/>
+      <c r="LM2" s="0"/>
+      <c r="LN2" s="0"/>
+      <c r="LO2" s="0"/>
+      <c r="LP2" s="0"/>
+      <c r="LQ2" s="0"/>
+      <c r="LR2" s="0"/>
+      <c r="LS2" s="0"/>
+      <c r="LT2" s="0"/>
+      <c r="LU2" s="0"/>
+      <c r="LV2" s="0"/>
+      <c r="LW2" s="0"/>
+      <c r="LX2" s="0"/>
+      <c r="LY2" s="0"/>
+      <c r="LZ2" s="0"/>
+      <c r="MA2" s="0"/>
+      <c r="MB2" s="0"/>
+      <c r="MC2" s="0"/>
+      <c r="MD2" s="0"/>
+      <c r="ME2" s="0"/>
+      <c r="MF2" s="0"/>
+      <c r="MG2" s="0"/>
+      <c r="MH2" s="0"/>
+      <c r="MI2" s="0"/>
+      <c r="MJ2" s="0"/>
+      <c r="MK2" s="0"/>
+      <c r="ML2" s="0"/>
+      <c r="MM2" s="0"/>
+      <c r="MN2" s="0"/>
+      <c r="MO2" s="0"/>
+      <c r="MP2" s="0"/>
+      <c r="MQ2" s="0"/>
+      <c r="MR2" s="0"/>
+      <c r="MS2" s="0"/>
+      <c r="MT2" s="0"/>
+      <c r="MU2" s="0"/>
+      <c r="MV2" s="0"/>
+      <c r="MW2" s="0"/>
+      <c r="MX2" s="0"/>
+      <c r="MY2" s="0"/>
+      <c r="MZ2" s="0"/>
+      <c r="NA2" s="0"/>
+      <c r="NB2" s="0"/>
+      <c r="NC2" s="0"/>
+      <c r="ND2" s="0"/>
+      <c r="NE2" s="0"/>
+      <c r="NF2" s="0"/>
+      <c r="NG2" s="0"/>
+      <c r="NH2" s="0"/>
+      <c r="NI2" s="0"/>
+      <c r="NJ2" s="0"/>
+      <c r="NK2" s="0"/>
+      <c r="NL2" s="0"/>
+      <c r="NM2" s="0"/>
+      <c r="NN2" s="0"/>
+      <c r="NO2" s="0"/>
+      <c r="NP2" s="0"/>
+      <c r="NQ2" s="0"/>
+      <c r="NR2" s="0"/>
+      <c r="NS2" s="0"/>
+      <c r="NT2" s="0"/>
+      <c r="NU2" s="0"/>
+      <c r="NV2" s="0"/>
+      <c r="NW2" s="0"/>
+      <c r="NX2" s="0"/>
+      <c r="NY2" s="0"/>
+      <c r="NZ2" s="0"/>
+      <c r="OA2" s="0"/>
+      <c r="OB2" s="0"/>
+      <c r="OC2" s="0"/>
+      <c r="OD2" s="0"/>
+      <c r="OE2" s="0"/>
+      <c r="OF2" s="0"/>
+      <c r="OG2" s="0"/>
+      <c r="OH2" s="0"/>
+      <c r="OI2" s="0"/>
+      <c r="OJ2" s="0"/>
+      <c r="OK2" s="0"/>
+      <c r="OL2" s="0"/>
+      <c r="OM2" s="0"/>
+      <c r="ON2" s="0"/>
+      <c r="OO2" s="0"/>
+      <c r="OP2" s="0"/>
+      <c r="OQ2" s="0"/>
+      <c r="OR2" s="0"/>
+      <c r="OS2" s="0"/>
+      <c r="OT2" s="0"/>
+      <c r="OU2" s="0"/>
+      <c r="OV2" s="0"/>
+      <c r="OW2" s="0"/>
+      <c r="OX2" s="0"/>
+      <c r="OY2" s="0"/>
+      <c r="OZ2" s="0"/>
+      <c r="PA2" s="0"/>
+      <c r="PB2" s="0"/>
+      <c r="PC2" s="0"/>
+      <c r="PD2" s="0"/>
+      <c r="PE2" s="0"/>
+      <c r="PF2" s="0"/>
+      <c r="PG2" s="0"/>
+      <c r="PH2" s="0"/>
+      <c r="PI2" s="0"/>
+      <c r="PJ2" s="0"/>
+      <c r="PK2" s="0"/>
+      <c r="PL2" s="0"/>
+      <c r="PM2" s="0"/>
+      <c r="PN2" s="0"/>
+      <c r="PO2" s="0"/>
+      <c r="PP2" s="0"/>
+      <c r="PQ2" s="0"/>
+      <c r="PR2" s="0"/>
+      <c r="PS2" s="0"/>
+      <c r="PT2" s="0"/>
+      <c r="PU2" s="0"/>
+      <c r="PV2" s="0"/>
+      <c r="PW2" s="0"/>
+      <c r="PX2" s="0"/>
+      <c r="PY2" s="0"/>
+      <c r="PZ2" s="0"/>
+      <c r="QA2" s="0"/>
+      <c r="QB2" s="0"/>
+      <c r="QC2" s="0"/>
+      <c r="QD2" s="0"/>
+      <c r="QE2" s="0"/>
+      <c r="QF2" s="0"/>
+      <c r="QG2" s="0"/>
+      <c r="QH2" s="0"/>
+      <c r="QI2" s="0"/>
+      <c r="QJ2" s="0"/>
+      <c r="QK2" s="0"/>
+      <c r="QL2" s="0"/>
+      <c r="QM2" s="0"/>
+      <c r="QN2" s="0"/>
+      <c r="QO2" s="0"/>
+      <c r="QP2" s="0"/>
+      <c r="QQ2" s="0"/>
+      <c r="QR2" s="0"/>
+      <c r="QS2" s="0"/>
+      <c r="QT2" s="0"/>
+      <c r="QU2" s="0"/>
+      <c r="QV2" s="0"/>
+      <c r="QW2" s="0"/>
+      <c r="QX2" s="0"/>
+      <c r="QY2" s="0"/>
+      <c r="QZ2" s="0"/>
+      <c r="RA2" s="0"/>
+      <c r="RB2" s="0"/>
+      <c r="RC2" s="0"/>
+      <c r="RD2" s="0"/>
+      <c r="RE2" s="0"/>
+      <c r="RF2" s="0"/>
+      <c r="RG2" s="0"/>
+      <c r="RH2" s="0"/>
+      <c r="RI2" s="0"/>
+      <c r="RJ2" s="0"/>
+      <c r="RK2" s="0"/>
+      <c r="RL2" s="0"/>
+      <c r="RM2" s="0"/>
+      <c r="RN2" s="0"/>
+      <c r="RO2" s="0"/>
+      <c r="RP2" s="0"/>
+      <c r="RQ2" s="0"/>
+      <c r="RR2" s="0"/>
+      <c r="RS2" s="0"/>
+      <c r="RT2" s="0"/>
+      <c r="RU2" s="0"/>
+      <c r="RV2" s="0"/>
+      <c r="RW2" s="0"/>
+      <c r="RX2" s="0"/>
+      <c r="RY2" s="0"/>
+      <c r="RZ2" s="0"/>
+      <c r="SA2" s="0"/>
+      <c r="SB2" s="0"/>
+      <c r="SC2" s="0"/>
+      <c r="SD2" s="0"/>
+      <c r="SE2" s="0"/>
+      <c r="SF2" s="0"/>
+      <c r="SG2" s="0"/>
+      <c r="SH2" s="0"/>
+      <c r="SI2" s="0"/>
+      <c r="SJ2" s="0"/>
+      <c r="SK2" s="0"/>
+      <c r="SL2" s="0"/>
+      <c r="SM2" s="0"/>
+      <c r="SN2" s="0"/>
+      <c r="SO2" s="0"/>
+      <c r="SP2" s="0"/>
+      <c r="SQ2" s="0"/>
+      <c r="SR2" s="0"/>
+      <c r="SS2" s="0"/>
+      <c r="ST2" s="0"/>
+      <c r="SU2" s="0"/>
+      <c r="SV2" s="0"/>
+      <c r="SW2" s="0"/>
+      <c r="SX2" s="0"/>
+      <c r="SY2" s="0"/>
+      <c r="SZ2" s="0"/>
+      <c r="TA2" s="0"/>
+      <c r="TB2" s="0"/>
+      <c r="TC2" s="0"/>
+      <c r="TD2" s="0"/>
+      <c r="TE2" s="0"/>
+      <c r="TF2" s="0"/>
+      <c r="TG2" s="0"/>
+      <c r="TH2" s="0"/>
+      <c r="TI2" s="0"/>
+      <c r="TJ2" s="0"/>
+      <c r="TK2" s="0"/>
+      <c r="TL2" s="0"/>
+      <c r="TM2" s="0"/>
+      <c r="TN2" s="0"/>
+      <c r="TO2" s="0"/>
+      <c r="TP2" s="0"/>
+      <c r="TQ2" s="0"/>
+      <c r="TR2" s="0"/>
+      <c r="TS2" s="0"/>
+      <c r="TT2" s="0"/>
+      <c r="TU2" s="0"/>
+      <c r="TV2" s="0"/>
+      <c r="TW2" s="0"/>
+      <c r="TX2" s="0"/>
+      <c r="TY2" s="0"/>
+      <c r="TZ2" s="0"/>
+      <c r="UA2" s="0"/>
+      <c r="UB2" s="0"/>
+      <c r="UC2" s="0"/>
+      <c r="UD2" s="0"/>
+      <c r="UE2" s="0"/>
+      <c r="UF2" s="0"/>
+      <c r="UG2" s="0"/>
+      <c r="UH2" s="0"/>
+      <c r="UI2" s="0"/>
+      <c r="UJ2" s="0"/>
+      <c r="UK2" s="0"/>
+      <c r="UL2" s="0"/>
+      <c r="UM2" s="0"/>
+      <c r="UN2" s="0"/>
+      <c r="UO2" s="0"/>
+      <c r="UP2" s="0"/>
+      <c r="UQ2" s="0"/>
+      <c r="UR2" s="0"/>
+      <c r="US2" s="0"/>
+      <c r="UT2" s="0"/>
+      <c r="UU2" s="0"/>
+      <c r="UV2" s="0"/>
+      <c r="UW2" s="0"/>
+      <c r="UX2" s="0"/>
+      <c r="UY2" s="0"/>
+      <c r="UZ2" s="0"/>
+      <c r="VA2" s="0"/>
+      <c r="VB2" s="0"/>
+      <c r="VC2" s="0"/>
+      <c r="VD2" s="0"/>
+      <c r="VE2" s="0"/>
+      <c r="VF2" s="0"/>
+      <c r="VG2" s="0"/>
+      <c r="VH2" s="0"/>
+      <c r="VI2" s="0"/>
+      <c r="VJ2" s="0"/>
+      <c r="VK2" s="0"/>
+      <c r="VL2" s="0"/>
+      <c r="VM2" s="0"/>
+      <c r="VN2" s="0"/>
+      <c r="VO2" s="0"/>
+      <c r="VP2" s="0"/>
+      <c r="VQ2" s="0"/>
+      <c r="VR2" s="0"/>
+      <c r="VS2" s="0"/>
+      <c r="VT2" s="0"/>
+      <c r="VU2" s="0"/>
+      <c r="VV2" s="0"/>
+      <c r="VW2" s="0"/>
+      <c r="VX2" s="0"/>
+      <c r="VY2" s="0"/>
+      <c r="VZ2" s="0"/>
+      <c r="WA2" s="0"/>
+      <c r="WB2" s="0"/>
+      <c r="WC2" s="0"/>
+      <c r="WD2" s="0"/>
+      <c r="WE2" s="0"/>
+      <c r="WF2" s="0"/>
+      <c r="WG2" s="0"/>
+      <c r="WH2" s="0"/>
+      <c r="WI2" s="0"/>
+      <c r="WJ2" s="0"/>
+      <c r="WK2" s="0"/>
+      <c r="WL2" s="0"/>
+      <c r="WM2" s="0"/>
+      <c r="WN2" s="0"/>
+      <c r="WO2" s="0"/>
+      <c r="WP2" s="0"/>
+      <c r="WQ2" s="0"/>
+      <c r="WR2" s="0"/>
+      <c r="WS2" s="0"/>
+      <c r="WT2" s="0"/>
+      <c r="WU2" s="0"/>
+      <c r="WV2" s="0"/>
+      <c r="WW2" s="0"/>
+      <c r="WX2" s="0"/>
+      <c r="WY2" s="0"/>
+      <c r="WZ2" s="0"/>
+      <c r="XA2" s="0"/>
+      <c r="XB2" s="0"/>
+      <c r="XC2" s="0"/>
+      <c r="XD2" s="0"/>
+      <c r="XE2" s="0"/>
+      <c r="XF2" s="0"/>
+      <c r="XG2" s="0"/>
+      <c r="XH2" s="0"/>
+      <c r="XI2" s="0"/>
+      <c r="XJ2" s="0"/>
+      <c r="XK2" s="0"/>
+      <c r="XL2" s="0"/>
+      <c r="XM2" s="0"/>
+      <c r="XN2" s="0"/>
+      <c r="XO2" s="0"/>
+      <c r="XP2" s="0"/>
+      <c r="XQ2" s="0"/>
+      <c r="XR2" s="0"/>
+      <c r="XS2" s="0"/>
+      <c r="XT2" s="0"/>
+      <c r="XU2" s="0"/>
+      <c r="XV2" s="0"/>
+      <c r="XW2" s="0"/>
+      <c r="XX2" s="0"/>
+      <c r="XY2" s="0"/>
+      <c r="XZ2" s="0"/>
+      <c r="YA2" s="0"/>
+      <c r="YB2" s="0"/>
+      <c r="YC2" s="0"/>
+      <c r="YD2" s="0"/>
+      <c r="YE2" s="0"/>
+      <c r="YF2" s="0"/>
+      <c r="YG2" s="0"/>
+      <c r="YH2" s="0"/>
+      <c r="YI2" s="0"/>
+      <c r="YJ2" s="0"/>
+      <c r="YK2" s="0"/>
+      <c r="YL2" s="0"/>
+      <c r="YM2" s="0"/>
+      <c r="YN2" s="0"/>
+      <c r="YO2" s="0"/>
+      <c r="YP2" s="0"/>
+      <c r="YQ2" s="0"/>
+      <c r="YR2" s="0"/>
+      <c r="YS2" s="0"/>
+      <c r="YT2" s="0"/>
+      <c r="YU2" s="0"/>
+      <c r="YV2" s="0"/>
+      <c r="YW2" s="0"/>
+      <c r="YX2" s="0"/>
+      <c r="YY2" s="0"/>
+      <c r="YZ2" s="0"/>
+      <c r="ZA2" s="0"/>
+      <c r="ZB2" s="0"/>
+      <c r="ZC2" s="0"/>
+      <c r="ZD2" s="0"/>
+      <c r="ZE2" s="0"/>
+      <c r="ZF2" s="0"/>
+      <c r="ZG2" s="0"/>
+      <c r="ZH2" s="0"/>
+      <c r="ZI2" s="0"/>
+      <c r="ZJ2" s="0"/>
+      <c r="ZK2" s="0"/>
+      <c r="ZL2" s="0"/>
+      <c r="ZM2" s="0"/>
+      <c r="ZN2" s="0"/>
+      <c r="ZO2" s="0"/>
+      <c r="ZP2" s="0"/>
+      <c r="ZQ2" s="0"/>
+      <c r="ZR2" s="0"/>
+      <c r="ZS2" s="0"/>
+      <c r="ZT2" s="0"/>
+      <c r="ZU2" s="0"/>
+      <c r="ZV2" s="0"/>
+      <c r="ZW2" s="0"/>
+      <c r="ZX2" s="0"/>
+      <c r="ZY2" s="0"/>
+      <c r="ZZ2" s="0"/>
+      <c r="AAA2" s="0"/>
+      <c r="AAB2" s="0"/>
+      <c r="AAC2" s="0"/>
+      <c r="AAD2" s="0"/>
+      <c r="AAE2" s="0"/>
+      <c r="AAF2" s="0"/>
+      <c r="AAG2" s="0"/>
+      <c r="AAH2" s="0"/>
+      <c r="AAI2" s="0"/>
+      <c r="AAJ2" s="0"/>
+      <c r="AAK2" s="0"/>
+      <c r="AAL2" s="0"/>
+      <c r="AAM2" s="0"/>
+      <c r="AAN2" s="0"/>
+      <c r="AAO2" s="0"/>
+      <c r="AAP2" s="0"/>
+      <c r="AAQ2" s="0"/>
+      <c r="AAR2" s="0"/>
+      <c r="AAS2" s="0"/>
+      <c r="AAT2" s="0"/>
+      <c r="AAU2" s="0"/>
+      <c r="AAV2" s="0"/>
+      <c r="AAW2" s="0"/>
+      <c r="AAX2" s="0"/>
+      <c r="AAY2" s="0"/>
+      <c r="AAZ2" s="0"/>
+      <c r="ABA2" s="0"/>
+      <c r="ABB2" s="0"/>
+      <c r="ABC2" s="0"/>
+      <c r="ABD2" s="0"/>
+      <c r="ABE2" s="0"/>
+      <c r="ABF2" s="0"/>
+      <c r="ABG2" s="0"/>
+      <c r="ABH2" s="0"/>
+      <c r="ABI2" s="0"/>
+      <c r="ABJ2" s="0"/>
+      <c r="ABK2" s="0"/>
+      <c r="ABL2" s="0"/>
+      <c r="ABM2" s="0"/>
+      <c r="ABN2" s="0"/>
+      <c r="ABO2" s="0"/>
+      <c r="ABP2" s="0"/>
+      <c r="ABQ2" s="0"/>
+      <c r="ABR2" s="0"/>
+      <c r="ABS2" s="0"/>
+      <c r="ABT2" s="0"/>
+      <c r="ABU2" s="0"/>
+      <c r="ABV2" s="0"/>
+      <c r="ABW2" s="0"/>
+      <c r="ABX2" s="0"/>
+      <c r="ABY2" s="0"/>
+      <c r="ABZ2" s="0"/>
+      <c r="ACA2" s="0"/>
+      <c r="ACB2" s="0"/>
+      <c r="ACC2" s="0"/>
+      <c r="ACD2" s="0"/>
+      <c r="ACE2" s="0"/>
+      <c r="ACF2" s="0"/>
+      <c r="ACG2" s="0"/>
+      <c r="ACH2" s="0"/>
+      <c r="ACI2" s="0"/>
+      <c r="ACJ2" s="0"/>
+      <c r="ACK2" s="0"/>
+      <c r="ACL2" s="0"/>
+      <c r="ACM2" s="0"/>
+      <c r="ACN2" s="0"/>
+      <c r="ACO2" s="0"/>
+      <c r="ACP2" s="0"/>
+      <c r="ACQ2" s="0"/>
+      <c r="ACR2" s="0"/>
+      <c r="ACS2" s="0"/>
+      <c r="ACT2" s="0"/>
+      <c r="ACU2" s="0"/>
+      <c r="ACV2" s="0"/>
+      <c r="ACW2" s="0"/>
+      <c r="ACX2" s="0"/>
+      <c r="ACY2" s="0"/>
+      <c r="ACZ2" s="0"/>
+      <c r="ADA2" s="0"/>
+      <c r="ADB2" s="0"/>
+      <c r="ADC2" s="0"/>
+      <c r="ADD2" s="0"/>
+      <c r="ADE2" s="0"/>
+      <c r="ADF2" s="0"/>
+      <c r="ADG2" s="0"/>
+      <c r="ADH2" s="0"/>
+      <c r="ADI2" s="0"/>
+      <c r="ADJ2" s="0"/>
+      <c r="ADK2" s="0"/>
+      <c r="ADL2" s="0"/>
+      <c r="ADM2" s="0"/>
+      <c r="ADN2" s="0"/>
+      <c r="ADO2" s="0"/>
+      <c r="ADP2" s="0"/>
+      <c r="ADQ2" s="0"/>
+      <c r="ADR2" s="0"/>
+      <c r="ADS2" s="0"/>
+      <c r="ADT2" s="0"/>
+      <c r="ADU2" s="0"/>
+      <c r="ADV2" s="0"/>
+      <c r="ADW2" s="0"/>
+      <c r="ADX2" s="0"/>
+      <c r="ADY2" s="0"/>
+      <c r="ADZ2" s="0"/>
+      <c r="AEA2" s="0"/>
+      <c r="AEB2" s="0"/>
+      <c r="AEC2" s="0"/>
+      <c r="AED2" s="0"/>
+      <c r="AEE2" s="0"/>
+      <c r="AEF2" s="0"/>
+      <c r="AEG2" s="0"/>
+      <c r="AEH2" s="0"/>
+      <c r="AEI2" s="0"/>
+      <c r="AEJ2" s="0"/>
+      <c r="AEK2" s="0"/>
+      <c r="AEL2" s="0"/>
+      <c r="AEM2" s="0"/>
+      <c r="AEN2" s="0"/>
+      <c r="AEO2" s="0"/>
+      <c r="AEP2" s="0"/>
+      <c r="AEQ2" s="0"/>
+      <c r="AER2" s="0"/>
+      <c r="AES2" s="0"/>
+      <c r="AET2" s="0"/>
+      <c r="AEU2" s="0"/>
+      <c r="AEV2" s="0"/>
+      <c r="AEW2" s="0"/>
+      <c r="AEX2" s="0"/>
+      <c r="AEY2" s="0"/>
+      <c r="AEZ2" s="0"/>
+      <c r="AFA2" s="0"/>
+      <c r="AFB2" s="0"/>
+      <c r="AFC2" s="0"/>
+      <c r="AFD2" s="0"/>
+      <c r="AFE2" s="0"/>
+      <c r="AFF2" s="0"/>
+      <c r="AFG2" s="0"/>
+      <c r="AFH2" s="0"/>
+      <c r="AFI2" s="0"/>
+      <c r="AFJ2" s="0"/>
+      <c r="AFK2" s="0"/>
+      <c r="AFL2" s="0"/>
+      <c r="AFM2" s="0"/>
+      <c r="AFN2" s="0"/>
+      <c r="AFO2" s="0"/>
+      <c r="AFP2" s="0"/>
+      <c r="AFQ2" s="0"/>
+      <c r="AFR2" s="0"/>
+      <c r="AFS2" s="0"/>
+      <c r="AFT2" s="0"/>
+      <c r="AFU2" s="0"/>
+      <c r="AFV2" s="0"/>
+      <c r="AFW2" s="0"/>
+      <c r="AFX2" s="0"/>
+      <c r="AFY2" s="0"/>
+      <c r="AFZ2" s="0"/>
+      <c r="AGA2" s="0"/>
+      <c r="AGB2" s="0"/>
+      <c r="AGC2" s="0"/>
+      <c r="AGD2" s="0"/>
+      <c r="AGE2" s="0"/>
+      <c r="AGF2" s="0"/>
+      <c r="AGG2" s="0"/>
+      <c r="AGH2" s="0"/>
+      <c r="AGI2" s="0"/>
+      <c r="AGJ2" s="0"/>
+      <c r="AGK2" s="0"/>
+      <c r="AGL2" s="0"/>
+      <c r="AGM2" s="0"/>
+      <c r="AGN2" s="0"/>
+      <c r="AGO2" s="0"/>
+      <c r="AGP2" s="0"/>
+      <c r="AGQ2" s="0"/>
+      <c r="AGR2" s="0"/>
+      <c r="AGS2" s="0"/>
+      <c r="AGT2" s="0"/>
+      <c r="AGU2" s="0"/>
+      <c r="AGV2" s="0"/>
+      <c r="AGW2" s="0"/>
+      <c r="AGX2" s="0"/>
+      <c r="AGY2" s="0"/>
+      <c r="AGZ2" s="0"/>
+      <c r="AHA2" s="0"/>
+      <c r="AHB2" s="0"/>
+      <c r="AHC2" s="0"/>
+      <c r="AHD2" s="0"/>
+      <c r="AHE2" s="0"/>
+      <c r="AHF2" s="0"/>
+      <c r="AHG2" s="0"/>
+      <c r="AHH2" s="0"/>
+      <c r="AHI2" s="0"/>
+      <c r="AHJ2" s="0"/>
+      <c r="AHK2" s="0"/>
+      <c r="AHL2" s="0"/>
+      <c r="AHM2" s="0"/>
+      <c r="AHN2" s="0"/>
+      <c r="AHO2" s="0"/>
+      <c r="AHP2" s="0"/>
+      <c r="AHQ2" s="0"/>
+      <c r="AHR2" s="0"/>
+      <c r="AHS2" s="0"/>
+      <c r="AHT2" s="0"/>
+      <c r="AHU2" s="0"/>
+      <c r="AHV2" s="0"/>
+      <c r="AHW2" s="0"/>
+      <c r="AHX2" s="0"/>
+      <c r="AHY2" s="0"/>
+      <c r="AHZ2" s="0"/>
+      <c r="AIA2" s="0"/>
+      <c r="AIB2" s="0"/>
+      <c r="AIC2" s="0"/>
+      <c r="AID2" s="0"/>
+      <c r="AIE2" s="0"/>
+      <c r="AIF2" s="0"/>
+      <c r="AIG2" s="0"/>
+      <c r="AIH2" s="0"/>
+      <c r="AII2" s="0"/>
+      <c r="AIJ2" s="0"/>
+      <c r="AIK2" s="0"/>
+      <c r="AIL2" s="0"/>
+      <c r="AIM2" s="0"/>
+      <c r="AIN2" s="0"/>
+      <c r="AIO2" s="0"/>
+      <c r="AIP2" s="0"/>
+      <c r="AIQ2" s="0"/>
+      <c r="AIR2" s="0"/>
+      <c r="AIS2" s="0"/>
+      <c r="AIT2" s="0"/>
+      <c r="AIU2" s="0"/>
+      <c r="AIV2" s="0"/>
+      <c r="AIW2" s="0"/>
+      <c r="AIX2" s="0"/>
+      <c r="AIY2" s="0"/>
+      <c r="AIZ2" s="0"/>
+      <c r="AJA2" s="0"/>
+      <c r="AJB2" s="0"/>
+      <c r="AJC2" s="0"/>
+      <c r="AJD2" s="0"/>
+      <c r="AJE2" s="0"/>
+      <c r="AJF2" s="0"/>
+      <c r="AJG2" s="0"/>
+      <c r="AJH2" s="0"/>
+      <c r="AJI2" s="0"/>
+      <c r="AJJ2" s="0"/>
+      <c r="AJK2" s="0"/>
+      <c r="AJL2" s="0"/>
+      <c r="AJM2" s="0"/>
+      <c r="AJN2" s="0"/>
+      <c r="AJO2" s="0"/>
+      <c r="AJP2" s="0"/>
+      <c r="AJQ2" s="0"/>
+      <c r="AJR2" s="0"/>
+      <c r="AJS2" s="0"/>
+      <c r="AJT2" s="0"/>
+      <c r="AJU2" s="0"/>
+      <c r="AJV2" s="0"/>
+      <c r="AJW2" s="0"/>
+      <c r="AJX2" s="0"/>
+      <c r="AJY2" s="0"/>
+      <c r="AJZ2" s="0"/>
+      <c r="AKA2" s="0"/>
+      <c r="AKB2" s="0"/>
+      <c r="AKC2" s="0"/>
+      <c r="AKD2" s="0"/>
+      <c r="AKE2" s="0"/>
+      <c r="AKF2" s="0"/>
+      <c r="AKG2" s="0"/>
+      <c r="AKH2" s="0"/>
+      <c r="AKI2" s="0"/>
+      <c r="AKJ2" s="0"/>
+      <c r="AKK2" s="0"/>
+      <c r="AKL2" s="0"/>
+      <c r="AKM2" s="0"/>
+      <c r="AKN2" s="0"/>
+      <c r="AKO2" s="0"/>
+      <c r="AKP2" s="0"/>
+      <c r="AKQ2" s="0"/>
+      <c r="AKR2" s="0"/>
+      <c r="AKS2" s="0"/>
+      <c r="AKT2" s="0"/>
+      <c r="AKU2" s="0"/>
+      <c r="AKV2" s="0"/>
+      <c r="AKW2" s="0"/>
+      <c r="AKX2" s="0"/>
+      <c r="AKY2" s="0"/>
+      <c r="AKZ2" s="0"/>
+      <c r="ALA2" s="0"/>
+      <c r="ALB2" s="0"/>
+      <c r="ALC2" s="0"/>
+      <c r="ALD2" s="0"/>
+      <c r="ALE2" s="0"/>
+      <c r="ALF2" s="0"/>
+      <c r="ALG2" s="0"/>
+      <c r="ALH2" s="0"/>
+      <c r="ALI2" s="0"/>
+      <c r="ALJ2" s="0"/>
+      <c r="ALK2" s="0"/>
+      <c r="ALL2" s="0"/>
+      <c r="ALM2" s="0"/>
+      <c r="ALN2" s="0"/>
+      <c r="ALO2" s="0"/>
+      <c r="ALP2" s="0"/>
+      <c r="ALQ2" s="0"/>
+      <c r="ALR2" s="0"/>
+      <c r="ALS2" s="0"/>
+      <c r="ALT2" s="0"/>
+      <c r="ALU2" s="0"/>
+      <c r="ALV2" s="0"/>
+      <c r="ALW2" s="0"/>
+      <c r="ALX2" s="0"/>
+      <c r="ALY2" s="0"/>
+      <c r="ALZ2" s="0"/>
+      <c r="AMA2" s="0"/>
+      <c r="AMB2" s="0"/>
+      <c r="AMC2" s="0"/>
+      <c r="AMD2" s="0"/>
+      <c r="AME2" s="0"/>
+      <c r="AMF2" s="0"/>
+      <c r="AMG2" s="0"/>
+      <c r="AMH2" s="0"/>
+      <c r="AMI2" s="0"/>
+      <c r="AMJ2" s="0"/>
     </row>
-    <row r="3" customFormat="false" ht="24.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="72" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="73" t="s">
-        <v>40</v>
-      </c>
-      <c r="C3" s="73" t="s">
-        <v>41</v>
-      </c>
-      <c r="D3" s="74" t="s">
-        <v>73</v>
-      </c>
-      <c r="E3" s="75" t="s">
-        <v>74</v>
-      </c>
-      <c r="F3" s="76" t="n">
-        <v>1</v>
-      </c>
-      <c r="G3" s="77" t="n">
-        <v>0</v>
-      </c>
-      <c r="H3" s="76" t="n">
-        <v>1</v>
-      </c>
-      <c r="I3" s="77" t="n">
-        <v>0</v>
-      </c>
+      <c r="B3" s="73"/>
+      <c r="C3" s="73"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="75"/>
+      <c r="F3" s="76"/>
+      <c r="G3" s="77"/>
+      <c r="H3" s="76"/>
+      <c r="I3" s="77"/>
+      <c r="J3" s="0"/>
+      <c r="K3" s="0"/>
+      <c r="L3" s="0"/>
+      <c r="M3" s="0"/>
+      <c r="N3" s="0"/>
+      <c r="O3" s="0"/>
+      <c r="P3" s="0"/>
+      <c r="Q3" s="0"/>
+      <c r="R3" s="0"/>
+      <c r="S3" s="0"/>
+      <c r="T3" s="0"/>
+      <c r="U3" s="0"/>
+      <c r="V3" s="0"/>
+      <c r="W3" s="0"/>
+      <c r="X3" s="0"/>
+      <c r="Y3" s="0"/>
+      <c r="Z3" s="0"/>
+      <c r="AA3" s="0"/>
+      <c r="AB3" s="0"/>
+      <c r="AC3" s="0"/>
+      <c r="AD3" s="0"/>
+      <c r="AE3" s="0"/>
+      <c r="AF3" s="0"/>
+      <c r="AG3" s="0"/>
+      <c r="AH3" s="0"/>
+      <c r="AI3" s="0"/>
+      <c r="AJ3" s="0"/>
+      <c r="AK3" s="0"/>
+      <c r="AL3" s="0"/>
+      <c r="AM3" s="0"/>
+      <c r="AN3" s="0"/>
+      <c r="AO3" s="0"/>
+      <c r="AP3" s="0"/>
+      <c r="AQ3" s="0"/>
+      <c r="AR3" s="0"/>
+      <c r="AS3" s="0"/>
+      <c r="AT3" s="0"/>
+      <c r="AU3" s="0"/>
+      <c r="AV3" s="0"/>
+      <c r="AW3" s="0"/>
+      <c r="AX3" s="0"/>
+      <c r="AY3" s="0"/>
+      <c r="AZ3" s="0"/>
+      <c r="BA3" s="0"/>
+      <c r="BB3" s="0"/>
+      <c r="BC3" s="0"/>
+      <c r="BD3" s="0"/>
+      <c r="BE3" s="0"/>
+      <c r="BF3" s="0"/>
+      <c r="BG3" s="0"/>
+      <c r="BH3" s="0"/>
+      <c r="BI3" s="0"/>
+      <c r="BJ3" s="0"/>
+      <c r="BK3" s="0"/>
+      <c r="BL3" s="0"/>
+      <c r="BM3" s="0"/>
+      <c r="BN3" s="0"/>
+      <c r="BO3" s="0"/>
+      <c r="BP3" s="0"/>
+      <c r="BQ3" s="0"/>
+      <c r="BR3" s="0"/>
+      <c r="BS3" s="0"/>
+      <c r="BT3" s="0"/>
+      <c r="BU3" s="0"/>
+      <c r="BV3" s="0"/>
+      <c r="BW3" s="0"/>
+      <c r="BX3" s="0"/>
+      <c r="BY3" s="0"/>
+      <c r="BZ3" s="0"/>
+      <c r="CA3" s="0"/>
+      <c r="CB3" s="0"/>
+      <c r="CC3" s="0"/>
+      <c r="CD3" s="0"/>
+      <c r="CE3" s="0"/>
+      <c r="CF3" s="0"/>
+      <c r="CG3" s="0"/>
+      <c r="CH3" s="0"/>
+      <c r="CI3" s="0"/>
+      <c r="CJ3" s="0"/>
+      <c r="CK3" s="0"/>
+      <c r="CL3" s="0"/>
+      <c r="CM3" s="0"/>
+      <c r="CN3" s="0"/>
+      <c r="CO3" s="0"/>
+      <c r="CP3" s="0"/>
+      <c r="CQ3" s="0"/>
+      <c r="CR3" s="0"/>
+      <c r="CS3" s="0"/>
+      <c r="CT3" s="0"/>
+      <c r="CU3" s="0"/>
+      <c r="CV3" s="0"/>
+      <c r="CW3" s="0"/>
+      <c r="CX3" s="0"/>
+      <c r="CY3" s="0"/>
+      <c r="CZ3" s="0"/>
+      <c r="DA3" s="0"/>
+      <c r="DB3" s="0"/>
+      <c r="DC3" s="0"/>
+      <c r="DD3" s="0"/>
+      <c r="DE3" s="0"/>
+      <c r="DF3" s="0"/>
+      <c r="DG3" s="0"/>
+      <c r="DH3" s="0"/>
+      <c r="DI3" s="0"/>
+      <c r="DJ3" s="0"/>
+      <c r="DK3" s="0"/>
+      <c r="DL3" s="0"/>
+      <c r="DM3" s="0"/>
+      <c r="DN3" s="0"/>
+      <c r="DO3" s="0"/>
+      <c r="DP3" s="0"/>
+      <c r="DQ3" s="0"/>
+      <c r="DR3" s="0"/>
+      <c r="DS3" s="0"/>
+      <c r="DT3" s="0"/>
+      <c r="DU3" s="0"/>
+      <c r="DV3" s="0"/>
+      <c r="DW3" s="0"/>
+      <c r="DX3" s="0"/>
+      <c r="DY3" s="0"/>
+      <c r="DZ3" s="0"/>
+      <c r="EA3" s="0"/>
+      <c r="EB3" s="0"/>
+      <c r="EC3" s="0"/>
+      <c r="ED3" s="0"/>
+      <c r="EE3" s="0"/>
+      <c r="EF3" s="0"/>
+      <c r="EG3" s="0"/>
+      <c r="EH3" s="0"/>
+      <c r="EI3" s="0"/>
+      <c r="EJ3" s="0"/>
+      <c r="EK3" s="0"/>
+      <c r="EL3" s="0"/>
+      <c r="EM3" s="0"/>
+      <c r="EN3" s="0"/>
+      <c r="EO3" s="0"/>
+      <c r="EP3" s="0"/>
+      <c r="EQ3" s="0"/>
+      <c r="ER3" s="0"/>
+      <c r="ES3" s="0"/>
+      <c r="ET3" s="0"/>
+      <c r="EU3" s="0"/>
+      <c r="EV3" s="0"/>
+      <c r="EW3" s="0"/>
+      <c r="EX3" s="0"/>
+      <c r="EY3" s="0"/>
+      <c r="EZ3" s="0"/>
+      <c r="FA3" s="0"/>
+      <c r="FB3" s="0"/>
+      <c r="FC3" s="0"/>
+      <c r="FD3" s="0"/>
+      <c r="FE3" s="0"/>
+      <c r="FF3" s="0"/>
+      <c r="FG3" s="0"/>
+      <c r="FH3" s="0"/>
+      <c r="FI3" s="0"/>
+      <c r="FJ3" s="0"/>
+      <c r="FK3" s="0"/>
+      <c r="FL3" s="0"/>
+      <c r="FM3" s="0"/>
+      <c r="FN3" s="0"/>
+      <c r="FO3" s="0"/>
+      <c r="FP3" s="0"/>
+      <c r="FQ3" s="0"/>
+      <c r="FR3" s="0"/>
+      <c r="FS3" s="0"/>
+      <c r="FT3" s="0"/>
+      <c r="FU3" s="0"/>
+      <c r="FV3" s="0"/>
+      <c r="FW3" s="0"/>
+      <c r="FX3" s="0"/>
+      <c r="FY3" s="0"/>
+      <c r="FZ3" s="0"/>
+      <c r="GA3" s="0"/>
+      <c r="GB3" s="0"/>
+      <c r="GC3" s="0"/>
+      <c r="GD3" s="0"/>
+      <c r="GE3" s="0"/>
+      <c r="GF3" s="0"/>
+      <c r="GG3" s="0"/>
+      <c r="GH3" s="0"/>
+      <c r="GI3" s="0"/>
+      <c r="GJ3" s="0"/>
+      <c r="GK3" s="0"/>
+      <c r="GL3" s="0"/>
+      <c r="GM3" s="0"/>
+      <c r="GN3" s="0"/>
+      <c r="GO3" s="0"/>
+      <c r="GP3" s="0"/>
+      <c r="GQ3" s="0"/>
+      <c r="GR3" s="0"/>
+      <c r="GS3" s="0"/>
+      <c r="GT3" s="0"/>
+      <c r="GU3" s="0"/>
+      <c r="GV3" s="0"/>
+      <c r="GW3" s="0"/>
+      <c r="GX3" s="0"/>
+      <c r="GY3" s="0"/>
+      <c r="GZ3" s="0"/>
+      <c r="HA3" s="0"/>
+      <c r="HB3" s="0"/>
+      <c r="HC3" s="0"/>
+      <c r="HD3" s="0"/>
+      <c r="HE3" s="0"/>
+      <c r="HF3" s="0"/>
+      <c r="HG3" s="0"/>
+      <c r="HH3" s="0"/>
+      <c r="HI3" s="0"/>
+      <c r="HJ3" s="0"/>
+      <c r="HK3" s="0"/>
+      <c r="HL3" s="0"/>
+      <c r="HM3" s="0"/>
+      <c r="HN3" s="0"/>
+      <c r="HO3" s="0"/>
+      <c r="HP3" s="0"/>
+      <c r="HQ3" s="0"/>
+      <c r="HR3" s="0"/>
+      <c r="HS3" s="0"/>
+      <c r="HT3" s="0"/>
+      <c r="HU3" s="0"/>
+      <c r="HV3" s="0"/>
+      <c r="HW3" s="0"/>
+      <c r="HX3" s="0"/>
+      <c r="HY3" s="0"/>
+      <c r="HZ3" s="0"/>
+      <c r="IA3" s="0"/>
+      <c r="IB3" s="0"/>
+      <c r="IC3" s="0"/>
+      <c r="ID3" s="0"/>
+      <c r="IE3" s="0"/>
+      <c r="IF3" s="0"/>
+      <c r="IG3" s="0"/>
+      <c r="IH3" s="0"/>
+      <c r="II3" s="0"/>
+      <c r="IJ3" s="0"/>
+      <c r="IK3" s="0"/>
+      <c r="IL3" s="0"/>
+      <c r="IM3" s="0"/>
+      <c r="IN3" s="0"/>
+      <c r="IO3" s="0"/>
+      <c r="IP3" s="0"/>
+      <c r="IQ3" s="0"/>
+      <c r="IR3" s="0"/>
+      <c r="IS3" s="0"/>
+      <c r="IT3" s="0"/>
+      <c r="IU3" s="0"/>
+      <c r="IV3" s="0"/>
+      <c r="IW3" s="0"/>
+      <c r="IX3" s="0"/>
+      <c r="IY3" s="0"/>
+      <c r="IZ3" s="0"/>
+      <c r="JA3" s="0"/>
+      <c r="JB3" s="0"/>
+      <c r="JC3" s="0"/>
+      <c r="JD3" s="0"/>
+      <c r="JE3" s="0"/>
+      <c r="JF3" s="0"/>
+      <c r="JG3" s="0"/>
+      <c r="JH3" s="0"/>
+      <c r="JI3" s="0"/>
+      <c r="JJ3" s="0"/>
+      <c r="JK3" s="0"/>
+      <c r="JL3" s="0"/>
+      <c r="JM3" s="0"/>
+      <c r="JN3" s="0"/>
+      <c r="JO3" s="0"/>
+      <c r="JP3" s="0"/>
+      <c r="JQ3" s="0"/>
+      <c r="JR3" s="0"/>
+      <c r="JS3" s="0"/>
+      <c r="JT3" s="0"/>
+      <c r="JU3" s="0"/>
+      <c r="JV3" s="0"/>
+      <c r="JW3" s="0"/>
+      <c r="JX3" s="0"/>
+      <c r="JY3" s="0"/>
+      <c r="JZ3" s="0"/>
+      <c r="KA3" s="0"/>
+      <c r="KB3" s="0"/>
+      <c r="KC3" s="0"/>
+      <c r="KD3" s="0"/>
+      <c r="KE3" s="0"/>
+      <c r="KF3" s="0"/>
+      <c r="KG3" s="0"/>
+      <c r="KH3" s="0"/>
+      <c r="KI3" s="0"/>
+      <c r="KJ3" s="0"/>
+      <c r="KK3" s="0"/>
+      <c r="KL3" s="0"/>
+      <c r="KM3" s="0"/>
+      <c r="KN3" s="0"/>
+      <c r="KO3" s="0"/>
+      <c r="KP3" s="0"/>
+      <c r="KQ3" s="0"/>
+      <c r="KR3" s="0"/>
+      <c r="KS3" s="0"/>
+      <c r="KT3" s="0"/>
+      <c r="KU3" s="0"/>
+      <c r="KV3" s="0"/>
+      <c r="KW3" s="0"/>
+      <c r="KX3" s="0"/>
+      <c r="KY3" s="0"/>
+      <c r="KZ3" s="0"/>
+      <c r="LA3" s="0"/>
+      <c r="LB3" s="0"/>
+      <c r="LC3" s="0"/>
+      <c r="LD3" s="0"/>
+      <c r="LE3" s="0"/>
+      <c r="LF3" s="0"/>
+      <c r="LG3" s="0"/>
+      <c r="LH3" s="0"/>
+      <c r="LI3" s="0"/>
+      <c r="LJ3" s="0"/>
+      <c r="LK3" s="0"/>
+      <c r="LL3" s="0"/>
+      <c r="LM3" s="0"/>
+      <c r="LN3" s="0"/>
+      <c r="LO3" s="0"/>
+      <c r="LP3" s="0"/>
+      <c r="LQ3" s="0"/>
+      <c r="LR3" s="0"/>
+      <c r="LS3" s="0"/>
+      <c r="LT3" s="0"/>
+      <c r="LU3" s="0"/>
+      <c r="LV3" s="0"/>
+      <c r="LW3" s="0"/>
+      <c r="LX3" s="0"/>
+      <c r="LY3" s="0"/>
+      <c r="LZ3" s="0"/>
+      <c r="MA3" s="0"/>
+      <c r="MB3" s="0"/>
+      <c r="MC3" s="0"/>
+      <c r="MD3" s="0"/>
+      <c r="ME3" s="0"/>
+      <c r="MF3" s="0"/>
+      <c r="MG3" s="0"/>
+      <c r="MH3" s="0"/>
+      <c r="MI3" s="0"/>
+      <c r="MJ3" s="0"/>
+      <c r="MK3" s="0"/>
+      <c r="ML3" s="0"/>
+      <c r="MM3" s="0"/>
+      <c r="MN3" s="0"/>
+      <c r="MO3" s="0"/>
+      <c r="MP3" s="0"/>
+      <c r="MQ3" s="0"/>
+      <c r="MR3" s="0"/>
+      <c r="MS3" s="0"/>
+      <c r="MT3" s="0"/>
+      <c r="MU3" s="0"/>
+      <c r="MV3" s="0"/>
+      <c r="MW3" s="0"/>
+      <c r="MX3" s="0"/>
+      <c r="MY3" s="0"/>
+      <c r="MZ3" s="0"/>
+      <c r="NA3" s="0"/>
+      <c r="NB3" s="0"/>
+      <c r="NC3" s="0"/>
+      <c r="ND3" s="0"/>
+      <c r="NE3" s="0"/>
+      <c r="NF3" s="0"/>
+      <c r="NG3" s="0"/>
+      <c r="NH3" s="0"/>
+      <c r="NI3" s="0"/>
+      <c r="NJ3" s="0"/>
+      <c r="NK3" s="0"/>
+      <c r="NL3" s="0"/>
+      <c r="NM3" s="0"/>
+      <c r="NN3" s="0"/>
+      <c r="NO3" s="0"/>
+      <c r="NP3" s="0"/>
+      <c r="NQ3" s="0"/>
+      <c r="NR3" s="0"/>
+      <c r="NS3" s="0"/>
+      <c r="NT3" s="0"/>
+      <c r="NU3" s="0"/>
+      <c r="NV3" s="0"/>
+      <c r="NW3" s="0"/>
+      <c r="NX3" s="0"/>
+      <c r="NY3" s="0"/>
+      <c r="NZ3" s="0"/>
+      <c r="OA3" s="0"/>
+      <c r="OB3" s="0"/>
+      <c r="OC3" s="0"/>
+      <c r="OD3" s="0"/>
+      <c r="OE3" s="0"/>
+      <c r="OF3" s="0"/>
+      <c r="OG3" s="0"/>
+      <c r="OH3" s="0"/>
+      <c r="OI3" s="0"/>
+      <c r="OJ3" s="0"/>
+      <c r="OK3" s="0"/>
+      <c r="OL3" s="0"/>
+      <c r="OM3" s="0"/>
+      <c r="ON3" s="0"/>
+      <c r="OO3" s="0"/>
+      <c r="OP3" s="0"/>
+      <c r="OQ3" s="0"/>
+      <c r="OR3" s="0"/>
+      <c r="OS3" s="0"/>
+      <c r="OT3" s="0"/>
+      <c r="OU3" s="0"/>
+      <c r="OV3" s="0"/>
+      <c r="OW3" s="0"/>
+      <c r="OX3" s="0"/>
+      <c r="OY3" s="0"/>
+      <c r="OZ3" s="0"/>
+      <c r="PA3" s="0"/>
+      <c r="PB3" s="0"/>
+      <c r="PC3" s="0"/>
+      <c r="PD3" s="0"/>
+      <c r="PE3" s="0"/>
+      <c r="PF3" s="0"/>
+      <c r="PG3" s="0"/>
+      <c r="PH3" s="0"/>
+      <c r="PI3" s="0"/>
+      <c r="PJ3" s="0"/>
+      <c r="PK3" s="0"/>
+      <c r="PL3" s="0"/>
+      <c r="PM3" s="0"/>
+      <c r="PN3" s="0"/>
+      <c r="PO3" s="0"/>
+      <c r="PP3" s="0"/>
+      <c r="PQ3" s="0"/>
+      <c r="PR3" s="0"/>
+      <c r="PS3" s="0"/>
+      <c r="PT3" s="0"/>
+      <c r="PU3" s="0"/>
+      <c r="PV3" s="0"/>
+      <c r="PW3" s="0"/>
+      <c r="PX3" s="0"/>
+      <c r="PY3" s="0"/>
+      <c r="PZ3" s="0"/>
+      <c r="QA3" s="0"/>
+      <c r="QB3" s="0"/>
+      <c r="QC3" s="0"/>
+      <c r="QD3" s="0"/>
+      <c r="QE3" s="0"/>
+      <c r="QF3" s="0"/>
+      <c r="QG3" s="0"/>
+      <c r="QH3" s="0"/>
+      <c r="QI3" s="0"/>
+      <c r="QJ3" s="0"/>
+      <c r="QK3" s="0"/>
+      <c r="QL3" s="0"/>
+      <c r="QM3" s="0"/>
+      <c r="QN3" s="0"/>
+      <c r="QO3" s="0"/>
+      <c r="QP3" s="0"/>
+      <c r="QQ3" s="0"/>
+      <c r="QR3" s="0"/>
+      <c r="QS3" s="0"/>
+      <c r="QT3" s="0"/>
+      <c r="QU3" s="0"/>
+      <c r="QV3" s="0"/>
+      <c r="QW3" s="0"/>
+      <c r="QX3" s="0"/>
+      <c r="QY3" s="0"/>
+      <c r="QZ3" s="0"/>
+      <c r="RA3" s="0"/>
+      <c r="RB3" s="0"/>
+      <c r="RC3" s="0"/>
+      <c r="RD3" s="0"/>
+      <c r="RE3" s="0"/>
+      <c r="RF3" s="0"/>
+      <c r="RG3" s="0"/>
+      <c r="RH3" s="0"/>
+      <c r="RI3" s="0"/>
+      <c r="RJ3" s="0"/>
+      <c r="RK3" s="0"/>
+      <c r="RL3" s="0"/>
+      <c r="RM3" s="0"/>
+      <c r="RN3" s="0"/>
+      <c r="RO3" s="0"/>
+      <c r="RP3" s="0"/>
+      <c r="RQ3" s="0"/>
+      <c r="RR3" s="0"/>
+      <c r="RS3" s="0"/>
+      <c r="RT3" s="0"/>
+      <c r="RU3" s="0"/>
+      <c r="RV3" s="0"/>
+      <c r="RW3" s="0"/>
+      <c r="RX3" s="0"/>
+      <c r="RY3" s="0"/>
+      <c r="RZ3" s="0"/>
+      <c r="SA3" s="0"/>
+      <c r="SB3" s="0"/>
+      <c r="SC3" s="0"/>
+      <c r="SD3" s="0"/>
+      <c r="SE3" s="0"/>
+      <c r="SF3" s="0"/>
+      <c r="SG3" s="0"/>
+      <c r="SH3" s="0"/>
+      <c r="SI3" s="0"/>
+      <c r="SJ3" s="0"/>
+      <c r="SK3" s="0"/>
+      <c r="SL3" s="0"/>
+      <c r="SM3" s="0"/>
+      <c r="SN3" s="0"/>
+      <c r="SO3" s="0"/>
+      <c r="SP3" s="0"/>
+      <c r="SQ3" s="0"/>
+      <c r="SR3" s="0"/>
+      <c r="SS3" s="0"/>
+      <c r="ST3" s="0"/>
+      <c r="SU3" s="0"/>
+      <c r="SV3" s="0"/>
+      <c r="SW3" s="0"/>
+      <c r="SX3" s="0"/>
+      <c r="SY3" s="0"/>
+      <c r="SZ3" s="0"/>
+      <c r="TA3" s="0"/>
+      <c r="TB3" s="0"/>
+      <c r="TC3" s="0"/>
+      <c r="TD3" s="0"/>
+      <c r="TE3" s="0"/>
+      <c r="TF3" s="0"/>
+      <c r="TG3" s="0"/>
+      <c r="TH3" s="0"/>
+      <c r="TI3" s="0"/>
+      <c r="TJ3" s="0"/>
+      <c r="TK3" s="0"/>
+      <c r="TL3" s="0"/>
+      <c r="TM3" s="0"/>
+      <c r="TN3" s="0"/>
+      <c r="TO3" s="0"/>
+      <c r="TP3" s="0"/>
+      <c r="TQ3" s="0"/>
+      <c r="TR3" s="0"/>
+      <c r="TS3" s="0"/>
+      <c r="TT3" s="0"/>
+      <c r="TU3" s="0"/>
+      <c r="TV3" s="0"/>
+      <c r="TW3" s="0"/>
+      <c r="TX3" s="0"/>
+      <c r="TY3" s="0"/>
+      <c r="TZ3" s="0"/>
+      <c r="UA3" s="0"/>
+      <c r="UB3" s="0"/>
+      <c r="UC3" s="0"/>
+      <c r="UD3" s="0"/>
+      <c r="UE3" s="0"/>
+      <c r="UF3" s="0"/>
+      <c r="UG3" s="0"/>
+      <c r="UH3" s="0"/>
+      <c r="UI3" s="0"/>
+      <c r="UJ3" s="0"/>
+      <c r="UK3" s="0"/>
+      <c r="UL3" s="0"/>
+      <c r="UM3" s="0"/>
+      <c r="UN3" s="0"/>
+      <c r="UO3" s="0"/>
+      <c r="UP3" s="0"/>
+      <c r="UQ3" s="0"/>
+      <c r="UR3" s="0"/>
+      <c r="US3" s="0"/>
+      <c r="UT3" s="0"/>
+      <c r="UU3" s="0"/>
+      <c r="UV3" s="0"/>
+      <c r="UW3" s="0"/>
+      <c r="UX3" s="0"/>
+      <c r="UY3" s="0"/>
+      <c r="UZ3" s="0"/>
+      <c r="VA3" s="0"/>
+      <c r="VB3" s="0"/>
+      <c r="VC3" s="0"/>
+      <c r="VD3" s="0"/>
+      <c r="VE3" s="0"/>
+      <c r="VF3" s="0"/>
+      <c r="VG3" s="0"/>
+      <c r="VH3" s="0"/>
+      <c r="VI3" s="0"/>
+      <c r="VJ3" s="0"/>
+      <c r="VK3" s="0"/>
+      <c r="VL3" s="0"/>
+      <c r="VM3" s="0"/>
+      <c r="VN3" s="0"/>
+      <c r="VO3" s="0"/>
+      <c r="VP3" s="0"/>
+      <c r="VQ3" s="0"/>
+      <c r="VR3" s="0"/>
+      <c r="VS3" s="0"/>
+      <c r="VT3" s="0"/>
+      <c r="VU3" s="0"/>
+      <c r="VV3" s="0"/>
+      <c r="VW3" s="0"/>
+      <c r="VX3" s="0"/>
+      <c r="VY3" s="0"/>
+      <c r="VZ3" s="0"/>
+      <c r="WA3" s="0"/>
+      <c r="WB3" s="0"/>
+      <c r="WC3" s="0"/>
+      <c r="WD3" s="0"/>
+      <c r="WE3" s="0"/>
+      <c r="WF3" s="0"/>
+      <c r="WG3" s="0"/>
+      <c r="WH3" s="0"/>
+      <c r="WI3" s="0"/>
+      <c r="WJ3" s="0"/>
+      <c r="WK3" s="0"/>
+      <c r="WL3" s="0"/>
+      <c r="WM3" s="0"/>
+      <c r="WN3" s="0"/>
+      <c r="WO3" s="0"/>
+      <c r="WP3" s="0"/>
+      <c r="WQ3" s="0"/>
+      <c r="WR3" s="0"/>
+      <c r="WS3" s="0"/>
+      <c r="WT3" s="0"/>
+      <c r="WU3" s="0"/>
+      <c r="WV3" s="0"/>
+      <c r="WW3" s="0"/>
+      <c r="WX3" s="0"/>
+      <c r="WY3" s="0"/>
+      <c r="WZ3" s="0"/>
+      <c r="XA3" s="0"/>
+      <c r="XB3" s="0"/>
+      <c r="XC3" s="0"/>
+      <c r="XD3" s="0"/>
+      <c r="XE3" s="0"/>
+      <c r="XF3" s="0"/>
+      <c r="XG3" s="0"/>
+      <c r="XH3" s="0"/>
+      <c r="XI3" s="0"/>
+      <c r="XJ3" s="0"/>
+      <c r="XK3" s="0"/>
+      <c r="XL3" s="0"/>
+      <c r="XM3" s="0"/>
+      <c r="XN3" s="0"/>
+      <c r="XO3" s="0"/>
+      <c r="XP3" s="0"/>
+      <c r="XQ3" s="0"/>
+      <c r="XR3" s="0"/>
+      <c r="XS3" s="0"/>
+      <c r="XT3" s="0"/>
+      <c r="XU3" s="0"/>
+      <c r="XV3" s="0"/>
+      <c r="XW3" s="0"/>
+      <c r="XX3" s="0"/>
+      <c r="XY3" s="0"/>
+      <c r="XZ3" s="0"/>
+      <c r="YA3" s="0"/>
+      <c r="YB3" s="0"/>
+      <c r="YC3" s="0"/>
+      <c r="YD3" s="0"/>
+      <c r="YE3" s="0"/>
+      <c r="YF3" s="0"/>
+      <c r="YG3" s="0"/>
+      <c r="YH3" s="0"/>
+      <c r="YI3" s="0"/>
+      <c r="YJ3" s="0"/>
+      <c r="YK3" s="0"/>
+      <c r="YL3" s="0"/>
+      <c r="YM3" s="0"/>
+      <c r="YN3" s="0"/>
+      <c r="YO3" s="0"/>
+      <c r="YP3" s="0"/>
+      <c r="YQ3" s="0"/>
+      <c r="YR3" s="0"/>
+      <c r="YS3" s="0"/>
+      <c r="YT3" s="0"/>
+      <c r="YU3" s="0"/>
+      <c r="YV3" s="0"/>
+      <c r="YW3" s="0"/>
+      <c r="YX3" s="0"/>
+      <c r="YY3" s="0"/>
+      <c r="YZ3" s="0"/>
+      <c r="ZA3" s="0"/>
+      <c r="ZB3" s="0"/>
+      <c r="ZC3" s="0"/>
+      <c r="ZD3" s="0"/>
+      <c r="ZE3" s="0"/>
+      <c r="ZF3" s="0"/>
+      <c r="ZG3" s="0"/>
+      <c r="ZH3" s="0"/>
+      <c r="ZI3" s="0"/>
+      <c r="ZJ3" s="0"/>
+      <c r="ZK3" s="0"/>
+      <c r="ZL3" s="0"/>
+      <c r="ZM3" s="0"/>
+      <c r="ZN3" s="0"/>
+      <c r="ZO3" s="0"/>
+      <c r="ZP3" s="0"/>
+      <c r="ZQ3" s="0"/>
+      <c r="ZR3" s="0"/>
+      <c r="ZS3" s="0"/>
+      <c r="ZT3" s="0"/>
+      <c r="ZU3" s="0"/>
+      <c r="ZV3" s="0"/>
+      <c r="ZW3" s="0"/>
+      <c r="ZX3" s="0"/>
+      <c r="ZY3" s="0"/>
+      <c r="ZZ3" s="0"/>
+      <c r="AAA3" s="0"/>
+      <c r="AAB3" s="0"/>
+      <c r="AAC3" s="0"/>
+      <c r="AAD3" s="0"/>
+      <c r="AAE3" s="0"/>
+      <c r="AAF3" s="0"/>
+      <c r="AAG3" s="0"/>
+      <c r="AAH3" s="0"/>
+      <c r="AAI3" s="0"/>
+      <c r="AAJ3" s="0"/>
+      <c r="AAK3" s="0"/>
+      <c r="AAL3" s="0"/>
+      <c r="AAM3" s="0"/>
+      <c r="AAN3" s="0"/>
+      <c r="AAO3" s="0"/>
+      <c r="AAP3" s="0"/>
+      <c r="AAQ3" s="0"/>
+      <c r="AAR3" s="0"/>
+      <c r="AAS3" s="0"/>
+      <c r="AAT3" s="0"/>
+      <c r="AAU3" s="0"/>
+      <c r="AAV3" s="0"/>
+      <c r="AAW3" s="0"/>
+      <c r="AAX3" s="0"/>
+      <c r="AAY3" s="0"/>
+      <c r="AAZ3" s="0"/>
+      <c r="ABA3" s="0"/>
+      <c r="ABB3" s="0"/>
+      <c r="ABC3" s="0"/>
+      <c r="ABD3" s="0"/>
+      <c r="ABE3" s="0"/>
+      <c r="ABF3" s="0"/>
+      <c r="ABG3" s="0"/>
+      <c r="ABH3" s="0"/>
+      <c r="ABI3" s="0"/>
+      <c r="ABJ3" s="0"/>
+      <c r="ABK3" s="0"/>
+      <c r="ABL3" s="0"/>
+      <c r="ABM3" s="0"/>
+      <c r="ABN3" s="0"/>
+      <c r="ABO3" s="0"/>
+      <c r="ABP3" s="0"/>
+      <c r="ABQ3" s="0"/>
+      <c r="ABR3" s="0"/>
+      <c r="ABS3" s="0"/>
+      <c r="ABT3" s="0"/>
+      <c r="ABU3" s="0"/>
+      <c r="ABV3" s="0"/>
+      <c r="ABW3" s="0"/>
+      <c r="ABX3" s="0"/>
+      <c r="ABY3" s="0"/>
+      <c r="ABZ3" s="0"/>
+      <c r="ACA3" s="0"/>
+      <c r="ACB3" s="0"/>
+      <c r="ACC3" s="0"/>
+      <c r="ACD3" s="0"/>
+      <c r="ACE3" s="0"/>
+      <c r="ACF3" s="0"/>
+      <c r="ACG3" s="0"/>
+      <c r="ACH3" s="0"/>
+      <c r="ACI3" s="0"/>
+      <c r="ACJ3" s="0"/>
+      <c r="ACK3" s="0"/>
+      <c r="ACL3" s="0"/>
+      <c r="ACM3" s="0"/>
+      <c r="ACN3" s="0"/>
+      <c r="ACO3" s="0"/>
+      <c r="ACP3" s="0"/>
+      <c r="ACQ3" s="0"/>
+      <c r="ACR3" s="0"/>
+      <c r="ACS3" s="0"/>
+      <c r="ACT3" s="0"/>
+      <c r="ACU3" s="0"/>
+      <c r="ACV3" s="0"/>
+      <c r="ACW3" s="0"/>
+      <c r="ACX3" s="0"/>
+      <c r="ACY3" s="0"/>
+      <c r="ACZ3" s="0"/>
+      <c r="ADA3" s="0"/>
+      <c r="ADB3" s="0"/>
+      <c r="ADC3" s="0"/>
+      <c r="ADD3" s="0"/>
+      <c r="ADE3" s="0"/>
+      <c r="ADF3" s="0"/>
+      <c r="ADG3" s="0"/>
+      <c r="ADH3" s="0"/>
+      <c r="ADI3" s="0"/>
+      <c r="ADJ3" s="0"/>
+      <c r="ADK3" s="0"/>
+      <c r="ADL3" s="0"/>
+      <c r="ADM3" s="0"/>
+      <c r="ADN3" s="0"/>
+      <c r="ADO3" s="0"/>
+      <c r="ADP3" s="0"/>
+      <c r="ADQ3" s="0"/>
+      <c r="ADR3" s="0"/>
+      <c r="ADS3" s="0"/>
+      <c r="ADT3" s="0"/>
+      <c r="ADU3" s="0"/>
+      <c r="ADV3" s="0"/>
+      <c r="ADW3" s="0"/>
+      <c r="ADX3" s="0"/>
+      <c r="ADY3" s="0"/>
+      <c r="ADZ3" s="0"/>
+      <c r="AEA3" s="0"/>
+      <c r="AEB3" s="0"/>
+      <c r="AEC3" s="0"/>
+      <c r="AED3" s="0"/>
+      <c r="AEE3" s="0"/>
+      <c r="AEF3" s="0"/>
+      <c r="AEG3" s="0"/>
+      <c r="AEH3" s="0"/>
+      <c r="AEI3" s="0"/>
+      <c r="AEJ3" s="0"/>
+      <c r="AEK3" s="0"/>
+      <c r="AEL3" s="0"/>
+      <c r="AEM3" s="0"/>
+      <c r="AEN3" s="0"/>
+      <c r="AEO3" s="0"/>
+      <c r="AEP3" s="0"/>
+      <c r="AEQ3" s="0"/>
+      <c r="AER3" s="0"/>
+      <c r="AES3" s="0"/>
+      <c r="AET3" s="0"/>
+      <c r="AEU3" s="0"/>
+      <c r="AEV3" s="0"/>
+      <c r="AEW3" s="0"/>
+      <c r="AEX3" s="0"/>
+      <c r="AEY3" s="0"/>
+      <c r="AEZ3" s="0"/>
+      <c r="AFA3" s="0"/>
+      <c r="AFB3" s="0"/>
+      <c r="AFC3" s="0"/>
+      <c r="AFD3" s="0"/>
+      <c r="AFE3" s="0"/>
+      <c r="AFF3" s="0"/>
+      <c r="AFG3" s="0"/>
+      <c r="AFH3" s="0"/>
+      <c r="AFI3" s="0"/>
+      <c r="AFJ3" s="0"/>
+      <c r="AFK3" s="0"/>
+      <c r="AFL3" s="0"/>
+      <c r="AFM3" s="0"/>
+      <c r="AFN3" s="0"/>
+      <c r="AFO3" s="0"/>
+      <c r="AFP3" s="0"/>
+      <c r="AFQ3" s="0"/>
+      <c r="AFR3" s="0"/>
+      <c r="AFS3" s="0"/>
+      <c r="AFT3" s="0"/>
+      <c r="AFU3" s="0"/>
+      <c r="AFV3" s="0"/>
+      <c r="AFW3" s="0"/>
+      <c r="AFX3" s="0"/>
+      <c r="AFY3" s="0"/>
+      <c r="AFZ3" s="0"/>
+      <c r="AGA3" s="0"/>
+      <c r="AGB3" s="0"/>
+      <c r="AGC3" s="0"/>
+      <c r="AGD3" s="0"/>
+      <c r="AGE3" s="0"/>
+      <c r="AGF3" s="0"/>
+      <c r="AGG3" s="0"/>
+      <c r="AGH3" s="0"/>
+      <c r="AGI3" s="0"/>
+      <c r="AGJ3" s="0"/>
+      <c r="AGK3" s="0"/>
+      <c r="AGL3" s="0"/>
+      <c r="AGM3" s="0"/>
+      <c r="AGN3" s="0"/>
+      <c r="AGO3" s="0"/>
+      <c r="AGP3" s="0"/>
+      <c r="AGQ3" s="0"/>
+      <c r="AGR3" s="0"/>
+      <c r="AGS3" s="0"/>
+      <c r="AGT3" s="0"/>
+      <c r="AGU3" s="0"/>
+      <c r="AGV3" s="0"/>
+      <c r="AGW3" s="0"/>
+      <c r="AGX3" s="0"/>
+      <c r="AGY3" s="0"/>
+      <c r="AGZ3" s="0"/>
+      <c r="AHA3" s="0"/>
+      <c r="AHB3" s="0"/>
+      <c r="AHC3" s="0"/>
+      <c r="AHD3" s="0"/>
+      <c r="AHE3" s="0"/>
+      <c r="AHF3" s="0"/>
+      <c r="AHG3" s="0"/>
+      <c r="AHH3" s="0"/>
+      <c r="AHI3" s="0"/>
+      <c r="AHJ3" s="0"/>
+      <c r="AHK3" s="0"/>
+      <c r="AHL3" s="0"/>
+      <c r="AHM3" s="0"/>
+      <c r="AHN3" s="0"/>
+      <c r="AHO3" s="0"/>
+      <c r="AHP3" s="0"/>
+      <c r="AHQ3" s="0"/>
+      <c r="AHR3" s="0"/>
+      <c r="AHS3" s="0"/>
+      <c r="AHT3" s="0"/>
+      <c r="AHU3" s="0"/>
+      <c r="AHV3" s="0"/>
+      <c r="AHW3" s="0"/>
+      <c r="AHX3" s="0"/>
+      <c r="AHY3" s="0"/>
+      <c r="AHZ3" s="0"/>
+      <c r="AIA3" s="0"/>
+      <c r="AIB3" s="0"/>
+      <c r="AIC3" s="0"/>
+      <c r="AID3" s="0"/>
+      <c r="AIE3" s="0"/>
+      <c r="AIF3" s="0"/>
+      <c r="AIG3" s="0"/>
+      <c r="AIH3" s="0"/>
+      <c r="AII3" s="0"/>
+      <c r="AIJ3" s="0"/>
+      <c r="AIK3" s="0"/>
+      <c r="AIL3" s="0"/>
+      <c r="AIM3" s="0"/>
+      <c r="AIN3" s="0"/>
+      <c r="AIO3" s="0"/>
+      <c r="AIP3" s="0"/>
+      <c r="AIQ3" s="0"/>
+      <c r="AIR3" s="0"/>
+      <c r="AIS3" s="0"/>
+      <c r="AIT3" s="0"/>
+      <c r="AIU3" s="0"/>
+      <c r="AIV3" s="0"/>
+      <c r="AIW3" s="0"/>
+      <c r="AIX3" s="0"/>
+      <c r="AIY3" s="0"/>
+      <c r="AIZ3" s="0"/>
+      <c r="AJA3" s="0"/>
+      <c r="AJB3" s="0"/>
+      <c r="AJC3" s="0"/>
+      <c r="AJD3" s="0"/>
+      <c r="AJE3" s="0"/>
+      <c r="AJF3" s="0"/>
+      <c r="AJG3" s="0"/>
+      <c r="AJH3" s="0"/>
+      <c r="AJI3" s="0"/>
+      <c r="AJJ3" s="0"/>
+      <c r="AJK3" s="0"/>
+      <c r="AJL3" s="0"/>
+      <c r="AJM3" s="0"/>
+      <c r="AJN3" s="0"/>
+      <c r="AJO3" s="0"/>
+      <c r="AJP3" s="0"/>
+      <c r="AJQ3" s="0"/>
+      <c r="AJR3" s="0"/>
+      <c r="AJS3" s="0"/>
+      <c r="AJT3" s="0"/>
+      <c r="AJU3" s="0"/>
+      <c r="AJV3" s="0"/>
+      <c r="AJW3" s="0"/>
+      <c r="AJX3" s="0"/>
+      <c r="AJY3" s="0"/>
+      <c r="AJZ3" s="0"/>
+      <c r="AKA3" s="0"/>
+      <c r="AKB3" s="0"/>
+      <c r="AKC3" s="0"/>
+      <c r="AKD3" s="0"/>
+      <c r="AKE3" s="0"/>
+      <c r="AKF3" s="0"/>
+      <c r="AKG3" s="0"/>
+      <c r="AKH3" s="0"/>
+      <c r="AKI3" s="0"/>
+      <c r="AKJ3" s="0"/>
+      <c r="AKK3" s="0"/>
+      <c r="AKL3" s="0"/>
+      <c r="AKM3" s="0"/>
+      <c r="AKN3" s="0"/>
+      <c r="AKO3" s="0"/>
+      <c r="AKP3" s="0"/>
+      <c r="AKQ3" s="0"/>
+      <c r="AKR3" s="0"/>
+      <c r="AKS3" s="0"/>
+      <c r="AKT3" s="0"/>
+      <c r="AKU3" s="0"/>
+      <c r="AKV3" s="0"/>
+      <c r="AKW3" s="0"/>
+      <c r="AKX3" s="0"/>
+      <c r="AKY3" s="0"/>
+      <c r="AKZ3" s="0"/>
+      <c r="ALA3" s="0"/>
+      <c r="ALB3" s="0"/>
+      <c r="ALC3" s="0"/>
+      <c r="ALD3" s="0"/>
+      <c r="ALE3" s="0"/>
+      <c r="ALF3" s="0"/>
+      <c r="ALG3" s="0"/>
+      <c r="ALH3" s="0"/>
+      <c r="ALI3" s="0"/>
+      <c r="ALJ3" s="0"/>
+      <c r="ALK3" s="0"/>
+      <c r="ALL3" s="0"/>
+      <c r="ALM3" s="0"/>
+      <c r="ALN3" s="0"/>
+      <c r="ALO3" s="0"/>
+      <c r="ALP3" s="0"/>
+      <c r="ALQ3" s="0"/>
+      <c r="ALR3" s="0"/>
+      <c r="ALS3" s="0"/>
+      <c r="ALT3" s="0"/>
+      <c r="ALU3" s="0"/>
+      <c r="ALV3" s="0"/>
+      <c r="ALW3" s="0"/>
+      <c r="ALX3" s="0"/>
+      <c r="ALY3" s="0"/>
+      <c r="ALZ3" s="0"/>
+      <c r="AMA3" s="0"/>
+      <c r="AMB3" s="0"/>
+      <c r="AMC3" s="0"/>
+      <c r="AMD3" s="0"/>
+      <c r="AME3" s="0"/>
+      <c r="AMF3" s="0"/>
+      <c r="AMG3" s="0"/>
+      <c r="AMH3" s="0"/>
+      <c r="AMI3" s="0"/>
+      <c r="AMJ3" s="0"/>
     </row>
-    <row r="4" s="82" customFormat="true" ht="24.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" s="82" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="73" t="s">
-        <v>47</v>
-      </c>
-      <c r="C4" s="73" t="s">
-        <v>48</v>
-      </c>
-      <c r="D4" s="74" t="s">
-        <v>75</v>
-      </c>
-      <c r="E4" s="79" t="s">
-        <v>76</v>
-      </c>
-      <c r="F4" s="80" t="n">
-        <v>1</v>
-      </c>
-      <c r="G4" s="81" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" s="80" t="n">
-        <v>1</v>
-      </c>
-      <c r="I4" s="81" t="n">
-        <v>0</v>
-      </c>
+      <c r="B4" s="73"/>
+      <c r="C4" s="73"/>
+      <c r="D4" s="74"/>
+      <c r="E4" s="79"/>
+      <c r="F4" s="80"/>
+      <c r="G4" s="81"/>
+      <c r="H4" s="80"/>
+      <c r="I4" s="81"/>
       <c r="AMI4" s="1"/>
       <c r="AMJ4" s="1"/>
     </row>
-    <row r="5" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="73" t="s">
-        <v>44</v>
-      </c>
-      <c r="C5" s="73" t="s">
-        <v>45</v>
-      </c>
-      <c r="D5" s="74" t="s">
-        <v>43</v>
-      </c>
-      <c r="E5" s="75" t="n">
-        <v>652426</v>
-      </c>
-      <c r="F5" s="80" t="n">
-        <v>1</v>
-      </c>
-      <c r="G5" s="81" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" s="80" t="n">
-        <v>1</v>
-      </c>
-      <c r="I5" s="81" t="n">
-        <v>0</v>
-      </c>
+      <c r="B5" s="73"/>
+      <c r="C5" s="73"/>
+      <c r="D5" s="74"/>
+      <c r="E5" s="75"/>
+      <c r="F5" s="80"/>
+      <c r="G5" s="81"/>
+      <c r="H5" s="80"/>
+      <c r="I5" s="81"/>
+      <c r="J5" s="0"/>
+      <c r="K5" s="0"/>
+      <c r="L5" s="0"/>
+      <c r="M5" s="0"/>
+      <c r="N5" s="0"/>
+      <c r="O5" s="0"/>
+      <c r="P5" s="0"/>
+      <c r="Q5" s="0"/>
+      <c r="R5" s="0"/>
+      <c r="S5" s="0"/>
+      <c r="T5" s="0"/>
+      <c r="U5" s="0"/>
+      <c r="V5" s="0"/>
+      <c r="W5" s="0"/>
+      <c r="X5" s="0"/>
+      <c r="Y5" s="0"/>
+      <c r="Z5" s="0"/>
+      <c r="AA5" s="0"/>
+      <c r="AB5" s="0"/>
+      <c r="AC5" s="0"/>
+      <c r="AD5" s="0"/>
+      <c r="AE5" s="0"/>
+      <c r="AF5" s="0"/>
+      <c r="AG5" s="0"/>
+      <c r="AH5" s="0"/>
+      <c r="AI5" s="0"/>
+      <c r="AJ5" s="0"/>
+      <c r="AK5" s="0"/>
+      <c r="AL5" s="0"/>
+      <c r="AM5" s="0"/>
+      <c r="AN5" s="0"/>
+      <c r="AO5" s="0"/>
+      <c r="AP5" s="0"/>
+      <c r="AQ5" s="0"/>
+      <c r="AR5" s="0"/>
+      <c r="AS5" s="0"/>
+      <c r="AT5" s="0"/>
+      <c r="AU5" s="0"/>
+      <c r="AV5" s="0"/>
+      <c r="AW5" s="0"/>
+      <c r="AX5" s="0"/>
+      <c r="AY5" s="0"/>
+      <c r="AZ5" s="0"/>
+      <c r="BA5" s="0"/>
+      <c r="BB5" s="0"/>
+      <c r="BC5" s="0"/>
+      <c r="BD5" s="0"/>
+      <c r="BE5" s="0"/>
+      <c r="BF5" s="0"/>
+      <c r="BG5" s="0"/>
+      <c r="BH5" s="0"/>
+      <c r="BI5" s="0"/>
+      <c r="BJ5" s="0"/>
+      <c r="BK5" s="0"/>
+      <c r="BL5" s="0"/>
+      <c r="BM5" s="0"/>
+      <c r="BN5" s="0"/>
+      <c r="BO5" s="0"/>
+      <c r="BP5" s="0"/>
+      <c r="BQ5" s="0"/>
+      <c r="BR5" s="0"/>
+      <c r="BS5" s="0"/>
+      <c r="BT5" s="0"/>
+      <c r="BU5" s="0"/>
+      <c r="BV5" s="0"/>
+      <c r="BW5" s="0"/>
+      <c r="BX5" s="0"/>
+      <c r="BY5" s="0"/>
+      <c r="BZ5" s="0"/>
+      <c r="CA5" s="0"/>
+      <c r="CB5" s="0"/>
+      <c r="CC5" s="0"/>
+      <c r="CD5" s="0"/>
+      <c r="CE5" s="0"/>
+      <c r="CF5" s="0"/>
+      <c r="CG5" s="0"/>
+      <c r="CH5" s="0"/>
+      <c r="CI5" s="0"/>
+      <c r="CJ5" s="0"/>
+      <c r="CK5" s="0"/>
+      <c r="CL5" s="0"/>
+      <c r="CM5" s="0"/>
+      <c r="CN5" s="0"/>
+      <c r="CO5" s="0"/>
+      <c r="CP5" s="0"/>
+      <c r="CQ5" s="0"/>
+      <c r="CR5" s="0"/>
+      <c r="CS5" s="0"/>
+      <c r="CT5" s="0"/>
+      <c r="CU5" s="0"/>
+      <c r="CV5" s="0"/>
+      <c r="CW5" s="0"/>
+      <c r="CX5" s="0"/>
+      <c r="CY5" s="0"/>
+      <c r="CZ5" s="0"/>
+      <c r="DA5" s="0"/>
+      <c r="DB5" s="0"/>
+      <c r="DC5" s="0"/>
+      <c r="DD5" s="0"/>
+      <c r="DE5" s="0"/>
+      <c r="DF5" s="0"/>
+      <c r="DG5" s="0"/>
+      <c r="DH5" s="0"/>
+      <c r="DI5" s="0"/>
+      <c r="DJ5" s="0"/>
+      <c r="DK5" s="0"/>
+      <c r="DL5" s="0"/>
+      <c r="DM5" s="0"/>
+      <c r="DN5" s="0"/>
+      <c r="DO5" s="0"/>
+      <c r="DP5" s="0"/>
+      <c r="DQ5" s="0"/>
+      <c r="DR5" s="0"/>
+      <c r="DS5" s="0"/>
+      <c r="DT5" s="0"/>
+      <c r="DU5" s="0"/>
+      <c r="DV5" s="0"/>
+      <c r="DW5" s="0"/>
+      <c r="DX5" s="0"/>
+      <c r="DY5" s="0"/>
+      <c r="DZ5" s="0"/>
+      <c r="EA5" s="0"/>
+      <c r="EB5" s="0"/>
+      <c r="EC5" s="0"/>
+      <c r="ED5" s="0"/>
+      <c r="EE5" s="0"/>
+      <c r="EF5" s="0"/>
+      <c r="EG5" s="0"/>
+      <c r="EH5" s="0"/>
+      <c r="EI5" s="0"/>
+      <c r="EJ5" s="0"/>
+      <c r="EK5" s="0"/>
+      <c r="EL5" s="0"/>
+      <c r="EM5" s="0"/>
+      <c r="EN5" s="0"/>
+      <c r="EO5" s="0"/>
+      <c r="EP5" s="0"/>
+      <c r="EQ5" s="0"/>
+      <c r="ER5" s="0"/>
+      <c r="ES5" s="0"/>
+      <c r="ET5" s="0"/>
+      <c r="EU5" s="0"/>
+      <c r="EV5" s="0"/>
+      <c r="EW5" s="0"/>
+      <c r="EX5" s="0"/>
+      <c r="EY5" s="0"/>
+      <c r="EZ5" s="0"/>
+      <c r="FA5" s="0"/>
+      <c r="FB5" s="0"/>
+      <c r="FC5" s="0"/>
+      <c r="FD5" s="0"/>
+      <c r="FE5" s="0"/>
+      <c r="FF5" s="0"/>
+      <c r="FG5" s="0"/>
+      <c r="FH5" s="0"/>
+      <c r="FI5" s="0"/>
+      <c r="FJ5" s="0"/>
+      <c r="FK5" s="0"/>
+      <c r="FL5" s="0"/>
+      <c r="FM5" s="0"/>
+      <c r="FN5" s="0"/>
+      <c r="FO5" s="0"/>
+      <c r="FP5" s="0"/>
+      <c r="FQ5" s="0"/>
+      <c r="FR5" s="0"/>
+      <c r="FS5" s="0"/>
+      <c r="FT5" s="0"/>
+      <c r="FU5" s="0"/>
+      <c r="FV5" s="0"/>
+      <c r="FW5" s="0"/>
+      <c r="FX5" s="0"/>
+      <c r="FY5" s="0"/>
+      <c r="FZ5" s="0"/>
+      <c r="GA5" s="0"/>
+      <c r="GB5" s="0"/>
+      <c r="GC5" s="0"/>
+      <c r="GD5" s="0"/>
+      <c r="GE5" s="0"/>
+      <c r="GF5" s="0"/>
+      <c r="GG5" s="0"/>
+      <c r="GH5" s="0"/>
+      <c r="GI5" s="0"/>
+      <c r="GJ5" s="0"/>
+      <c r="GK5" s="0"/>
+      <c r="GL5" s="0"/>
+      <c r="GM5" s="0"/>
+      <c r="GN5" s="0"/>
+      <c r="GO5" s="0"/>
+      <c r="GP5" s="0"/>
+      <c r="GQ5" s="0"/>
+      <c r="GR5" s="0"/>
+      <c r="GS5" s="0"/>
+      <c r="GT5" s="0"/>
+      <c r="GU5" s="0"/>
+      <c r="GV5" s="0"/>
+      <c r="GW5" s="0"/>
+      <c r="GX5" s="0"/>
+      <c r="GY5" s="0"/>
+      <c r="GZ5" s="0"/>
+      <c r="HA5" s="0"/>
+      <c r="HB5" s="0"/>
+      <c r="HC5" s="0"/>
+      <c r="HD5" s="0"/>
+      <c r="HE5" s="0"/>
+      <c r="HF5" s="0"/>
+      <c r="HG5" s="0"/>
+      <c r="HH5" s="0"/>
+      <c r="HI5" s="0"/>
+      <c r="HJ5" s="0"/>
+      <c r="HK5" s="0"/>
+      <c r="HL5" s="0"/>
+      <c r="HM5" s="0"/>
+      <c r="HN5" s="0"/>
+      <c r="HO5" s="0"/>
+      <c r="HP5" s="0"/>
+      <c r="HQ5" s="0"/>
+      <c r="HR5" s="0"/>
+      <c r="HS5" s="0"/>
+      <c r="HT5" s="0"/>
+      <c r="HU5" s="0"/>
+      <c r="HV5" s="0"/>
+      <c r="HW5" s="0"/>
+      <c r="HX5" s="0"/>
+      <c r="HY5" s="0"/>
+      <c r="HZ5" s="0"/>
+      <c r="IA5" s="0"/>
+      <c r="IB5" s="0"/>
+      <c r="IC5" s="0"/>
+      <c r="ID5" s="0"/>
+      <c r="IE5" s="0"/>
+      <c r="IF5" s="0"/>
+      <c r="IG5" s="0"/>
+      <c r="IH5" s="0"/>
+      <c r="II5" s="0"/>
+      <c r="IJ5" s="0"/>
+      <c r="IK5" s="0"/>
+      <c r="IL5" s="0"/>
+      <c r="IM5" s="0"/>
+      <c r="IN5" s="0"/>
+      <c r="IO5" s="0"/>
+      <c r="IP5" s="0"/>
+      <c r="IQ5" s="0"/>
+      <c r="IR5" s="0"/>
+      <c r="IS5" s="0"/>
+      <c r="IT5" s="0"/>
+      <c r="IU5" s="0"/>
+      <c r="IV5" s="0"/>
+      <c r="IW5" s="0"/>
+      <c r="IX5" s="0"/>
+      <c r="IY5" s="0"/>
+      <c r="IZ5" s="0"/>
+      <c r="JA5" s="0"/>
+      <c r="JB5" s="0"/>
+      <c r="JC5" s="0"/>
+      <c r="JD5" s="0"/>
+      <c r="JE5" s="0"/>
+      <c r="JF5" s="0"/>
+      <c r="JG5" s="0"/>
+      <c r="JH5" s="0"/>
+      <c r="JI5" s="0"/>
+      <c r="JJ5" s="0"/>
+      <c r="JK5" s="0"/>
+      <c r="JL5" s="0"/>
+      <c r="JM5" s="0"/>
+      <c r="JN5" s="0"/>
+      <c r="JO5" s="0"/>
+      <c r="JP5" s="0"/>
+      <c r="JQ5" s="0"/>
+      <c r="JR5" s="0"/>
+      <c r="JS5" s="0"/>
+      <c r="JT5" s="0"/>
+      <c r="JU5" s="0"/>
+      <c r="JV5" s="0"/>
+      <c r="JW5" s="0"/>
+      <c r="JX5" s="0"/>
+      <c r="JY5" s="0"/>
+      <c r="JZ5" s="0"/>
+      <c r="KA5" s="0"/>
+      <c r="KB5" s="0"/>
+      <c r="KC5" s="0"/>
+      <c r="KD5" s="0"/>
+      <c r="KE5" s="0"/>
+      <c r="KF5" s="0"/>
+      <c r="KG5" s="0"/>
+      <c r="KH5" s="0"/>
+      <c r="KI5" s="0"/>
+      <c r="KJ5" s="0"/>
+      <c r="KK5" s="0"/>
+      <c r="KL5" s="0"/>
+      <c r="KM5" s="0"/>
+      <c r="KN5" s="0"/>
+      <c r="KO5" s="0"/>
+      <c r="KP5" s="0"/>
+      <c r="KQ5" s="0"/>
+      <c r="KR5" s="0"/>
+      <c r="KS5" s="0"/>
+      <c r="KT5" s="0"/>
+      <c r="KU5" s="0"/>
+      <c r="KV5" s="0"/>
+      <c r="KW5" s="0"/>
+      <c r="KX5" s="0"/>
+      <c r="KY5" s="0"/>
+      <c r="KZ5" s="0"/>
+      <c r="LA5" s="0"/>
+      <c r="LB5" s="0"/>
+      <c r="LC5" s="0"/>
+      <c r="LD5" s="0"/>
+      <c r="LE5" s="0"/>
+      <c r="LF5" s="0"/>
+      <c r="LG5" s="0"/>
+      <c r="LH5" s="0"/>
+      <c r="LI5" s="0"/>
+      <c r="LJ5" s="0"/>
+      <c r="LK5" s="0"/>
+      <c r="LL5" s="0"/>
+      <c r="LM5" s="0"/>
+      <c r="LN5" s="0"/>
+      <c r="LO5" s="0"/>
+      <c r="LP5" s="0"/>
+      <c r="LQ5" s="0"/>
+      <c r="LR5" s="0"/>
+      <c r="LS5" s="0"/>
+      <c r="LT5" s="0"/>
+      <c r="LU5" s="0"/>
+      <c r="LV5" s="0"/>
+      <c r="LW5" s="0"/>
+      <c r="LX5" s="0"/>
+      <c r="LY5" s="0"/>
+      <c r="LZ5" s="0"/>
+      <c r="MA5" s="0"/>
+      <c r="MB5" s="0"/>
+      <c r="MC5" s="0"/>
+      <c r="MD5" s="0"/>
+      <c r="ME5" s="0"/>
+      <c r="MF5" s="0"/>
+      <c r="MG5" s="0"/>
+      <c r="MH5" s="0"/>
+      <c r="MI5" s="0"/>
+      <c r="MJ5" s="0"/>
+      <c r="MK5" s="0"/>
+      <c r="ML5" s="0"/>
+      <c r="MM5" s="0"/>
+      <c r="MN5" s="0"/>
+      <c r="MO5" s="0"/>
+      <c r="MP5" s="0"/>
+      <c r="MQ5" s="0"/>
+      <c r="MR5" s="0"/>
+      <c r="MS5" s="0"/>
+      <c r="MT5" s="0"/>
+      <c r="MU5" s="0"/>
+      <c r="MV5" s="0"/>
+      <c r="MW5" s="0"/>
+      <c r="MX5" s="0"/>
+      <c r="MY5" s="0"/>
+      <c r="MZ5" s="0"/>
+      <c r="NA5" s="0"/>
+      <c r="NB5" s="0"/>
+      <c r="NC5" s="0"/>
+      <c r="ND5" s="0"/>
+      <c r="NE5" s="0"/>
+      <c r="NF5" s="0"/>
+      <c r="NG5" s="0"/>
+      <c r="NH5" s="0"/>
+      <c r="NI5" s="0"/>
+      <c r="NJ5" s="0"/>
+      <c r="NK5" s="0"/>
+      <c r="NL5" s="0"/>
+      <c r="NM5" s="0"/>
+      <c r="NN5" s="0"/>
+      <c r="NO5" s="0"/>
+      <c r="NP5" s="0"/>
+      <c r="NQ5" s="0"/>
+      <c r="NR5" s="0"/>
+      <c r="NS5" s="0"/>
+      <c r="NT5" s="0"/>
+      <c r="NU5" s="0"/>
+      <c r="NV5" s="0"/>
+      <c r="NW5" s="0"/>
+      <c r="NX5" s="0"/>
+      <c r="NY5" s="0"/>
+      <c r="NZ5" s="0"/>
+      <c r="OA5" s="0"/>
+      <c r="OB5" s="0"/>
+      <c r="OC5" s="0"/>
+      <c r="OD5" s="0"/>
+      <c r="OE5" s="0"/>
+      <c r="OF5" s="0"/>
+      <c r="OG5" s="0"/>
+      <c r="OH5" s="0"/>
+      <c r="OI5" s="0"/>
+      <c r="OJ5" s="0"/>
+      <c r="OK5" s="0"/>
+      <c r="OL5" s="0"/>
+      <c r="OM5" s="0"/>
+      <c r="ON5" s="0"/>
+      <c r="OO5" s="0"/>
+      <c r="OP5" s="0"/>
+      <c r="OQ5" s="0"/>
+      <c r="OR5" s="0"/>
+      <c r="OS5" s="0"/>
+      <c r="OT5" s="0"/>
+      <c r="OU5" s="0"/>
+      <c r="OV5" s="0"/>
+      <c r="OW5" s="0"/>
+      <c r="OX5" s="0"/>
+      <c r="OY5" s="0"/>
+      <c r="OZ5" s="0"/>
+      <c r="PA5" s="0"/>
+      <c r="PB5" s="0"/>
+      <c r="PC5" s="0"/>
+      <c r="PD5" s="0"/>
+      <c r="PE5" s="0"/>
+      <c r="PF5" s="0"/>
+      <c r="PG5" s="0"/>
+      <c r="PH5" s="0"/>
+      <c r="PI5" s="0"/>
+      <c r="PJ5" s="0"/>
+      <c r="PK5" s="0"/>
+      <c r="PL5" s="0"/>
+      <c r="PM5" s="0"/>
+      <c r="PN5" s="0"/>
+      <c r="PO5" s="0"/>
+      <c r="PP5" s="0"/>
+      <c r="PQ5" s="0"/>
+      <c r="PR5" s="0"/>
+      <c r="PS5" s="0"/>
+      <c r="PT5" s="0"/>
+      <c r="PU5" s="0"/>
+      <c r="PV5" s="0"/>
+      <c r="PW5" s="0"/>
+      <c r="PX5" s="0"/>
+      <c r="PY5" s="0"/>
+      <c r="PZ5" s="0"/>
+      <c r="QA5" s="0"/>
+      <c r="QB5" s="0"/>
+      <c r="QC5" s="0"/>
+      <c r="QD5" s="0"/>
+      <c r="QE5" s="0"/>
+      <c r="QF5" s="0"/>
+      <c r="QG5" s="0"/>
+      <c r="QH5" s="0"/>
+      <c r="QI5" s="0"/>
+      <c r="QJ5" s="0"/>
+      <c r="QK5" s="0"/>
+      <c r="QL5" s="0"/>
+      <c r="QM5" s="0"/>
+      <c r="QN5" s="0"/>
+      <c r="QO5" s="0"/>
+      <c r="QP5" s="0"/>
+      <c r="QQ5" s="0"/>
+      <c r="QR5" s="0"/>
+      <c r="QS5" s="0"/>
+      <c r="QT5" s="0"/>
+      <c r="QU5" s="0"/>
+      <c r="QV5" s="0"/>
+      <c r="QW5" s="0"/>
+      <c r="QX5" s="0"/>
+      <c r="QY5" s="0"/>
+      <c r="QZ5" s="0"/>
+      <c r="RA5" s="0"/>
+      <c r="RB5" s="0"/>
+      <c r="RC5" s="0"/>
+      <c r="RD5" s="0"/>
+      <c r="RE5" s="0"/>
+      <c r="RF5" s="0"/>
+      <c r="RG5" s="0"/>
+      <c r="RH5" s="0"/>
+      <c r="RI5" s="0"/>
+      <c r="RJ5" s="0"/>
+      <c r="RK5" s="0"/>
+      <c r="RL5" s="0"/>
+      <c r="RM5" s="0"/>
+      <c r="RN5" s="0"/>
+      <c r="RO5" s="0"/>
+      <c r="RP5" s="0"/>
+      <c r="RQ5" s="0"/>
+      <c r="RR5" s="0"/>
+      <c r="RS5" s="0"/>
+      <c r="RT5" s="0"/>
+      <c r="RU5" s="0"/>
+      <c r="RV5" s="0"/>
+      <c r="RW5" s="0"/>
+      <c r="RX5" s="0"/>
+      <c r="RY5" s="0"/>
+      <c r="RZ5" s="0"/>
+      <c r="SA5" s="0"/>
+      <c r="SB5" s="0"/>
+      <c r="SC5" s="0"/>
+      <c r="SD5" s="0"/>
+      <c r="SE5" s="0"/>
+      <c r="SF5" s="0"/>
+      <c r="SG5" s="0"/>
+      <c r="SH5" s="0"/>
+      <c r="SI5" s="0"/>
+      <c r="SJ5" s="0"/>
+      <c r="SK5" s="0"/>
+      <c r="SL5" s="0"/>
+      <c r="SM5" s="0"/>
+      <c r="SN5" s="0"/>
+      <c r="SO5" s="0"/>
+      <c r="SP5" s="0"/>
+      <c r="SQ5" s="0"/>
+      <c r="SR5" s="0"/>
+      <c r="SS5" s="0"/>
+      <c r="ST5" s="0"/>
+      <c r="SU5" s="0"/>
+      <c r="SV5" s="0"/>
+      <c r="SW5" s="0"/>
+      <c r="SX5" s="0"/>
+      <c r="SY5" s="0"/>
+      <c r="SZ5" s="0"/>
+      <c r="TA5" s="0"/>
+      <c r="TB5" s="0"/>
+      <c r="TC5" s="0"/>
+      <c r="TD5" s="0"/>
+      <c r="TE5" s="0"/>
+      <c r="TF5" s="0"/>
+      <c r="TG5" s="0"/>
+      <c r="TH5" s="0"/>
+      <c r="TI5" s="0"/>
+      <c r="TJ5" s="0"/>
+      <c r="TK5" s="0"/>
+      <c r="TL5" s="0"/>
+      <c r="TM5" s="0"/>
+      <c r="TN5" s="0"/>
+      <c r="TO5" s="0"/>
+      <c r="TP5" s="0"/>
+      <c r="TQ5" s="0"/>
+      <c r="TR5" s="0"/>
+      <c r="TS5" s="0"/>
+      <c r="TT5" s="0"/>
+      <c r="TU5" s="0"/>
+      <c r="TV5" s="0"/>
+      <c r="TW5" s="0"/>
+      <c r="TX5" s="0"/>
+      <c r="TY5" s="0"/>
+      <c r="TZ5" s="0"/>
+      <c r="UA5" s="0"/>
+      <c r="UB5" s="0"/>
+      <c r="UC5" s="0"/>
+      <c r="UD5" s="0"/>
+      <c r="UE5" s="0"/>
+      <c r="UF5" s="0"/>
+      <c r="UG5" s="0"/>
+      <c r="UH5" s="0"/>
+      <c r="UI5" s="0"/>
+      <c r="UJ5" s="0"/>
+      <c r="UK5" s="0"/>
+      <c r="UL5" s="0"/>
+      <c r="UM5" s="0"/>
+      <c r="UN5" s="0"/>
+      <c r="UO5" s="0"/>
+      <c r="UP5" s="0"/>
+      <c r="UQ5" s="0"/>
+      <c r="UR5" s="0"/>
+      <c r="US5" s="0"/>
+      <c r="UT5" s="0"/>
+      <c r="UU5" s="0"/>
+      <c r="UV5" s="0"/>
+      <c r="UW5" s="0"/>
+      <c r="UX5" s="0"/>
+      <c r="UY5" s="0"/>
+      <c r="UZ5" s="0"/>
+      <c r="VA5" s="0"/>
+      <c r="VB5" s="0"/>
+      <c r="VC5" s="0"/>
+      <c r="VD5" s="0"/>
+      <c r="VE5" s="0"/>
+      <c r="VF5" s="0"/>
+      <c r="VG5" s="0"/>
+      <c r="VH5" s="0"/>
+      <c r="VI5" s="0"/>
+      <c r="VJ5" s="0"/>
+      <c r="VK5" s="0"/>
+      <c r="VL5" s="0"/>
+      <c r="VM5" s="0"/>
+      <c r="VN5" s="0"/>
+      <c r="VO5" s="0"/>
+      <c r="VP5" s="0"/>
+      <c r="VQ5" s="0"/>
+      <c r="VR5" s="0"/>
+      <c r="VS5" s="0"/>
+      <c r="VT5" s="0"/>
+      <c r="VU5" s="0"/>
+      <c r="VV5" s="0"/>
+      <c r="VW5" s="0"/>
+      <c r="VX5" s="0"/>
+      <c r="VY5" s="0"/>
+      <c r="VZ5" s="0"/>
+      <c r="WA5" s="0"/>
+      <c r="WB5" s="0"/>
+      <c r="WC5" s="0"/>
+      <c r="WD5" s="0"/>
+      <c r="WE5" s="0"/>
+      <c r="WF5" s="0"/>
+      <c r="WG5" s="0"/>
+      <c r="WH5" s="0"/>
+      <c r="WI5" s="0"/>
+      <c r="WJ5" s="0"/>
+      <c r="WK5" s="0"/>
+      <c r="WL5" s="0"/>
+      <c r="WM5" s="0"/>
+      <c r="WN5" s="0"/>
+      <c r="WO5" s="0"/>
+      <c r="WP5" s="0"/>
+      <c r="WQ5" s="0"/>
+      <c r="WR5" s="0"/>
+      <c r="WS5" s="0"/>
+      <c r="WT5" s="0"/>
+      <c r="WU5" s="0"/>
+      <c r="WV5" s="0"/>
+      <c r="WW5" s="0"/>
+      <c r="WX5" s="0"/>
+      <c r="WY5" s="0"/>
+      <c r="WZ5" s="0"/>
+      <c r="XA5" s="0"/>
+      <c r="XB5" s="0"/>
+      <c r="XC5" s="0"/>
+      <c r="XD5" s="0"/>
+      <c r="XE5" s="0"/>
+      <c r="XF5" s="0"/>
+      <c r="XG5" s="0"/>
+      <c r="XH5" s="0"/>
+      <c r="XI5" s="0"/>
+      <c r="XJ5" s="0"/>
+      <c r="XK5" s="0"/>
+      <c r="XL5" s="0"/>
+      <c r="XM5" s="0"/>
+      <c r="XN5" s="0"/>
+      <c r="XO5" s="0"/>
+      <c r="XP5" s="0"/>
+      <c r="XQ5" s="0"/>
+      <c r="XR5" s="0"/>
+      <c r="XS5" s="0"/>
+      <c r="XT5" s="0"/>
+      <c r="XU5" s="0"/>
+      <c r="XV5" s="0"/>
+      <c r="XW5" s="0"/>
+      <c r="XX5" s="0"/>
+      <c r="XY5" s="0"/>
+      <c r="XZ5" s="0"/>
+      <c r="YA5" s="0"/>
+      <c r="YB5" s="0"/>
+      <c r="YC5" s="0"/>
+      <c r="YD5" s="0"/>
+      <c r="YE5" s="0"/>
+      <c r="YF5" s="0"/>
+      <c r="YG5" s="0"/>
+      <c r="YH5" s="0"/>
+      <c r="YI5" s="0"/>
+      <c r="YJ5" s="0"/>
+      <c r="YK5" s="0"/>
+      <c r="YL5" s="0"/>
+      <c r="YM5" s="0"/>
+      <c r="YN5" s="0"/>
+      <c r="YO5" s="0"/>
+      <c r="YP5" s="0"/>
+      <c r="YQ5" s="0"/>
+      <c r="YR5" s="0"/>
+      <c r="YS5" s="0"/>
+      <c r="YT5" s="0"/>
+      <c r="YU5" s="0"/>
+      <c r="YV5" s="0"/>
+      <c r="YW5" s="0"/>
+      <c r="YX5" s="0"/>
+      <c r="YY5" s="0"/>
+      <c r="YZ5" s="0"/>
+      <c r="ZA5" s="0"/>
+      <c r="ZB5" s="0"/>
+      <c r="ZC5" s="0"/>
+      <c r="ZD5" s="0"/>
+      <c r="ZE5" s="0"/>
+      <c r="ZF5" s="0"/>
+      <c r="ZG5" s="0"/>
+      <c r="ZH5" s="0"/>
+      <c r="ZI5" s="0"/>
+      <c r="ZJ5" s="0"/>
+      <c r="ZK5" s="0"/>
+      <c r="ZL5" s="0"/>
+      <c r="ZM5" s="0"/>
+      <c r="ZN5" s="0"/>
+      <c r="ZO5" s="0"/>
+      <c r="ZP5" s="0"/>
+      <c r="ZQ5" s="0"/>
+      <c r="ZR5" s="0"/>
+      <c r="ZS5" s="0"/>
+      <c r="ZT5" s="0"/>
+      <c r="ZU5" s="0"/>
+      <c r="ZV5" s="0"/>
+      <c r="ZW5" s="0"/>
+      <c r="ZX5" s="0"/>
+      <c r="ZY5" s="0"/>
+      <c r="ZZ5" s="0"/>
+      <c r="AAA5" s="0"/>
+      <c r="AAB5" s="0"/>
+      <c r="AAC5" s="0"/>
+      <c r="AAD5" s="0"/>
+      <c r="AAE5" s="0"/>
+      <c r="AAF5" s="0"/>
+      <c r="AAG5" s="0"/>
+      <c r="AAH5" s="0"/>
+      <c r="AAI5" s="0"/>
+      <c r="AAJ5" s="0"/>
+      <c r="AAK5" s="0"/>
+      <c r="AAL5" s="0"/>
+      <c r="AAM5" s="0"/>
+      <c r="AAN5" s="0"/>
+      <c r="AAO5" s="0"/>
+      <c r="AAP5" s="0"/>
+      <c r="AAQ5" s="0"/>
+      <c r="AAR5" s="0"/>
+      <c r="AAS5" s="0"/>
+      <c r="AAT5" s="0"/>
+      <c r="AAU5" s="0"/>
+      <c r="AAV5" s="0"/>
+      <c r="AAW5" s="0"/>
+      <c r="AAX5" s="0"/>
+      <c r="AAY5" s="0"/>
+      <c r="AAZ5" s="0"/>
+      <c r="ABA5" s="0"/>
+      <c r="ABB5" s="0"/>
+      <c r="ABC5" s="0"/>
+      <c r="ABD5" s="0"/>
+      <c r="ABE5" s="0"/>
+      <c r="ABF5" s="0"/>
+      <c r="ABG5" s="0"/>
+      <c r="ABH5" s="0"/>
+      <c r="ABI5" s="0"/>
+      <c r="ABJ5" s="0"/>
+      <c r="ABK5" s="0"/>
+      <c r="ABL5" s="0"/>
+      <c r="ABM5" s="0"/>
+      <c r="ABN5" s="0"/>
+      <c r="ABO5" s="0"/>
+      <c r="ABP5" s="0"/>
+      <c r="ABQ5" s="0"/>
+      <c r="ABR5" s="0"/>
+      <c r="ABS5" s="0"/>
+      <c r="ABT5" s="0"/>
+      <c r="ABU5" s="0"/>
+      <c r="ABV5" s="0"/>
+      <c r="ABW5" s="0"/>
+      <c r="ABX5" s="0"/>
+      <c r="ABY5" s="0"/>
+      <c r="ABZ5" s="0"/>
+      <c r="ACA5" s="0"/>
+      <c r="ACB5" s="0"/>
+      <c r="ACC5" s="0"/>
+      <c r="ACD5" s="0"/>
+      <c r="ACE5" s="0"/>
+      <c r="ACF5" s="0"/>
+      <c r="ACG5" s="0"/>
+      <c r="ACH5" s="0"/>
+      <c r="ACI5" s="0"/>
+      <c r="ACJ5" s="0"/>
+      <c r="ACK5" s="0"/>
+      <c r="ACL5" s="0"/>
+      <c r="ACM5" s="0"/>
+      <c r="ACN5" s="0"/>
+      <c r="ACO5" s="0"/>
+      <c r="ACP5" s="0"/>
+      <c r="ACQ5" s="0"/>
+      <c r="ACR5" s="0"/>
+      <c r="ACS5" s="0"/>
+      <c r="ACT5" s="0"/>
+      <c r="ACU5" s="0"/>
+      <c r="ACV5" s="0"/>
+      <c r="ACW5" s="0"/>
+      <c r="ACX5" s="0"/>
+      <c r="ACY5" s="0"/>
+      <c r="ACZ5" s="0"/>
+      <c r="ADA5" s="0"/>
+      <c r="ADB5" s="0"/>
+      <c r="ADC5" s="0"/>
+      <c r="ADD5" s="0"/>
+      <c r="ADE5" s="0"/>
+      <c r="ADF5" s="0"/>
+      <c r="ADG5" s="0"/>
+      <c r="ADH5" s="0"/>
+      <c r="ADI5" s="0"/>
+      <c r="ADJ5" s="0"/>
+      <c r="ADK5" s="0"/>
+      <c r="ADL5" s="0"/>
+      <c r="ADM5" s="0"/>
+      <c r="ADN5" s="0"/>
+      <c r="ADO5" s="0"/>
+      <c r="ADP5" s="0"/>
+      <c r="ADQ5" s="0"/>
+      <c r="ADR5" s="0"/>
+      <c r="ADS5" s="0"/>
+      <c r="ADT5" s="0"/>
+      <c r="ADU5" s="0"/>
+      <c r="ADV5" s="0"/>
+      <c r="ADW5" s="0"/>
+      <c r="ADX5" s="0"/>
+      <c r="ADY5" s="0"/>
+      <c r="ADZ5" s="0"/>
+      <c r="AEA5" s="0"/>
+      <c r="AEB5" s="0"/>
+      <c r="AEC5" s="0"/>
+      <c r="AED5" s="0"/>
+      <c r="AEE5" s="0"/>
+      <c r="AEF5" s="0"/>
+      <c r="AEG5" s="0"/>
+      <c r="AEH5" s="0"/>
+      <c r="AEI5" s="0"/>
+      <c r="AEJ5" s="0"/>
+      <c r="AEK5" s="0"/>
+      <c r="AEL5" s="0"/>
+      <c r="AEM5" s="0"/>
+      <c r="AEN5" s="0"/>
+      <c r="AEO5" s="0"/>
+      <c r="AEP5" s="0"/>
+      <c r="AEQ5" s="0"/>
+      <c r="AER5" s="0"/>
+      <c r="AES5" s="0"/>
+      <c r="AET5" s="0"/>
+      <c r="AEU5" s="0"/>
+      <c r="AEV5" s="0"/>
+      <c r="AEW5" s="0"/>
+      <c r="AEX5" s="0"/>
+      <c r="AEY5" s="0"/>
+      <c r="AEZ5" s="0"/>
+      <c r="AFA5" s="0"/>
+      <c r="AFB5" s="0"/>
+      <c r="AFC5" s="0"/>
+      <c r="AFD5" s="0"/>
+      <c r="AFE5" s="0"/>
+      <c r="AFF5" s="0"/>
+      <c r="AFG5" s="0"/>
+      <c r="AFH5" s="0"/>
+      <c r="AFI5" s="0"/>
+      <c r="AFJ5" s="0"/>
+      <c r="AFK5" s="0"/>
+      <c r="AFL5" s="0"/>
+      <c r="AFM5" s="0"/>
+      <c r="AFN5" s="0"/>
+      <c r="AFO5" s="0"/>
+      <c r="AFP5" s="0"/>
+      <c r="AFQ5" s="0"/>
+      <c r="AFR5" s="0"/>
+      <c r="AFS5" s="0"/>
+      <c r="AFT5" s="0"/>
+      <c r="AFU5" s="0"/>
+      <c r="AFV5" s="0"/>
+      <c r="AFW5" s="0"/>
+      <c r="AFX5" s="0"/>
+      <c r="AFY5" s="0"/>
+      <c r="AFZ5" s="0"/>
+      <c r="AGA5" s="0"/>
+      <c r="AGB5" s="0"/>
+      <c r="AGC5" s="0"/>
+      <c r="AGD5" s="0"/>
+      <c r="AGE5" s="0"/>
+      <c r="AGF5" s="0"/>
+      <c r="AGG5" s="0"/>
+      <c r="AGH5" s="0"/>
+      <c r="AGI5" s="0"/>
+      <c r="AGJ5" s="0"/>
+      <c r="AGK5" s="0"/>
+      <c r="AGL5" s="0"/>
+      <c r="AGM5" s="0"/>
+      <c r="AGN5" s="0"/>
+      <c r="AGO5" s="0"/>
+      <c r="AGP5" s="0"/>
+      <c r="AGQ5" s="0"/>
+      <c r="AGR5" s="0"/>
+      <c r="AGS5" s="0"/>
+      <c r="AGT5" s="0"/>
+      <c r="AGU5" s="0"/>
+      <c r="AGV5" s="0"/>
+      <c r="AGW5" s="0"/>
+      <c r="AGX5" s="0"/>
+      <c r="AGY5" s="0"/>
+      <c r="AGZ5" s="0"/>
+      <c r="AHA5" s="0"/>
+      <c r="AHB5" s="0"/>
+      <c r="AHC5" s="0"/>
+      <c r="AHD5" s="0"/>
+      <c r="AHE5" s="0"/>
+      <c r="AHF5" s="0"/>
+      <c r="AHG5" s="0"/>
+      <c r="AHH5" s="0"/>
+      <c r="AHI5" s="0"/>
+      <c r="AHJ5" s="0"/>
+      <c r="AHK5" s="0"/>
+      <c r="AHL5" s="0"/>
+      <c r="AHM5" s="0"/>
+      <c r="AHN5" s="0"/>
+      <c r="AHO5" s="0"/>
+      <c r="AHP5" s="0"/>
+      <c r="AHQ5" s="0"/>
+      <c r="AHR5" s="0"/>
+      <c r="AHS5" s="0"/>
+      <c r="AHT5" s="0"/>
+      <c r="AHU5" s="0"/>
+      <c r="AHV5" s="0"/>
+      <c r="AHW5" s="0"/>
+      <c r="AHX5" s="0"/>
+      <c r="AHY5" s="0"/>
+      <c r="AHZ5" s="0"/>
+      <c r="AIA5" s="0"/>
+      <c r="AIB5" s="0"/>
+      <c r="AIC5" s="0"/>
+      <c r="AID5" s="0"/>
+      <c r="AIE5" s="0"/>
+      <c r="AIF5" s="0"/>
+      <c r="AIG5" s="0"/>
+      <c r="AIH5" s="0"/>
+      <c r="AII5" s="0"/>
+      <c r="AIJ5" s="0"/>
+      <c r="AIK5" s="0"/>
+      <c r="AIL5" s="0"/>
+      <c r="AIM5" s="0"/>
+      <c r="AIN5" s="0"/>
+      <c r="AIO5" s="0"/>
+      <c r="AIP5" s="0"/>
+      <c r="AIQ5" s="0"/>
+      <c r="AIR5" s="0"/>
+      <c r="AIS5" s="0"/>
+      <c r="AIT5" s="0"/>
+      <c r="AIU5" s="0"/>
+      <c r="AIV5" s="0"/>
+      <c r="AIW5" s="0"/>
+      <c r="AIX5" s="0"/>
+      <c r="AIY5" s="0"/>
+      <c r="AIZ5" s="0"/>
+      <c r="AJA5" s="0"/>
+      <c r="AJB5" s="0"/>
+      <c r="AJC5" s="0"/>
+      <c r="AJD5" s="0"/>
+      <c r="AJE5" s="0"/>
+      <c r="AJF5" s="0"/>
+      <c r="AJG5" s="0"/>
+      <c r="AJH5" s="0"/>
+      <c r="AJI5" s="0"/>
+      <c r="AJJ5" s="0"/>
+      <c r="AJK5" s="0"/>
+      <c r="AJL5" s="0"/>
+      <c r="AJM5" s="0"/>
+      <c r="AJN5" s="0"/>
+      <c r="AJO5" s="0"/>
+      <c r="AJP5" s="0"/>
+      <c r="AJQ5" s="0"/>
+      <c r="AJR5" s="0"/>
+      <c r="AJS5" s="0"/>
+      <c r="AJT5" s="0"/>
+      <c r="AJU5" s="0"/>
+      <c r="AJV5" s="0"/>
+      <c r="AJW5" s="0"/>
+      <c r="AJX5" s="0"/>
+      <c r="AJY5" s="0"/>
+      <c r="AJZ5" s="0"/>
+      <c r="AKA5" s="0"/>
+      <c r="AKB5" s="0"/>
+      <c r="AKC5" s="0"/>
+      <c r="AKD5" s="0"/>
+      <c r="AKE5" s="0"/>
+      <c r="AKF5" s="0"/>
+      <c r="AKG5" s="0"/>
+      <c r="AKH5" s="0"/>
+      <c r="AKI5" s="0"/>
+      <c r="AKJ5" s="0"/>
+      <c r="AKK5" s="0"/>
+      <c r="AKL5" s="0"/>
+      <c r="AKM5" s="0"/>
+      <c r="AKN5" s="0"/>
+      <c r="AKO5" s="0"/>
+      <c r="AKP5" s="0"/>
+      <c r="AKQ5" s="0"/>
+      <c r="AKR5" s="0"/>
+      <c r="AKS5" s="0"/>
+      <c r="AKT5" s="0"/>
+      <c r="AKU5" s="0"/>
+      <c r="AKV5" s="0"/>
+      <c r="AKW5" s="0"/>
+      <c r="AKX5" s="0"/>
+      <c r="AKY5" s="0"/>
+      <c r="AKZ5" s="0"/>
+      <c r="ALA5" s="0"/>
+      <c r="ALB5" s="0"/>
+      <c r="ALC5" s="0"/>
+      <c r="ALD5" s="0"/>
+      <c r="ALE5" s="0"/>
+      <c r="ALF5" s="0"/>
+      <c r="ALG5" s="0"/>
+      <c r="ALH5" s="0"/>
+      <c r="ALI5" s="0"/>
+      <c r="ALJ5" s="0"/>
+      <c r="ALK5" s="0"/>
+      <c r="ALL5" s="0"/>
+      <c r="ALM5" s="0"/>
+      <c r="ALN5" s="0"/>
+      <c r="ALO5" s="0"/>
+      <c r="ALP5" s="0"/>
+      <c r="ALQ5" s="0"/>
+      <c r="ALR5" s="0"/>
+      <c r="ALS5" s="0"/>
+      <c r="ALT5" s="0"/>
+      <c r="ALU5" s="0"/>
+      <c r="ALV5" s="0"/>
+      <c r="ALW5" s="0"/>
+      <c r="ALX5" s="0"/>
+      <c r="ALY5" s="0"/>
+      <c r="ALZ5" s="0"/>
+      <c r="AMA5" s="0"/>
+      <c r="AMB5" s="0"/>
+      <c r="AMC5" s="0"/>
+      <c r="AMD5" s="0"/>
+      <c r="AME5" s="0"/>
+      <c r="AMF5" s="0"/>
+      <c r="AMG5" s="0"/>
+      <c r="AMH5" s="0"/>
+      <c r="AMI5" s="0"/>
+      <c r="AMJ5" s="0"/>
     </row>
-    <row r="6" s="82" customFormat="true" ht="24.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" s="82" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="83" t="s">
-        <v>53</v>
-      </c>
-      <c r="C6" s="73" t="s">
-        <v>41</v>
-      </c>
-      <c r="D6" s="74" t="s">
-        <v>77</v>
-      </c>
-      <c r="E6" s="75" t="s">
-        <v>78</v>
-      </c>
-      <c r="F6" s="84" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" s="85" t="n">
-        <v>1</v>
-      </c>
-      <c r="H6" s="84" t="n">
-        <v>0</v>
-      </c>
-      <c r="I6" s="85" t="n">
-        <v>1</v>
-      </c>
+      <c r="B6" s="83"/>
+      <c r="C6" s="73"/>
+      <c r="D6" s="74"/>
+      <c r="E6" s="75"/>
+      <c r="F6" s="84"/>
+      <c r="G6" s="85"/>
+      <c r="H6" s="84"/>
+      <c r="I6" s="85"/>
       <c r="AMI6" s="1"/>
       <c r="AMJ6" s="1"/>
     </row>
-    <row r="7" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="83" t="s">
-        <v>63</v>
-      </c>
-      <c r="C7" s="73" t="s">
-        <v>41</v>
-      </c>
-      <c r="D7" s="74" t="s">
-        <v>79</v>
-      </c>
-      <c r="E7" s="75" t="n">
-        <v>329697</v>
-      </c>
-      <c r="F7" s="84" t="n">
-        <v>0</v>
-      </c>
-      <c r="G7" s="85" t="n">
-        <v>1</v>
-      </c>
-      <c r="H7" s="84" t="n">
-        <v>0</v>
-      </c>
-      <c r="I7" s="85" t="n">
-        <v>1</v>
-      </c>
+      <c r="B7" s="83"/>
+      <c r="C7" s="73"/>
+      <c r="D7" s="74"/>
+      <c r="E7" s="75"/>
+      <c r="F7" s="84"/>
+      <c r="G7" s="85"/>
+      <c r="H7" s="84"/>
+      <c r="I7" s="85"/>
     </row>
-    <row r="8" customFormat="false" ht="24.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="73" t="s">
-        <v>80</v>
-      </c>
-      <c r="C8" s="73" t="s">
-        <v>48</v>
-      </c>
-      <c r="D8" s="73" t="s">
-        <v>81</v>
-      </c>
-      <c r="E8" s="75" t="s">
-        <v>82</v>
-      </c>
-      <c r="F8" s="84" t="n">
-        <v>0</v>
-      </c>
-      <c r="G8" s="85" t="n">
-        <v>1</v>
-      </c>
-      <c r="H8" s="84" t="n">
-        <v>0</v>
-      </c>
-      <c r="I8" s="85" t="n">
-        <v>1</v>
-      </c>
+      <c r="B8" s="73"/>
+      <c r="C8" s="73"/>
+      <c r="D8" s="73"/>
+      <c r="E8" s="75"/>
+      <c r="F8" s="84"/>
+      <c r="G8" s="85"/>
+      <c r="H8" s="84"/>
+      <c r="I8" s="85"/>
     </row>
-    <row r="9" customFormat="false" ht="24.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="73" t="s">
-        <v>51</v>
-      </c>
-      <c r="C9" s="73" t="s">
-        <v>45</v>
-      </c>
-      <c r="D9" s="73" t="s">
-        <v>50</v>
-      </c>
-      <c r="E9" s="75" t="n">
-        <v>282998</v>
-      </c>
-      <c r="F9" s="84" t="n">
-        <v>0</v>
-      </c>
-      <c r="G9" s="85" t="n">
-        <v>1</v>
-      </c>
-      <c r="H9" s="84" t="n">
-        <v>0</v>
-      </c>
-      <c r="I9" s="85" t="n">
-        <v>1</v>
-      </c>
+      <c r="B9" s="73"/>
+      <c r="C9" s="73"/>
+      <c r="D9" s="73"/>
+      <c r="E9" s="75"/>
+      <c r="F9" s="84"/>
+      <c r="G9" s="85"/>
+      <c r="H9" s="84"/>
+      <c r="I9" s="85"/>
     </row>
-    <row r="10" customFormat="false" ht="24.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="83" t="s">
-        <v>56</v>
-      </c>
-      <c r="C10" s="86" t="s">
-        <v>83</v>
-      </c>
-      <c r="D10" s="86" t="s">
-        <v>84</v>
-      </c>
-      <c r="E10" s="75" t="s">
-        <v>85</v>
-      </c>
-      <c r="F10" s="84" t="n">
-        <v>0</v>
-      </c>
-      <c r="G10" s="85" t="n">
-        <v>1</v>
-      </c>
-      <c r="H10" s="84" t="n">
-        <v>0</v>
-      </c>
-      <c r="I10" s="85" t="n">
-        <v>1</v>
-      </c>
+      <c r="B10" s="83"/>
+      <c r="C10" s="86"/>
+      <c r="D10" s="86"/>
+      <c r="E10" s="75"/>
+      <c r="F10" s="84"/>
+      <c r="G10" s="85"/>
+      <c r="H10" s="84"/>
+      <c r="I10" s="85"/>
     </row>
-    <row r="11" customFormat="false" ht="24.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="87" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="83" t="s">
-        <v>65</v>
-      </c>
-      <c r="C11" s="88" t="s">
-        <v>86</v>
-      </c>
-      <c r="D11" s="74" t="s">
-        <v>87</v>
-      </c>
-      <c r="E11" s="89" t="n">
-        <v>528655</v>
-      </c>
-      <c r="F11" s="84" t="n">
-        <v>0</v>
-      </c>
-      <c r="G11" s="85" t="n">
-        <v>1</v>
-      </c>
-      <c r="H11" s="84" t="n">
-        <v>0</v>
-      </c>
-      <c r="I11" s="85" t="n">
-        <v>1</v>
-      </c>
+      <c r="B11" s="83"/>
+      <c r="C11" s="88"/>
+      <c r="D11" s="74"/>
+      <c r="E11" s="89"/>
+      <c r="F11" s="84"/>
+      <c r="G11" s="85"/>
+      <c r="H11" s="84"/>
+      <c r="I11" s="85"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -17004,7 +20806,6 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -17022,15 +20823,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="61" width="22.0647773279352"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="61" width="12.2105263157895"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="61" width="15.9595141700405"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="61" width="22.2793522267206"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="61" width="12.3198380566802"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="61" width="16.0688259109312"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="13.0688259109312"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="61" width="23.1376518218623"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="61" width="27.7449392712551"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="28.0647773279352"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="31.0647773279352"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="61" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="61" width="27.9595141700405"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="28.2793522267206"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="31.3846153846154"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -17081,16 +20882,16 @@
         <v>7</v>
       </c>
       <c r="B3" s="99" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="C3" s="100" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="D3" s="100" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="E3" s="100" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="F3" s="101" t="n">
         <v>0</v>
@@ -17110,16 +20911,16 @@
         <v>7</v>
       </c>
       <c r="B4" s="99" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="C4" s="100" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D4" s="100" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="E4" s="100" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="F4" s="104" t="n">
         <v>1</v>
@@ -17139,10 +20940,10 @@
         <v>20</v>
       </c>
       <c r="B5" s="99" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="C5" s="100" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="D5" s="100" t="s">
         <v>53</v>
@@ -17168,10 +20969,10 @@
         <v>20</v>
       </c>
       <c r="B6" s="99" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="C6" s="100" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="D6" s="100" t="s">
         <v>51</v>
@@ -17197,10 +20998,10 @@
         <v>20</v>
       </c>
       <c r="B7" s="99" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="C7" s="100" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="D7" s="108" t="s">
         <v>40</v>
@@ -17226,10 +21027,10 @@
         <v>20</v>
       </c>
       <c r="B8" s="99" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="C8" s="100" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="D8" s="109" t="s">
         <v>44</v>
@@ -17278,9 +21079,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="61" width="28.0647773279352"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="61" width="22.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="61" width="23.5668016194332"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="61" width="28.2793522267206"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="61" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="61" width="23.6720647773279"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="61" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="61" width="11.0323886639676"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="61" width="8.35627530364373"/>
@@ -20468,7 +24269,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="113" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
       <c r="C6" s="114" t="n">
         <v>653546</v>
@@ -20497,7 +24298,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="113" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="C7" s="114" t="n">
         <v>653545</v>
@@ -20613,7 +24414,7 @@
         <v>12</v>
       </c>
       <c r="B11" s="113" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="C11" s="114" t="n">
         <v>329697</v>
@@ -20651,7 +24452,7 @@
         <v>56</v>
       </c>
       <c r="E12" s="115" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="F12" s="84" t="n">
         <v>0</v>
@@ -20671,7 +24472,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="113" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="C13" s="114" t="n">
         <v>600458</v>
@@ -20680,7 +24481,7 @@
         <v>56</v>
       </c>
       <c r="E13" s="115" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="F13" s="84" t="n">
         <v>0</v>
@@ -20706,7 +24507,7 @@
         <v>510190</v>
       </c>
       <c r="D14" s="115" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="E14" s="115" t="s">
         <v>48</v>
@@ -20735,7 +24536,7 @@
         <v>613092</v>
       </c>
       <c r="D15" s="115" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="E15" s="115" t="s">
         <v>48</v>
@@ -20767,7 +24568,7 @@
         <v>65</v>
       </c>
       <c r="E16" s="115" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="F16" s="84" t="n">
         <v>0</v>
@@ -20812,7 +24613,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:G16"/>
+  <autoFilter ref="A2:F16"/>
   <mergeCells count="1">
     <mergeCell ref="F1:I1"/>
   </mergeCells>

</xml_diff>